<commit_message>
completando  de abajo hacia arriba
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documentos\Escritorio\PC 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C270FF31-8B18-41A7-B079-F800D41111ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="540" windowWidth="19905" windowHeight="9855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9015" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="C1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="270">
   <si>
     <t>Localización</t>
   </si>
@@ -683,13 +682,160 @@
   </si>
   <si>
     <t>KCNH8</t>
+  </si>
+  <si>
+    <t>Pentraxin 3</t>
+  </si>
+  <si>
+    <t>Protein Coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein Coding </t>
+  </si>
+  <si>
+    <t>65,10</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>nombre descrp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBC1 Domain Family Member 5 </t>
+  </si>
+  <si>
+    <t>26,37</t>
+  </si>
+  <si>
+    <t>SATB Homeobox 1</t>
+  </si>
+  <si>
+    <t>23,28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potassium Voltage-Gated Channel Subfamily H Member 8 </t>
+  </si>
+  <si>
+    <t>4,10</t>
+  </si>
+  <si>
+    <t>Phospholipase C Like 2</t>
+  </si>
+  <si>
+    <t>21,21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBX/Knotted 1 Homeobox 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adenosine Deaminase RNA Specific B1 </t>
+  </si>
+  <si>
+    <t>25,24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein O-Fucosyltransferase 2 </t>
+  </si>
+  <si>
+    <t>20,34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collagen Type XVIII Alpha 1 Chain </t>
+  </si>
+  <si>
+    <t>50,68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solute Carrier Family 19 Member 1 </t>
+  </si>
+  <si>
+    <t>20,15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poly(RC) Binding Protein 3 </t>
+  </si>
+  <si>
+    <t>24,11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collagen Type VI Alpha 1 Chain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collagen Type VI Alpha 2 Chain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formimidoyltransferase Cyclodeaminase </t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spermatogenesis And Centriole Associated 1 Like </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lanosterol Synthase </t>
+  </si>
+  <si>
+    <t>45,49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minichromosome Maintenance Complex Component 3 Associated Protein </t>
+  </si>
+  <si>
+    <t>41,44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromosome 21 Open Reading Frame 58 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">YbeY Metalloendoribonuclease </t>
+  </si>
+  <si>
+    <t>24,25</t>
+  </si>
+  <si>
+    <t>Pericentrin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disco Interacting Protein 2 Homolog A </t>
+  </si>
+  <si>
+    <t>25,31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S100 Calcium Binding Protein B </t>
+  </si>
+  <si>
+    <t>76,56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein Arginine Methyltransferase 2 </t>
+  </si>
+  <si>
+    <t>53,42</t>
+  </si>
+  <si>
+    <t>F-Box Protein 25</t>
+  </si>
+  <si>
+    <t>46,26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testis Development Related Protein </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deleted In Azoospermia Like </t>
+  </si>
+  <si>
+    <t>0.71,1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -740,8 +886,38 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -772,8 +948,14 @@
         <bgColor rgb="FFEAEAEA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -833,11 +1015,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -885,7 +1076,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -896,6 +1086,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,40 +1311,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V214"/>
+  <dimension ref="A1:V216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="G214" sqref="G214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="28" t="s">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -1161,13 +1362,13 @@
       <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1382,7 +1583,7 @@
       <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="11"/>
@@ -1412,7 +1613,7 @@
       <c r="V10" s="2"/>
     </row>
     <row r="11" spans="1:22" ht="15">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="26" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="11"/>
@@ -1442,7 +1643,7 @@
       <c r="V11" s="2"/>
     </row>
     <row r="12" spans="1:22" ht="15">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="11"/>
@@ -1472,7 +1673,7 @@
       <c r="V12" s="2"/>
     </row>
     <row r="13" spans="1:22" ht="15">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="26" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="11"/>
@@ -1502,7 +1703,7 @@
       <c r="V13" s="2"/>
     </row>
     <row r="14" spans="1:22" ht="15">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="11"/>
@@ -1532,7 +1733,7 @@
       <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" ht="15">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="11"/>
@@ -1562,7 +1763,7 @@
       <c r="V15" s="2"/>
     </row>
     <row r="16" spans="1:22" ht="15">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="11"/>
@@ -1592,7 +1793,7 @@
       <c r="V16" s="2"/>
     </row>
     <row r="17" spans="1:22" ht="15">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="11"/>
@@ -1622,7 +1823,7 @@
       <c r="V17" s="2"/>
     </row>
     <row r="18" spans="1:22" ht="15">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="4"/>
@@ -1652,7 +1853,7 @@
       <c r="V18" s="2"/>
     </row>
     <row r="19" spans="1:22" ht="15">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="11"/>
@@ -1682,7 +1883,7 @@
       <c r="V19" s="2"/>
     </row>
     <row r="20" spans="1:22" ht="15">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="11"/>
@@ -1712,7 +1913,7 @@
       <c r="V20" s="2"/>
     </row>
     <row r="21" spans="1:22" ht="15">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="11"/>
@@ -1742,7 +1943,7 @@
       <c r="V21" s="2"/>
     </row>
     <row r="22" spans="1:22" ht="15">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="11"/>
@@ -1772,7 +1973,7 @@
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="1:22" ht="15">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="26" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="16"/>
@@ -1802,7 +2003,7 @@
       <c r="V23" s="2"/>
     </row>
     <row r="24" spans="1:22" ht="15">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="26" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="16"/>
@@ -1832,7 +2033,7 @@
       <c r="V24" s="2"/>
     </row>
     <row r="25" spans="1:22" ht="15">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="16"/>
@@ -1862,7 +2063,7 @@
       <c r="V25" s="2"/>
     </row>
     <row r="26" spans="1:22" ht="15">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="16"/>
@@ -1892,7 +2093,7 @@
       <c r="V26" s="2"/>
     </row>
     <row r="27" spans="1:22" ht="15">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="26" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="16"/>
@@ -1922,7 +2123,7 @@
       <c r="V27" s="2"/>
     </row>
     <row r="28" spans="1:22" ht="15">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="26" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="16"/>
@@ -1952,7 +2153,7 @@
       <c r="V28" s="2"/>
     </row>
     <row r="29" spans="1:22" ht="15">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="16"/>
@@ -1982,7 +2183,7 @@
       <c r="V29" s="2"/>
     </row>
     <row r="30" spans="1:22" ht="15">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="16"/>
@@ -2012,7 +2213,7 @@
       <c r="V30" s="2"/>
     </row>
     <row r="31" spans="1:22" ht="15">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="16"/>
@@ -2042,7 +2243,7 @@
       <c r="V31" s="2"/>
     </row>
     <row r="32" spans="1:22" ht="15">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="16"/>
@@ -2072,7 +2273,7 @@
       <c r="V32" s="2"/>
     </row>
     <row r="33" spans="1:22" ht="15">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>40</v>
       </c>
       <c r="B33" s="16"/>
@@ -2102,7 +2303,7 @@
       <c r="V33" s="2"/>
     </row>
     <row r="34" spans="1:22" ht="15">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="26" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="16"/>
@@ -2132,7 +2333,7 @@
       <c r="V34" s="2"/>
     </row>
     <row r="35" spans="1:22" ht="15">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="11"/>
@@ -2162,7 +2363,7 @@
       <c r="V35" s="2"/>
     </row>
     <row r="36" spans="1:22" ht="15">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="16"/>
@@ -2192,7 +2393,7 @@
       <c r="V36" s="2"/>
     </row>
     <row r="37" spans="1:22" ht="15">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="16"/>
@@ -2222,7 +2423,7 @@
       <c r="V37" s="2"/>
     </row>
     <row r="38" spans="1:22" ht="15">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="26" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="11"/>
@@ -2252,7 +2453,7 @@
       <c r="V38" s="2"/>
     </row>
     <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11"/>
@@ -2282,7 +2483,7 @@
       <c r="V39" s="2"/>
     </row>
     <row r="40" spans="1:22" ht="15">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="26" t="s">
         <v>47</v>
       </c>
       <c r="B40" s="16"/>
@@ -2312,7 +2513,7 @@
       <c r="V40" s="2"/>
     </row>
     <row r="41" spans="1:22" ht="15">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="26" t="s">
         <v>48</v>
       </c>
       <c r="B41" s="16"/>
@@ -2342,7 +2543,7 @@
       <c r="V41" s="2"/>
     </row>
     <row r="42" spans="1:22" ht="15">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="26" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="16"/>
@@ -2372,7 +2573,7 @@
       <c r="V42" s="2"/>
     </row>
     <row r="43" spans="1:22" ht="15">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="26" t="s">
         <v>50</v>
       </c>
       <c r="B43" s="16"/>
@@ -2402,7 +2603,7 @@
       <c r="V43" s="2"/>
     </row>
     <row r="44" spans="1:22" ht="15">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="26" t="s">
         <v>51</v>
       </c>
       <c r="B44" s="11"/>
@@ -2432,7 +2633,7 @@
       <c r="V44" s="2"/>
     </row>
     <row r="45" spans="1:22" ht="15">
-      <c r="A45" s="27" t="s">
+      <c r="A45" s="26" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="16"/>
@@ -2462,7 +2663,7 @@
       <c r="V45" s="2"/>
     </row>
     <row r="46" spans="1:22" ht="15">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="26" t="s">
         <v>53</v>
       </c>
       <c r="B46" s="16"/>
@@ -2492,7 +2693,7 @@
       <c r="V46" s="2"/>
     </row>
     <row r="47" spans="1:22" ht="15">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="26" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="16"/>
@@ -2522,7 +2723,7 @@
       <c r="V47" s="2"/>
     </row>
     <row r="48" spans="1:22" ht="15">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B48" s="16"/>
@@ -2552,7 +2753,7 @@
       <c r="V48" s="2"/>
     </row>
     <row r="49" spans="1:22" ht="15">
-      <c r="A49" s="27" t="s">
+      <c r="A49" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B49" s="11"/>
@@ -2582,7 +2783,7 @@
       <c r="V49" s="2"/>
     </row>
     <row r="50" spans="1:22" ht="15">
-      <c r="A50" s="27" t="s">
+      <c r="A50" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="16"/>
@@ -2612,7 +2813,7 @@
       <c r="V50" s="2"/>
     </row>
     <row r="51" spans="1:22" ht="15">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B51" s="16"/>
@@ -2642,7 +2843,7 @@
       <c r="V51" s="2"/>
     </row>
     <row r="52" spans="1:22" ht="15">
-      <c r="A52" s="27" t="s">
+      <c r="A52" s="26" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="16"/>
@@ -2672,7 +2873,7 @@
       <c r="V52" s="2"/>
     </row>
     <row r="53" spans="1:22" ht="15">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="26" t="s">
         <v>60</v>
       </c>
       <c r="B53" s="11"/>
@@ -2702,7 +2903,7 @@
       <c r="V53" s="2"/>
     </row>
     <row r="54" spans="1:22" ht="15">
-      <c r="A54" s="27" t="s">
+      <c r="A54" s="26" t="s">
         <v>61</v>
       </c>
       <c r="B54" s="16"/>
@@ -2732,7 +2933,7 @@
       <c r="V54" s="2"/>
     </row>
     <row r="55" spans="1:22" ht="15">
-      <c r="A55" s="27" t="s">
+      <c r="A55" s="26" t="s">
         <v>62</v>
       </c>
       <c r="B55" s="16"/>
@@ -2762,7 +2963,7 @@
       <c r="V55" s="2"/>
     </row>
     <row r="56" spans="1:22" ht="15">
-      <c r="A56" s="27" t="s">
+      <c r="A56" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B56" s="16"/>
@@ -2792,7 +2993,7 @@
       <c r="V56" s="2"/>
     </row>
     <row r="57" spans="1:22" ht="15">
-      <c r="A57" s="27" t="s">
+      <c r="A57" s="26" t="s">
         <v>64</v>
       </c>
       <c r="B57" s="16"/>
@@ -2822,7 +3023,7 @@
       <c r="V57" s="2"/>
     </row>
     <row r="58" spans="1:22" ht="15">
-      <c r="A58" s="27" t="s">
+      <c r="A58" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B58" s="11"/>
@@ -2852,7 +3053,7 @@
       <c r="V58" s="2"/>
     </row>
     <row r="59" spans="1:22" ht="15">
-      <c r="A59" s="27" t="s">
+      <c r="A59" s="26" t="s">
         <v>66</v>
       </c>
       <c r="B59" s="16"/>
@@ -2882,7 +3083,7 @@
       <c r="V59" s="2"/>
     </row>
     <row r="60" spans="1:22" ht="15">
-      <c r="A60" s="27" t="s">
+      <c r="A60" s="26" t="s">
         <v>67</v>
       </c>
       <c r="B60" s="16"/>
@@ -2912,7 +3113,7 @@
       <c r="V60" s="2"/>
     </row>
     <row r="61" spans="1:22" ht="15">
-      <c r="A61" s="27" t="s">
+      <c r="A61" s="26" t="s">
         <v>68</v>
       </c>
       <c r="B61" s="11"/>
@@ -2942,7 +3143,7 @@
       <c r="V61" s="2"/>
     </row>
     <row r="62" spans="1:22" ht="15">
-      <c r="A62" s="27" t="s">
+      <c r="A62" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B62" s="16"/>
@@ -2972,7 +3173,7 @@
       <c r="V62" s="2"/>
     </row>
     <row r="63" spans="1:22" ht="15">
-      <c r="A63" s="27" t="s">
+      <c r="A63" s="26" t="s">
         <v>70</v>
       </c>
       <c r="B63" s="11"/>
@@ -3002,7 +3203,7 @@
       <c r="V63" s="2"/>
     </row>
     <row r="64" spans="1:22" ht="15">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="26" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="16"/>
@@ -3032,7 +3233,7 @@
       <c r="V64" s="2"/>
     </row>
     <row r="65" spans="1:22" ht="15">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="26" t="s">
         <v>72</v>
       </c>
       <c r="B65" s="16"/>
@@ -3062,7 +3263,7 @@
       <c r="V65" s="2"/>
     </row>
     <row r="66" spans="1:22" ht="15">
-      <c r="A66" s="27" t="s">
+      <c r="A66" s="26" t="s">
         <v>73</v>
       </c>
       <c r="B66" s="16"/>
@@ -3092,7 +3293,7 @@
       <c r="V66" s="2"/>
     </row>
     <row r="67" spans="1:22" ht="15">
-      <c r="A67" s="27" t="s">
+      <c r="A67" s="26" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="16"/>
@@ -3122,7 +3323,7 @@
       <c r="V67" s="2"/>
     </row>
     <row r="68" spans="1:22" ht="15">
-      <c r="A68" s="27" t="s">
+      <c r="A68" s="26" t="s">
         <v>75</v>
       </c>
       <c r="B68" s="16"/>
@@ -3152,7 +3353,7 @@
       <c r="V68" s="2"/>
     </row>
     <row r="69" spans="1:22" ht="15">
-      <c r="A69" s="27" t="s">
+      <c r="A69" s="26" t="s">
         <v>76</v>
       </c>
       <c r="B69" s="16"/>
@@ -3182,7 +3383,7 @@
       <c r="V69" s="2"/>
     </row>
     <row r="70" spans="1:22" ht="15">
-      <c r="A70" s="27" t="s">
+      <c r="A70" s="26" t="s">
         <v>77</v>
       </c>
       <c r="B70" s="16"/>
@@ -3212,7 +3413,7 @@
       <c r="V70" s="2"/>
     </row>
     <row r="71" spans="1:22" ht="15">
-      <c r="A71" s="27" t="s">
+      <c r="A71" s="26" t="s">
         <v>78</v>
       </c>
       <c r="B71" s="16"/>
@@ -3242,7 +3443,7 @@
       <c r="V71" s="2"/>
     </row>
     <row r="72" spans="1:22" ht="15">
-      <c r="A72" s="27" t="s">
+      <c r="A72" s="26" t="s">
         <v>79</v>
       </c>
       <c r="B72" s="4"/>
@@ -3272,7 +3473,7 @@
       <c r="V72" s="2"/>
     </row>
     <row r="73" spans="1:22" ht="15">
-      <c r="A73" s="27" t="s">
+      <c r="A73" s="26" t="s">
         <v>80</v>
       </c>
       <c r="B73" s="16"/>
@@ -3302,7 +3503,7 @@
       <c r="V73" s="2"/>
     </row>
     <row r="74" spans="1:22" ht="15">
-      <c r="A74" s="27" t="s">
+      <c r="A74" s="26" t="s">
         <v>81</v>
       </c>
       <c r="B74" s="16"/>
@@ -3332,7 +3533,7 @@
       <c r="V74" s="2"/>
     </row>
     <row r="75" spans="1:22" ht="15">
-      <c r="A75" s="27" t="s">
+      <c r="A75" s="26" t="s">
         <v>82</v>
       </c>
       <c r="B75" s="16"/>
@@ -3362,7 +3563,7 @@
       <c r="V75" s="2"/>
     </row>
     <row r="76" spans="1:22" ht="15">
-      <c r="A76" s="27" t="s">
+      <c r="A76" s="26" t="s">
         <v>83</v>
       </c>
       <c r="B76" s="16"/>
@@ -3392,7 +3593,7 @@
       <c r="V76" s="2"/>
     </row>
     <row r="77" spans="1:22" ht="15">
-      <c r="A77" s="27" t="s">
+      <c r="A77" s="26" t="s">
         <v>84</v>
       </c>
       <c r="B77" s="16"/>
@@ -3422,7 +3623,7 @@
       <c r="V77" s="2"/>
     </row>
     <row r="78" spans="1:22" ht="15">
-      <c r="A78" s="27" t="s">
+      <c r="A78" s="26" t="s">
         <v>85</v>
       </c>
       <c r="B78" s="4"/>
@@ -3452,7 +3653,7 @@
       <c r="V78" s="2"/>
     </row>
     <row r="79" spans="1:22" ht="15">
-      <c r="A79" s="27" t="s">
+      <c r="A79" s="26" t="s">
         <v>86</v>
       </c>
       <c r="B79" s="4"/>
@@ -3482,7 +3683,7 @@
       <c r="V79" s="2"/>
     </row>
     <row r="80" spans="1:22" ht="15">
-      <c r="A80" s="27" t="s">
+      <c r="A80" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B80" s="4"/>
@@ -3512,7 +3713,7 @@
       <c r="V80" s="2"/>
     </row>
     <row r="81" spans="1:22" ht="15">
-      <c r="A81" s="27" t="s">
+      <c r="A81" s="26" t="s">
         <v>88</v>
       </c>
       <c r="B81" s="16"/>
@@ -3542,7 +3743,7 @@
       <c r="V81" s="2"/>
     </row>
     <row r="82" spans="1:22" ht="15">
-      <c r="A82" s="27" t="s">
+      <c r="A82" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B82" s="16"/>
@@ -3572,7 +3773,7 @@
       <c r="V82" s="2"/>
     </row>
     <row r="83" spans="1:22" ht="15">
-      <c r="A83" s="27" t="s">
+      <c r="A83" s="26" t="s">
         <v>90</v>
       </c>
       <c r="B83" s="16"/>
@@ -3602,7 +3803,7 @@
       <c r="V83" s="2"/>
     </row>
     <row r="84" spans="1:22" ht="15">
-      <c r="A84" s="27" t="s">
+      <c r="A84" s="26" t="s">
         <v>91</v>
       </c>
       <c r="B84" s="16"/>
@@ -3632,7 +3833,7 @@
       <c r="V84" s="2"/>
     </row>
     <row r="85" spans="1:22" ht="15">
-      <c r="A85" s="27" t="s">
+      <c r="A85" s="26" t="s">
         <v>92</v>
       </c>
       <c r="B85" s="4"/>
@@ -3662,7 +3863,7 @@
       <c r="V85" s="2"/>
     </row>
     <row r="86" spans="1:22" ht="15">
-      <c r="A86" s="27" t="s">
+      <c r="A86" s="26" t="s">
         <v>93</v>
       </c>
       <c r="B86" s="16"/>
@@ -3692,7 +3893,7 @@
       <c r="V86" s="2"/>
     </row>
     <row r="87" spans="1:22" ht="15">
-      <c r="A87" s="27" t="s">
+      <c r="A87" s="26" t="s">
         <v>94</v>
       </c>
       <c r="B87" s="16"/>
@@ -3722,7 +3923,7 @@
       <c r="V87" s="2"/>
     </row>
     <row r="88" spans="1:22" ht="15">
-      <c r="A88" s="27" t="s">
+      <c r="A88" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B88" s="16"/>
@@ -3752,7 +3953,7 @@
       <c r="V88" s="2"/>
     </row>
     <row r="89" spans="1:22" ht="15">
-      <c r="A89" s="27" t="s">
+      <c r="A89" s="26" t="s">
         <v>96</v>
       </c>
       <c r="B89" s="16"/>
@@ -3782,7 +3983,7 @@
       <c r="V89" s="2"/>
     </row>
     <row r="90" spans="1:22" ht="15">
-      <c r="A90" s="27" t="s">
+      <c r="A90" s="26" t="s">
         <v>97</v>
       </c>
       <c r="B90" s="16"/>
@@ -3812,7 +4013,7 @@
       <c r="V90" s="2"/>
     </row>
     <row r="91" spans="1:22" ht="15">
-      <c r="A91" s="27" t="s">
+      <c r="A91" s="26" t="s">
         <v>98</v>
       </c>
       <c r="B91" s="16"/>
@@ -3842,7 +4043,7 @@
       <c r="V91" s="2"/>
     </row>
     <row r="92" spans="1:22" ht="15">
-      <c r="A92" s="27" t="s">
+      <c r="A92" s="26" t="s">
         <v>99</v>
       </c>
       <c r="B92" s="16"/>
@@ -3872,7 +4073,7 @@
       <c r="V92" s="2"/>
     </row>
     <row r="93" spans="1:22" ht="15">
-      <c r="A93" s="27" t="s">
+      <c r="A93" s="26" t="s">
         <v>100</v>
       </c>
       <c r="B93" s="16"/>
@@ -3902,7 +4103,7 @@
       <c r="V93" s="2"/>
     </row>
     <row r="94" spans="1:22" ht="15">
-      <c r="A94" s="27" t="s">
+      <c r="A94" s="26" t="s">
         <v>101</v>
       </c>
       <c r="B94" s="16"/>
@@ -3932,7 +4133,7 @@
       <c r="V94" s="2"/>
     </row>
     <row r="95" spans="1:22" ht="15">
-      <c r="A95" s="27" t="s">
+      <c r="A95" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B95" s="16"/>
@@ -3962,7 +4163,7 @@
       <c r="V95" s="2"/>
     </row>
     <row r="96" spans="1:22" ht="15">
-      <c r="A96" s="27" t="s">
+      <c r="A96" s="26" t="s">
         <v>103</v>
       </c>
       <c r="B96" s="16"/>
@@ -3992,7 +4193,7 @@
       <c r="V96" s="2"/>
     </row>
     <row r="97" spans="1:22" ht="15">
-      <c r="A97" s="27" t="s">
+      <c r="A97" s="26" t="s">
         <v>104</v>
       </c>
       <c r="B97" s="4"/>
@@ -4022,7 +4223,7 @@
       <c r="V97" s="2"/>
     </row>
     <row r="98" spans="1:22" ht="15">
-      <c r="A98" s="27" t="s">
+      <c r="A98" s="26" t="s">
         <v>105</v>
       </c>
       <c r="B98" s="4"/>
@@ -4052,7 +4253,7 @@
       <c r="V98" s="2"/>
     </row>
     <row r="99" spans="1:22" ht="15">
-      <c r="A99" s="27" t="s">
+      <c r="A99" s="26" t="s">
         <v>106</v>
       </c>
       <c r="B99" s="4"/>
@@ -4082,7 +4283,7 @@
       <c r="V99" s="2"/>
     </row>
     <row r="100" spans="1:22" ht="15">
-      <c r="A100" s="27" t="s">
+      <c r="A100" s="26" t="s">
         <v>107</v>
       </c>
       <c r="B100" s="4"/>
@@ -4112,7 +4313,7 @@
       <c r="V100" s="2"/>
     </row>
     <row r="101" spans="1:22" ht="15">
-      <c r="A101" s="27" t="s">
+      <c r="A101" s="26" t="s">
         <v>108</v>
       </c>
       <c r="B101" s="4"/>
@@ -4142,7 +4343,7 @@
       <c r="V101" s="2"/>
     </row>
     <row r="102" spans="1:22" ht="15">
-      <c r="A102" s="27" t="s">
+      <c r="A102" s="26" t="s">
         <v>109</v>
       </c>
       <c r="B102" s="16"/>
@@ -4172,7 +4373,7 @@
       <c r="V102" s="2"/>
     </row>
     <row r="103" spans="1:22" ht="15">
-      <c r="A103" s="27" t="s">
+      <c r="A103" s="26" t="s">
         <v>110</v>
       </c>
       <c r="B103" s="4"/>
@@ -4202,7 +4403,7 @@
       <c r="V103" s="2"/>
     </row>
     <row r="104" spans="1:22" ht="15">
-      <c r="A104" s="27" t="s">
+      <c r="A104" s="26" t="s">
         <v>111</v>
       </c>
       <c r="B104" s="16"/>
@@ -4232,7 +4433,7 @@
       <c r="V104" s="2"/>
     </row>
     <row r="105" spans="1:22" ht="15">
-      <c r="A105" s="27" t="s">
+      <c r="A105" s="26" t="s">
         <v>112</v>
       </c>
       <c r="B105" s="16"/>
@@ -4262,7 +4463,7 @@
       <c r="V105" s="2"/>
     </row>
     <row r="106" spans="1:22" ht="15">
-      <c r="A106" s="27" t="s">
+      <c r="A106" s="26" t="s">
         <v>113</v>
       </c>
       <c r="B106" s="16"/>
@@ -4292,7 +4493,7 @@
       <c r="V106" s="2"/>
     </row>
     <row r="107" spans="1:22" ht="15">
-      <c r="A107" s="27" t="s">
+      <c r="A107" s="26" t="s">
         <v>114</v>
       </c>
       <c r="B107" s="4"/>
@@ -4322,7 +4523,7 @@
       <c r="V107" s="2"/>
     </row>
     <row r="108" spans="1:22" ht="15">
-      <c r="A108" s="27" t="s">
+      <c r="A108" s="26" t="s">
         <v>115</v>
       </c>
       <c r="B108" s="16"/>
@@ -4352,7 +4553,7 @@
       <c r="V108" s="2"/>
     </row>
     <row r="109" spans="1:22" ht="15">
-      <c r="A109" s="27" t="s">
+      <c r="A109" s="26" t="s">
         <v>116</v>
       </c>
       <c r="B109" s="4"/>
@@ -4382,7 +4583,7 @@
       <c r="V109" s="2"/>
     </row>
     <row r="110" spans="1:22" ht="15">
-      <c r="A110" s="27" t="s">
+      <c r="A110" s="26" t="s">
         <v>117</v>
       </c>
       <c r="B110" s="16"/>
@@ -4412,7 +4613,7 @@
       <c r="V110" s="2"/>
     </row>
     <row r="111" spans="1:22" ht="15">
-      <c r="A111" s="27" t="s">
+      <c r="A111" s="26" t="s">
         <v>118</v>
       </c>
       <c r="B111" s="4"/>
@@ -4442,7 +4643,7 @@
       <c r="V111" s="2"/>
     </row>
     <row r="112" spans="1:22" ht="15">
-      <c r="A112" s="27" t="s">
+      <c r="A112" s="26" t="s">
         <v>119</v>
       </c>
       <c r="B112" s="16"/>
@@ -4472,7 +4673,7 @@
       <c r="V112" s="2"/>
     </row>
     <row r="113" spans="1:22" ht="15">
-      <c r="A113" s="27" t="s">
+      <c r="A113" s="26" t="s">
         <v>120</v>
       </c>
       <c r="B113" s="4"/>
@@ -4502,7 +4703,7 @@
       <c r="V113" s="2"/>
     </row>
     <row r="114" spans="1:22" ht="15">
-      <c r="A114" s="27" t="s">
+      <c r="A114" s="26" t="s">
         <v>121</v>
       </c>
       <c r="B114" s="4"/>
@@ -4532,7 +4733,7 @@
       <c r="V114" s="2"/>
     </row>
     <row r="115" spans="1:22" ht="15">
-      <c r="A115" s="27" t="s">
+      <c r="A115" s="26" t="s">
         <v>122</v>
       </c>
       <c r="B115" s="16"/>
@@ -4562,7 +4763,7 @@
       <c r="V115" s="2"/>
     </row>
     <row r="116" spans="1:22" ht="15">
-      <c r="A116" s="27" t="s">
+      <c r="A116" s="26" t="s">
         <v>123</v>
       </c>
       <c r="B116" s="4"/>
@@ -4592,7 +4793,7 @@
       <c r="V116" s="2"/>
     </row>
     <row r="117" spans="1:22" ht="15">
-      <c r="A117" s="27" t="s">
+      <c r="A117" s="26" t="s">
         <v>124</v>
       </c>
       <c r="B117" s="16"/>
@@ -4622,7 +4823,7 @@
       <c r="V117" s="2"/>
     </row>
     <row r="118" spans="1:22" ht="15">
-      <c r="A118" s="27" t="s">
+      <c r="A118" s="26" t="s">
         <v>125</v>
       </c>
       <c r="B118" s="16"/>
@@ -4652,7 +4853,7 @@
       <c r="V118" s="2"/>
     </row>
     <row r="119" spans="1:22" ht="15">
-      <c r="A119" s="27" t="s">
+      <c r="A119" s="26" t="s">
         <v>126</v>
       </c>
       <c r="B119" s="16"/>
@@ -4682,7 +4883,7 @@
       <c r="V119" s="2"/>
     </row>
     <row r="120" spans="1:22" ht="15">
-      <c r="A120" s="27" t="s">
+      <c r="A120" s="26" t="s">
         <v>127</v>
       </c>
       <c r="B120" s="16"/>
@@ -4712,7 +4913,7 @@
       <c r="V120" s="2"/>
     </row>
     <row r="121" spans="1:22" ht="15">
-      <c r="A121" s="27" t="s">
+      <c r="A121" s="26" t="s">
         <v>10</v>
       </c>
       <c r="B121" s="4"/>
@@ -4742,7 +4943,7 @@
       <c r="V121" s="2"/>
     </row>
     <row r="122" spans="1:22" ht="15">
-      <c r="A122" s="27" t="s">
+      <c r="A122" s="26" t="s">
         <v>128</v>
       </c>
       <c r="B122" s="20"/>
@@ -4772,7 +4973,7 @@
       <c r="V122" s="2"/>
     </row>
     <row r="123" spans="1:22" ht="15">
-      <c r="A123" s="27" t="s">
+      <c r="A123" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B123" s="16"/>
@@ -4802,7 +5003,7 @@
       <c r="V123" s="2"/>
     </row>
     <row r="124" spans="1:22" ht="15">
-      <c r="A124" s="27" t="s">
+      <c r="A124" s="26" t="s">
         <v>130</v>
       </c>
       <c r="B124" s="16"/>
@@ -4832,7 +5033,7 @@
       <c r="V124" s="2"/>
     </row>
     <row r="125" spans="1:22" ht="15">
-      <c r="A125" s="27" t="s">
+      <c r="A125" s="26" t="s">
         <v>131</v>
       </c>
       <c r="B125" s="11"/>
@@ -4862,7 +5063,7 @@
       <c r="V125" s="2"/>
     </row>
     <row r="126" spans="1:22" ht="15">
-      <c r="A126" s="27" t="s">
+      <c r="A126" s="26" t="s">
         <v>132</v>
       </c>
       <c r="B126" s="16"/>
@@ -4892,7 +5093,7 @@
       <c r="V126" s="2"/>
     </row>
     <row r="127" spans="1:22" ht="15">
-      <c r="A127" s="27" t="s">
+      <c r="A127" s="26" t="s">
         <v>133</v>
       </c>
       <c r="B127" s="16"/>
@@ -4922,7 +5123,7 @@
       <c r="V127" s="2"/>
     </row>
     <row r="128" spans="1:22" ht="15">
-      <c r="A128" s="27" t="s">
+      <c r="A128" s="26" t="s">
         <v>134</v>
       </c>
       <c r="B128" s="16"/>
@@ -4952,7 +5153,7 @@
       <c r="V128" s="2"/>
     </row>
     <row r="129" spans="1:22" ht="15">
-      <c r="A129" s="27" t="s">
+      <c r="A129" s="26" t="s">
         <v>135</v>
       </c>
       <c r="B129" s="16"/>
@@ -4982,7 +5183,7 @@
       <c r="V129" s="2"/>
     </row>
     <row r="130" spans="1:22" ht="15">
-      <c r="A130" s="27" t="s">
+      <c r="A130" s="26" t="s">
         <v>136</v>
       </c>
       <c r="B130" s="16"/>
@@ -5012,7 +5213,7 @@
       <c r="V130" s="2"/>
     </row>
     <row r="131" spans="1:22" ht="15">
-      <c r="A131" s="27" t="s">
+      <c r="A131" s="26" t="s">
         <v>137</v>
       </c>
       <c r="B131" s="16"/>
@@ -5042,7 +5243,7 @@
       <c r="V131" s="2"/>
     </row>
     <row r="132" spans="1:22" ht="15">
-      <c r="A132" s="27" t="s">
+      <c r="A132" s="26" t="s">
         <v>138</v>
       </c>
       <c r="B132" s="16"/>
@@ -5072,7 +5273,7 @@
       <c r="V132" s="2"/>
     </row>
     <row r="133" spans="1:22" ht="15">
-      <c r="A133" s="27" t="s">
+      <c r="A133" s="26" t="s">
         <v>139</v>
       </c>
       <c r="B133" s="1"/>
@@ -5102,7 +5303,7 @@
       <c r="V133" s="2"/>
     </row>
     <row r="134" spans="1:22" ht="15">
-      <c r="A134" s="27" t="s">
+      <c r="A134" s="26" t="s">
         <v>140</v>
       </c>
       <c r="B134" s="16"/>
@@ -5132,7 +5333,7 @@
       <c r="V134" s="2"/>
     </row>
     <row r="135" spans="1:22" ht="15">
-      <c r="A135" s="27" t="s">
+      <c r="A135" s="26" t="s">
         <v>141</v>
       </c>
       <c r="B135" s="1"/>
@@ -5162,7 +5363,7 @@
       <c r="V135" s="2"/>
     </row>
     <row r="136" spans="1:22" ht="15">
-      <c r="A136" s="27" t="s">
+      <c r="A136" s="26" t="s">
         <v>142</v>
       </c>
       <c r="B136" s="11"/>
@@ -5192,7 +5393,7 @@
       <c r="V136" s="2"/>
     </row>
     <row r="137" spans="1:22" ht="15">
-      <c r="A137" s="27" t="s">
+      <c r="A137" s="26" t="s">
         <v>143</v>
       </c>
       <c r="B137" s="16"/>
@@ -5222,7 +5423,7 @@
       <c r="V137" s="2"/>
     </row>
     <row r="138" spans="1:22" ht="15">
-      <c r="A138" s="27" t="s">
+      <c r="A138" s="26" t="s">
         <v>144</v>
       </c>
       <c r="B138" s="16"/>
@@ -5252,7 +5453,7 @@
       <c r="V138" s="2"/>
     </row>
     <row r="139" spans="1:22" ht="15">
-      <c r="A139" s="27" t="s">
+      <c r="A139" s="26" t="s">
         <v>145</v>
       </c>
       <c r="B139" s="16"/>
@@ -5282,7 +5483,7 @@
       <c r="V139" s="2"/>
     </row>
     <row r="140" spans="1:22" ht="15">
-      <c r="A140" s="27" t="s">
+      <c r="A140" s="26" t="s">
         <v>146</v>
       </c>
       <c r="B140" s="16"/>
@@ -5312,7 +5513,7 @@
       <c r="V140" s="2"/>
     </row>
     <row r="141" spans="1:22" ht="15">
-      <c r="A141" s="27" t="s">
+      <c r="A141" s="26" t="s">
         <v>147</v>
       </c>
       <c r="B141" s="21"/>
@@ -5342,7 +5543,7 @@
       <c r="V141" s="2"/>
     </row>
     <row r="142" spans="1:22" ht="15">
-      <c r="A142" s="27" t="s">
+      <c r="A142" s="26" t="s">
         <v>148</v>
       </c>
       <c r="B142" s="16"/>
@@ -5372,7 +5573,7 @@
       <c r="V142" s="2"/>
     </row>
     <row r="143" spans="1:22" ht="15">
-      <c r="A143" s="27" t="s">
+      <c r="A143" s="26" t="s">
         <v>149</v>
       </c>
       <c r="B143" s="16"/>
@@ -5402,7 +5603,7 @@
       <c r="V143" s="2"/>
     </row>
     <row r="144" spans="1:22" ht="15">
-      <c r="A144" s="27" t="s">
+      <c r="A144" s="26" t="s">
         <v>150</v>
       </c>
       <c r="B144" s="16"/>
@@ -5432,7 +5633,7 @@
       <c r="V144" s="2"/>
     </row>
     <row r="145" spans="1:22" ht="15">
-      <c r="A145" s="27" t="s">
+      <c r="A145" s="26" t="s">
         <v>151</v>
       </c>
       <c r="B145" s="21"/>
@@ -5462,7 +5663,7 @@
       <c r="V145" s="2"/>
     </row>
     <row r="146" spans="1:22" ht="15">
-      <c r="A146" s="27" t="s">
+      <c r="A146" s="26" t="s">
         <v>152</v>
       </c>
       <c r="B146" s="11"/>
@@ -5492,7 +5693,7 @@
       <c r="V146" s="2"/>
     </row>
     <row r="147" spans="1:22" ht="15">
-      <c r="A147" s="27" t="s">
+      <c r="A147" s="26" t="s">
         <v>153</v>
       </c>
       <c r="B147" s="11"/>
@@ -5522,7 +5723,7 @@
       <c r="V147" s="2"/>
     </row>
     <row r="148" spans="1:22" ht="15">
-      <c r="A148" s="27" t="s">
+      <c r="A148" s="26" t="s">
         <v>154</v>
       </c>
       <c r="B148" s="16"/>
@@ -5552,7 +5753,7 @@
       <c r="V148" s="2"/>
     </row>
     <row r="149" spans="1:22" ht="15">
-      <c r="A149" s="27" t="s">
+      <c r="A149" s="26" t="s">
         <v>155</v>
       </c>
       <c r="B149" s="16"/>
@@ -5581,8 +5782,8 @@
       <c r="U149" s="2"/>
       <c r="V149" s="2"/>
     </row>
-    <row r="150" spans="1:22" ht="15">
-      <c r="A150" s="27" t="s">
+    <row r="150" spans="1:22" thickBot="1">
+      <c r="A150" s="26" t="s">
         <v>156</v>
       </c>
       <c r="B150" s="4"/>
@@ -5612,20 +5813,28 @@
       <c r="V150" s="2"/>
     </row>
     <row r="151" spans="1:22" ht="15">
-      <c r="A151" s="27" t="s">
+      <c r="A151" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B151" s="4"/>
-      <c r="C151" s="3"/>
+      <c r="B151" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C151" s="31" t="s">
+        <v>221</v>
+      </c>
       <c r="D151" s="5">
         <v>109705012</v>
       </c>
       <c r="E151" s="5">
         <v>109711074</v>
       </c>
-      <c r="F151" s="4"/>
+      <c r="F151" s="32" t="s">
+        <v>224</v>
+      </c>
       <c r="G151" s="4"/>
-      <c r="H151" s="4"/>
+      <c r="H151" s="4">
+        <v>6</v>
+      </c>
       <c r="I151" s="2"/>
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
@@ -5642,7 +5851,7 @@
       <c r="V151" s="2"/>
     </row>
     <row r="152" spans="1:22" ht="15">
-      <c r="A152" s="27" t="s">
+      <c r="A152" s="26" t="s">
         <v>158</v>
       </c>
       <c r="B152" s="4"/>
@@ -5672,7 +5881,7 @@
       <c r="V152" s="2"/>
     </row>
     <row r="153" spans="1:22" ht="15">
-      <c r="A153" s="27" t="s">
+      <c r="A153" s="26" t="s">
         <v>159</v>
       </c>
       <c r="B153" s="4"/>
@@ -5702,7 +5911,7 @@
       <c r="V153" s="2"/>
     </row>
     <row r="154" spans="1:22" ht="15">
-      <c r="A154" s="27" t="s">
+      <c r="A154" s="26" t="s">
         <v>160</v>
       </c>
       <c r="B154" s="4"/>
@@ -5732,7 +5941,7 @@
       <c r="V154" s="2"/>
     </row>
     <row r="155" spans="1:22" ht="15">
-      <c r="A155" s="27" t="s">
+      <c r="A155" s="26" t="s">
         <v>161</v>
       </c>
       <c r="B155" s="4"/>
@@ -5762,7 +5971,7 @@
       <c r="V155" s="2"/>
     </row>
     <row r="156" spans="1:22" ht="15">
-      <c r="A156" s="27" t="s">
+      <c r="A156" s="26" t="s">
         <v>162</v>
       </c>
       <c r="B156" s="4"/>
@@ -5792,7 +6001,7 @@
       <c r="V156" s="2"/>
     </row>
     <row r="157" spans="1:22" ht="15">
-      <c r="A157" s="27" t="s">
+      <c r="A157" s="26" t="s">
         <v>163</v>
       </c>
       <c r="B157" s="4"/>
@@ -5822,7 +6031,7 @@
       <c r="V157" s="2"/>
     </row>
     <row r="158" spans="1:22" ht="15">
-      <c r="A158" s="27" t="s">
+      <c r="A158" s="26" t="s">
         <v>164</v>
       </c>
       <c r="B158" s="4"/>
@@ -5852,7 +6061,7 @@
       <c r="V158" s="2"/>
     </row>
     <row r="159" spans="1:22" ht="15">
-      <c r="A159" s="27" t="s">
+      <c r="A159" s="26" t="s">
         <v>165</v>
       </c>
       <c r="B159" s="6"/>
@@ -5882,7 +6091,7 @@
       <c r="V159" s="2"/>
     </row>
     <row r="160" spans="1:22" ht="15">
-      <c r="A160" s="27" t="s">
+      <c r="A160" s="26" t="s">
         <v>166</v>
       </c>
       <c r="B160" s="6"/>
@@ -5912,7 +6121,7 @@
       <c r="V160" s="2"/>
     </row>
     <row r="161" spans="1:22" ht="15">
-      <c r="A161" s="27" t="s">
+      <c r="A161" s="26" t="s">
         <v>167</v>
       </c>
       <c r="B161" s="6"/>
@@ -5942,7 +6151,7 @@
       <c r="V161" s="2"/>
     </row>
     <row r="162" spans="1:22" ht="15">
-      <c r="A162" s="27" t="s">
+      <c r="A162" s="26" t="s">
         <v>168</v>
       </c>
       <c r="B162" s="6"/>
@@ -5972,7 +6181,7 @@
       <c r="V162" s="2"/>
     </row>
     <row r="163" spans="1:22" ht="15">
-      <c r="A163" s="27" t="s">
+      <c r="A163" s="26" t="s">
         <v>169</v>
       </c>
       <c r="B163" s="6"/>
@@ -6002,7 +6211,7 @@
       <c r="V163" s="2"/>
     </row>
     <row r="164" spans="1:22" ht="15">
-      <c r="A164" s="27" t="s">
+      <c r="A164" s="26" t="s">
         <v>170</v>
       </c>
       <c r="B164" s="6"/>
@@ -6032,7 +6241,7 @@
       <c r="V164" s="2"/>
     </row>
     <row r="165" spans="1:22" ht="15">
-      <c r="A165" s="27" t="s">
+      <c r="A165" s="26" t="s">
         <v>171</v>
       </c>
       <c r="B165" s="6"/>
@@ -6062,7 +6271,7 @@
       <c r="V165" s="2"/>
     </row>
     <row r="166" spans="1:22" ht="15">
-      <c r="A166" s="27" t="s">
+      <c r="A166" s="26" t="s">
         <v>172</v>
       </c>
       <c r="B166" s="6"/>
@@ -6092,7 +6301,7 @@
       <c r="V166" s="2"/>
     </row>
     <row r="167" spans="1:22" ht="15">
-      <c r="A167" s="27" t="s">
+      <c r="A167" s="26" t="s">
         <v>173</v>
       </c>
       <c r="B167" s="6"/>
@@ -6122,7 +6331,7 @@
       <c r="V167" s="2"/>
     </row>
     <row r="168" spans="1:22" ht="15">
-      <c r="A168" s="27" t="s">
+      <c r="A168" s="26" t="s">
         <v>174</v>
       </c>
       <c r="B168" s="6"/>
@@ -6152,7 +6361,7 @@
       <c r="V168" s="2"/>
     </row>
     <row r="169" spans="1:22" ht="15">
-      <c r="A169" s="27" t="s">
+      <c r="A169" s="26" t="s">
         <v>175</v>
       </c>
       <c r="B169" s="6"/>
@@ -6182,7 +6391,7 @@
       <c r="V169" s="2"/>
     </row>
     <row r="170" spans="1:22" ht="15">
-      <c r="A170" s="27" t="s">
+      <c r="A170" s="26" t="s">
         <v>176</v>
       </c>
       <c r="B170" s="6"/>
@@ -6212,7 +6421,7 @@
       <c r="V170" s="2"/>
     </row>
     <row r="171" spans="1:22" ht="15">
-      <c r="A171" s="27" t="s">
+      <c r="A171" s="26" t="s">
         <v>177</v>
       </c>
       <c r="B171" s="6"/>
@@ -6242,7 +6451,7 @@
       <c r="V171" s="2"/>
     </row>
     <row r="172" spans="1:22" ht="15">
-      <c r="A172" s="27" t="s">
+      <c r="A172" s="26" t="s">
         <v>178</v>
       </c>
       <c r="B172" s="6"/>
@@ -6272,7 +6481,7 @@
       <c r="V172" s="2"/>
     </row>
     <row r="173" spans="1:22" ht="15">
-      <c r="A173" s="27" t="s">
+      <c r="A173" s="26" t="s">
         <v>179</v>
       </c>
       <c r="B173" s="6"/>
@@ -6302,7 +6511,7 @@
       <c r="V173" s="2"/>
     </row>
     <row r="174" spans="1:22" ht="15">
-      <c r="A174" s="27" t="s">
+      <c r="A174" s="26" t="s">
         <v>180</v>
       </c>
       <c r="B174" s="6"/>
@@ -6332,7 +6541,7 @@
       <c r="V174" s="2"/>
     </row>
     <row r="175" spans="1:22" ht="15">
-      <c r="A175" s="27" t="s">
+      <c r="A175" s="26" t="s">
         <v>181</v>
       </c>
       <c r="B175" s="4"/>
@@ -6362,7 +6571,7 @@
       <c r="V175" s="2"/>
     </row>
     <row r="176" spans="1:22" ht="15">
-      <c r="A176" s="27" t="s">
+      <c r="A176" s="26" t="s">
         <v>182</v>
       </c>
       <c r="B176" s="4"/>
@@ -6392,7 +6601,7 @@
       <c r="V176" s="2"/>
     </row>
     <row r="177" spans="1:22" ht="15">
-      <c r="A177" s="27" t="s">
+      <c r="A177" s="26" t="s">
         <v>183</v>
       </c>
       <c r="B177" s="4"/>
@@ -6422,7 +6631,7 @@
       <c r="V177" s="2"/>
     </row>
     <row r="178" spans="1:22" ht="15">
-      <c r="A178" s="27" t="s">
+      <c r="A178" s="26" t="s">
         <v>184</v>
       </c>
       <c r="B178" s="4"/>
@@ -6452,7 +6661,7 @@
       <c r="V178" s="2"/>
     </row>
     <row r="179" spans="1:22" ht="15">
-      <c r="A179" s="27" t="s">
+      <c r="A179" s="26" t="s">
         <v>185</v>
       </c>
       <c r="B179" s="4"/>
@@ -6482,7 +6691,7 @@
       <c r="V179" s="2"/>
     </row>
     <row r="180" spans="1:22" ht="15">
-      <c r="A180" s="27" t="s">
+      <c r="A180" s="26" t="s">
         <v>186</v>
       </c>
       <c r="B180" s="4"/>
@@ -6512,7 +6721,7 @@
       <c r="V180" s="2"/>
     </row>
     <row r="181" spans="1:22" ht="15">
-      <c r="A181" s="27" t="s">
+      <c r="A181" s="26" t="s">
         <v>187</v>
       </c>
       <c r="B181" s="4"/>
@@ -6542,7 +6751,7 @@
       <c r="V181" s="2"/>
     </row>
     <row r="182" spans="1:22" ht="15">
-      <c r="A182" s="27" t="s">
+      <c r="A182" s="26" t="s">
         <v>188</v>
       </c>
       <c r="B182" s="4"/>
@@ -6572,7 +6781,7 @@
       <c r="V182" s="2"/>
     </row>
     <row r="183" spans="1:22" ht="15">
-      <c r="A183" s="27" t="s">
+      <c r="A183" s="26" t="s">
         <v>189</v>
       </c>
       <c r="B183" s="4"/>
@@ -6601,8 +6810,8 @@
       <c r="U183" s="2"/>
       <c r="V183" s="2"/>
     </row>
-    <row r="184" spans="1:22" ht="15">
-      <c r="A184" s="27" t="s">
+    <row r="184" spans="1:22" thickBot="1">
+      <c r="A184" s="26" t="s">
         <v>190</v>
       </c>
       <c r="B184" s="4"/>
@@ -6631,19 +6840,25 @@
       <c r="U184" s="2"/>
       <c r="V184" s="2"/>
     </row>
-    <row r="185" spans="1:22" ht="15">
-      <c r="A185" s="27" t="s">
+    <row r="185" spans="1:22" thickBot="1">
+      <c r="A185" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="B185" s="4"/>
-      <c r="C185" s="12"/>
+      <c r="B185" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C185" s="36" t="s">
+        <v>235</v>
+      </c>
       <c r="D185" s="5">
         <v>142744432</v>
       </c>
       <c r="E185" s="5">
         <v>142789033</v>
       </c>
-      <c r="F185" s="4"/>
+      <c r="F185" s="4">
+        <v>19</v>
+      </c>
       <c r="G185" s="4"/>
       <c r="H185" s="4"/>
       <c r="I185" s="2"/>
@@ -6661,21 +6876,29 @@
       <c r="U185" s="2"/>
       <c r="V185" s="2"/>
     </row>
-    <row r="186" spans="1:22" ht="15">
-      <c r="A186" s="27" t="s">
+    <row r="186" spans="1:22" thickBot="1">
+      <c r="A186" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B186" s="4"/>
-      <c r="C186" s="12"/>
+      <c r="B186" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C186" s="36" t="s">
+        <v>236</v>
+      </c>
       <c r="D186" s="5">
         <v>144900016</v>
       </c>
       <c r="E186" s="5">
         <v>144991569</v>
       </c>
-      <c r="F186" s="4"/>
+      <c r="F186" s="32" t="s">
+        <v>237</v>
+      </c>
       <c r="G186" s="4"/>
-      <c r="H186" s="4"/>
+      <c r="H186" s="4">
+        <v>9</v>
+      </c>
       <c r="I186" s="2"/>
       <c r="J186" s="2"/>
       <c r="K186" s="2"/>
@@ -6691,21 +6914,29 @@
       <c r="U186" s="2"/>
       <c r="V186" s="2"/>
     </row>
-    <row r="187" spans="1:22" ht="15">
-      <c r="A187" s="27" t="s">
+    <row r="187" spans="1:22" thickBot="1">
+      <c r="A187" s="33" t="s">
         <v>193</v>
       </c>
-      <c r="B187" s="4"/>
-      <c r="C187" s="12"/>
+      <c r="B187" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C187" s="36" t="s">
+        <v>238</v>
+      </c>
       <c r="D187" s="5">
         <v>145035446</v>
       </c>
       <c r="E187" s="5">
         <v>145048712</v>
       </c>
-      <c r="F187" s="4"/>
+      <c r="F187" s="32" t="s">
+        <v>239</v>
+      </c>
       <c r="G187" s="4"/>
-      <c r="H187" s="4"/>
+      <c r="H187" s="4">
+        <v>9</v>
+      </c>
       <c r="I187" s="2"/>
       <c r="J187" s="2"/>
       <c r="K187" s="2"/>
@@ -6721,21 +6952,29 @@
       <c r="U187" s="2"/>
       <c r="V187" s="2"/>
     </row>
-    <row r="188" spans="1:22" ht="15">
-      <c r="A188" s="27" t="s">
+    <row r="188" spans="1:22" thickBot="1">
+      <c r="A188" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="B188" s="4"/>
-      <c r="C188" s="12"/>
+      <c r="B188" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C188" s="36" t="s">
+        <v>240</v>
+      </c>
       <c r="D188" s="5">
         <v>145152446</v>
       </c>
       <c r="E188" s="5">
         <v>145246309</v>
       </c>
-      <c r="F188" s="4"/>
+      <c r="F188" s="32" t="s">
+        <v>241</v>
+      </c>
       <c r="G188" s="4"/>
-      <c r="H188" s="4"/>
+      <c r="H188" s="4">
+        <v>47</v>
+      </c>
       <c r="I188" s="2"/>
       <c r="J188" s="2"/>
       <c r="K188" s="2"/>
@@ -6751,21 +6990,29 @@
       <c r="U188" s="2"/>
       <c r="V188" s="2"/>
     </row>
-    <row r="189" spans="1:22" ht="15">
-      <c r="A189" s="27" t="s">
+    <row r="189" spans="1:22" thickBot="1">
+      <c r="A189" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="B189" s="4"/>
-      <c r="C189" s="12"/>
+      <c r="B189" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C189" s="36" t="s">
+        <v>242</v>
+      </c>
       <c r="D189" s="5">
         <v>145249313</v>
       </c>
       <c r="E189" s="5">
         <v>145275187</v>
       </c>
-      <c r="F189" s="4"/>
+      <c r="F189" s="32" t="s">
+        <v>243</v>
+      </c>
       <c r="G189" s="4"/>
-      <c r="H189" s="4"/>
+      <c r="H189" s="4">
+        <v>1</v>
+      </c>
       <c r="I189" s="2"/>
       <c r="J189" s="2"/>
       <c r="K189" s="2"/>
@@ -6782,20 +7029,28 @@
       <c r="V189" s="2"/>
     </row>
     <row r="190" spans="1:22" ht="15">
-      <c r="A190" s="27" t="s">
+      <c r="A190" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="B190" s="4"/>
-      <c r="C190" s="12"/>
+      <c r="B190" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C190" s="36" t="s">
+        <v>244</v>
+      </c>
       <c r="D190" s="5">
         <v>145344482</v>
       </c>
       <c r="E190" s="5">
         <v>145581973</v>
       </c>
-      <c r="F190" s="4"/>
+      <c r="F190" s="32" t="s">
+        <v>245</v>
+      </c>
       <c r="G190" s="4"/>
-      <c r="H190" s="4"/>
+      <c r="H190" s="4">
+        <v>0</v>
+      </c>
       <c r="I190" s="2"/>
       <c r="J190" s="2"/>
       <c r="K190" s="2"/>
@@ -6812,7 +7067,7 @@
       <c r="V190" s="2"/>
     </row>
     <row r="191" spans="1:22" ht="15">
-      <c r="A191" s="27" t="s">
+      <c r="A191" s="33" t="s">
         <v>197</v>
       </c>
       <c r="B191" s="4"/>
@@ -6842,20 +7097,28 @@
       <c r="V191" s="2"/>
     </row>
     <row r="192" spans="1:22" ht="15">
-      <c r="A192" s="27" t="s">
+      <c r="A192" s="33" t="s">
         <v>198</v>
       </c>
-      <c r="B192" s="4"/>
-      <c r="C192" s="12"/>
+      <c r="B192" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C192" s="36" t="s">
+        <v>246</v>
+      </c>
       <c r="D192" s="5">
         <v>145631195</v>
       </c>
       <c r="E192" s="5">
         <v>145652325</v>
       </c>
-      <c r="F192" s="4"/>
+      <c r="F192" s="37">
+        <v>113159</v>
+      </c>
       <c r="G192" s="4"/>
-      <c r="H192" s="4"/>
+      <c r="H192" s="4">
+        <v>147</v>
+      </c>
       <c r="I192" s="2"/>
       <c r="J192" s="2"/>
       <c r="K192" s="2"/>
@@ -6872,20 +7135,28 @@
       <c r="V192" s="2"/>
     </row>
     <row r="193" spans="1:22" ht="15">
-      <c r="A193" s="27" t="s">
+      <c r="A193" s="33" t="s">
         <v>199</v>
       </c>
-      <c r="B193" s="4"/>
-      <c r="C193" s="12"/>
+      <c r="B193" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C193" s="36" t="s">
+        <v>247</v>
+      </c>
       <c r="D193" s="5">
         <v>145768042</v>
       </c>
       <c r="E193" s="5">
         <v>145799845</v>
       </c>
-      <c r="F193" s="4"/>
+      <c r="F193" s="37">
+        <v>126165</v>
+      </c>
       <c r="G193" s="4"/>
-      <c r="H193" s="4"/>
+      <c r="H193" s="4">
+        <v>77</v>
+      </c>
       <c r="I193" s="2"/>
       <c r="J193" s="2"/>
       <c r="K193" s="2"/>
@@ -6902,18 +7173,24 @@
       <c r="V193" s="2"/>
     </row>
     <row r="194" spans="1:22" ht="15">
-      <c r="A194" s="27" t="s">
+      <c r="A194" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="B194" s="4"/>
-      <c r="C194" s="12"/>
+      <c r="B194" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C194" s="36" t="s">
+        <v>248</v>
+      </c>
       <c r="D194" s="5">
         <v>145809671</v>
       </c>
       <c r="E194" s="5">
         <v>145824726</v>
       </c>
-      <c r="F194" s="4"/>
+      <c r="F194" s="32" t="s">
+        <v>249</v>
+      </c>
       <c r="G194" s="4"/>
       <c r="H194" s="4"/>
       <c r="I194" s="2"/>
@@ -6932,20 +7209,28 @@
       <c r="V194" s="2"/>
     </row>
     <row r="195" spans="1:22" ht="15">
-      <c r="A195" s="27" t="s">
+      <c r="A195" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="B195" s="4"/>
-      <c r="C195" s="12"/>
+      <c r="B195" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C195" s="36" t="s">
+        <v>250</v>
+      </c>
       <c r="D195" s="5">
         <v>145826815</v>
       </c>
       <c r="E195" s="5">
         <v>145847568</v>
       </c>
-      <c r="F195" s="4"/>
+      <c r="F195" s="4">
+        <v>20</v>
+      </c>
       <c r="G195" s="4"/>
-      <c r="H195" s="4"/>
+      <c r="H195" s="4">
+        <v>9</v>
+      </c>
       <c r="I195" s="2"/>
       <c r="J195" s="2"/>
       <c r="K195" s="2"/>
@@ -6962,20 +7247,28 @@
       <c r="V195" s="2"/>
     </row>
     <row r="196" spans="1:22" ht="15">
-      <c r="A196" s="27" t="s">
+      <c r="A196" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="B196" s="4"/>
-      <c r="C196" s="12"/>
+      <c r="B196" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C196" s="36" t="s">
+        <v>251</v>
+      </c>
       <c r="D196" s="5">
         <v>145851416</v>
       </c>
       <c r="E196" s="5">
         <v>145883591</v>
       </c>
-      <c r="F196" s="4"/>
+      <c r="F196" s="32" t="s">
+        <v>252</v>
+      </c>
       <c r="G196" s="4"/>
-      <c r="H196" s="4"/>
+      <c r="H196" s="4">
+        <v>3</v>
+      </c>
       <c r="I196" s="2"/>
       <c r="J196" s="2"/>
       <c r="K196" s="2"/>
@@ -6992,20 +7285,28 @@
       <c r="V196" s="2"/>
     </row>
     <row r="197" spans="1:22" ht="15">
-      <c r="A197" s="27" t="s">
+      <c r="A197" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="B197" s="4"/>
-      <c r="C197" s="12"/>
+      <c r="B197" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C197" s="36" t="s">
+        <v>253</v>
+      </c>
       <c r="D197" s="5">
         <v>145893289</v>
       </c>
       <c r="E197" s="5">
         <v>145937594</v>
       </c>
-      <c r="F197" s="4"/>
+      <c r="F197" s="32" t="s">
+        <v>254</v>
+      </c>
       <c r="G197" s="4"/>
-      <c r="H197" s="4"/>
+      <c r="H197" s="4">
+        <v>24</v>
+      </c>
       <c r="I197" s="2"/>
       <c r="J197" s="2"/>
       <c r="K197" s="2"/>
@@ -7022,20 +7323,28 @@
       <c r="V197" s="2"/>
     </row>
     <row r="198" spans="1:22" ht="15">
-      <c r="A198" s="27" t="s">
+      <c r="A198" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="B198" s="4"/>
-      <c r="C198" s="12"/>
+      <c r="B198" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C198" s="36" t="s">
+        <v>256</v>
+      </c>
       <c r="D198" s="5">
         <v>145937640</v>
       </c>
       <c r="E198" s="5">
         <v>145945394</v>
       </c>
-      <c r="F198" s="4"/>
+      <c r="F198" s="32" t="s">
+        <v>257</v>
+      </c>
       <c r="G198" s="4"/>
-      <c r="H198" s="4"/>
+      <c r="H198" s="4">
+        <v>0</v>
+      </c>
       <c r="I198" s="2"/>
       <c r="J198" s="2"/>
       <c r="K198" s="2"/>
@@ -7052,20 +7361,28 @@
       <c r="V198" s="2"/>
     </row>
     <row r="199" spans="1:22" ht="15">
-      <c r="A199" s="27" t="s">
+      <c r="A199" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="B199" s="4"/>
-      <c r="C199" s="12"/>
+      <c r="B199" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C199" s="36" t="s">
+        <v>255</v>
+      </c>
       <c r="D199" s="5">
         <v>145947155</v>
       </c>
       <c r="E199" s="5">
         <v>145959034</v>
       </c>
-      <c r="F199" s="4"/>
+      <c r="F199" s="4">
+        <v>12</v>
+      </c>
       <c r="G199" s="4"/>
-      <c r="H199" s="4"/>
+      <c r="H199" s="4">
+        <v>0</v>
+      </c>
       <c r="I199" s="2"/>
       <c r="J199" s="2"/>
       <c r="K199" s="2"/>
@@ -7082,20 +7399,28 @@
       <c r="V199" s="2"/>
     </row>
     <row r="200" spans="1:22" ht="15">
-      <c r="A200" s="27" t="s">
+      <c r="A200" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="B200" s="4"/>
-      <c r="C200" s="12"/>
+      <c r="B200" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C200" s="38" t="s">
+        <v>258</v>
+      </c>
       <c r="D200" s="5">
         <v>145965792</v>
       </c>
       <c r="E200" s="5">
         <v>146072360</v>
       </c>
-      <c r="F200" s="4"/>
+      <c r="F200" s="32" t="s">
+        <v>234</v>
+      </c>
       <c r="G200" s="4"/>
-      <c r="H200" s="4"/>
+      <c r="H200" s="4">
+        <v>3</v>
+      </c>
       <c r="I200" s="2"/>
       <c r="J200" s="2"/>
       <c r="K200" s="2"/>
@@ -7112,7 +7437,7 @@
       <c r="V200" s="2"/>
     </row>
     <row r="201" spans="1:22" ht="15">
-      <c r="A201" s="27" t="s">
+      <c r="A201" s="33" t="s">
         <v>207</v>
       </c>
       <c r="B201" s="4"/>
@@ -7142,7 +7467,7 @@
       <c r="V201" s="2"/>
     </row>
     <row r="202" spans="1:22" ht="15">
-      <c r="A202" s="27" t="s">
+      <c r="A202" s="33" t="s">
         <v>208</v>
       </c>
       <c r="B202" s="4"/>
@@ -7172,20 +7497,28 @@
       <c r="V202" s="2"/>
     </row>
     <row r="203" spans="1:22" ht="15">
-      <c r="A203" s="27" t="s">
+      <c r="A203" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="B203" s="4"/>
-      <c r="C203" s="12"/>
+      <c r="B203" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C203" s="36" t="s">
+        <v>259</v>
+      </c>
       <c r="D203" s="5">
         <v>146085595</v>
       </c>
       <c r="E203" s="5">
         <v>146195343</v>
       </c>
-      <c r="F203" s="4"/>
+      <c r="F203" s="32" t="s">
+        <v>260</v>
+      </c>
       <c r="G203" s="4"/>
-      <c r="H203" s="4"/>
+      <c r="H203" s="4">
+        <v>6</v>
+      </c>
       <c r="I203" s="2"/>
       <c r="J203" s="2"/>
       <c r="K203" s="2"/>
@@ -7202,20 +7535,28 @@
       <c r="V203" s="2"/>
     </row>
     <row r="204" spans="1:22" ht="15">
-      <c r="A204" s="27" t="s">
+      <c r="A204" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="B204" s="4"/>
-      <c r="C204" s="12"/>
+      <c r="B204" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C204" s="36" t="s">
+        <v>261</v>
+      </c>
       <c r="D204" s="5">
         <v>146236243</v>
       </c>
       <c r="E204" s="5">
         <v>146243445</v>
       </c>
-      <c r="F204" s="4"/>
+      <c r="F204" s="32" t="s">
+        <v>262</v>
+      </c>
       <c r="G204" s="4"/>
-      <c r="H204" s="4"/>
+      <c r="H204" s="4">
+        <v>9</v>
+      </c>
       <c r="I204" s="2"/>
       <c r="J204" s="2"/>
       <c r="K204" s="2"/>
@@ -7231,21 +7572,29 @@
       <c r="U204" s="2"/>
       <c r="V204" s="2"/>
     </row>
-    <row r="205" spans="1:22" ht="15">
-      <c r="A205" s="27" t="s">
+    <row r="205" spans="1:22" thickBot="1">
+      <c r="A205" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="B205" s="4"/>
-      <c r="C205" s="12"/>
+      <c r="B205" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C205" s="36" t="s">
+        <v>263</v>
+      </c>
       <c r="D205" s="5">
         <v>146282780</v>
       </c>
       <c r="E205" s="5">
         <v>146307587</v>
       </c>
-      <c r="F205" s="4"/>
+      <c r="F205" s="32" t="s">
+        <v>264</v>
+      </c>
       <c r="G205" s="4"/>
-      <c r="H205" s="4"/>
+      <c r="H205" s="4">
+        <v>24</v>
+      </c>
       <c r="I205" s="2"/>
       <c r="J205" s="2"/>
       <c r="K205" s="2"/>
@@ -7262,20 +7611,28 @@
       <c r="V205" s="2"/>
     </row>
     <row r="206" spans="1:22" ht="15">
-      <c r="A206" s="27" t="s">
+      <c r="A206" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="B206" s="11"/>
-      <c r="C206" s="20"/>
+      <c r="B206" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C206" s="31" t="s">
+        <v>265</v>
+      </c>
       <c r="D206" s="5">
         <v>146452171</v>
       </c>
       <c r="E206" s="5">
         <v>146480596</v>
       </c>
-      <c r="F206" s="4"/>
+      <c r="F206" s="32" t="s">
+        <v>266</v>
+      </c>
       <c r="G206" s="4"/>
-      <c r="H206" s="4"/>
+      <c r="H206" s="4">
+        <v>3</v>
+      </c>
       <c r="I206" s="2"/>
       <c r="J206" s="2"/>
       <c r="K206" s="2"/>
@@ -7292,18 +7649,24 @@
       <c r="V206" s="2"/>
     </row>
     <row r="207" spans="1:22" ht="15">
-      <c r="A207" s="27" t="s">
+      <c r="A207" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="B207" s="11"/>
-      <c r="C207" s="20"/>
+      <c r="B207" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C207" s="39" t="s">
+        <v>267</v>
+      </c>
       <c r="D207" s="5">
         <v>146484584</v>
       </c>
       <c r="E207" s="5">
         <v>146528594</v>
       </c>
-      <c r="F207" s="11"/>
+      <c r="F207" s="11">
+        <v>30</v>
+      </c>
       <c r="G207" s="11"/>
       <c r="H207" s="11"/>
       <c r="I207" s="2"/>
@@ -7321,8 +7684,8 @@
       <c r="U207" s="2"/>
       <c r="V207" s="2"/>
     </row>
-    <row r="208" spans="1:22" ht="15">
-      <c r="A208" s="27" t="s">
+    <row r="208" spans="1:22" thickBot="1">
+      <c r="A208" s="33" t="s">
         <v>214</v>
       </c>
       <c r="B208" s="11"/>
@@ -7351,21 +7714,29 @@
       <c r="U208" s="2"/>
       <c r="V208" s="2"/>
     </row>
-    <row r="209" spans="1:22" ht="15">
-      <c r="A209" s="27" t="s">
+    <row r="209" spans="1:22" thickBot="1">
+      <c r="A209" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="B209" s="11"/>
-      <c r="C209" s="25"/>
+      <c r="B209" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C209" s="36" t="s">
+        <v>268</v>
+      </c>
       <c r="D209" s="5">
         <v>153477636</v>
       </c>
       <c r="E209" s="5">
         <v>153498961</v>
       </c>
-      <c r="F209" s="11"/>
+      <c r="F209" s="34" t="s">
+        <v>269</v>
+      </c>
       <c r="G209" s="11"/>
-      <c r="H209" s="11"/>
+      <c r="H209" s="11">
+        <v>15</v>
+      </c>
       <c r="I209" s="2"/>
       <c r="J209" s="2"/>
       <c r="K209" s="2"/>
@@ -7382,20 +7753,28 @@
       <c r="V209" s="2"/>
     </row>
     <row r="210" spans="1:22" ht="15">
-      <c r="A210" s="27" t="s">
+      <c r="A210" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="B210" s="11"/>
-      <c r="C210" s="13"/>
+      <c r="B210" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C210" s="31" t="s">
+        <v>233</v>
+      </c>
       <c r="D210" s="5">
         <v>153722829</v>
       </c>
       <c r="E210" s="5">
         <v>153936148</v>
       </c>
-      <c r="F210" s="11"/>
+      <c r="F210" s="34" t="s">
+        <v>234</v>
+      </c>
       <c r="G210" s="11"/>
-      <c r="H210" s="11"/>
+      <c r="H210" s="11">
+        <v>6</v>
+      </c>
       <c r="I210" s="2"/>
       <c r="J210" s="2"/>
       <c r="K210" s="2"/>
@@ -7412,20 +7791,28 @@
       <c r="V210" s="2"/>
     </row>
     <row r="211" spans="1:22" ht="15">
-      <c r="A211" s="27" t="s">
+      <c r="A211" s="33" t="s">
         <v>217</v>
       </c>
-      <c r="B211" s="11"/>
-      <c r="C211" s="13"/>
+      <c r="B211" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="C211" s="33" t="s">
+        <v>227</v>
+      </c>
       <c r="D211" s="5">
         <v>153936559</v>
       </c>
       <c r="E211" s="5">
         <v>154524620</v>
       </c>
-      <c r="F211" s="11"/>
+      <c r="F211" s="34" t="s">
+        <v>228</v>
+      </c>
       <c r="G211" s="11"/>
-      <c r="H211" s="11"/>
+      <c r="H211" s="11">
+        <v>12</v>
+      </c>
       <c r="I211" s="2"/>
       <c r="J211" s="2"/>
       <c r="K211" s="2"/>
@@ -7441,8 +7828,8 @@
       <c r="U211" s="2"/>
       <c r="V211" s="2"/>
     </row>
-    <row r="212" spans="1:22" ht="15">
-      <c r="A212" s="27" t="s">
+    <row r="212" spans="1:22" thickBot="1">
+      <c r="A212" s="33" t="s">
         <v>218</v>
       </c>
       <c r="B212" s="4"/>
@@ -7472,20 +7859,28 @@
       <c r="V212" s="2"/>
     </row>
     <row r="213" spans="1:22" ht="15">
-      <c r="A213" s="27" t="s">
+      <c r="A213" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="B213" s="11"/>
-      <c r="C213" s="13"/>
+      <c r="B213" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="C213" s="31" t="s">
+        <v>229</v>
+      </c>
       <c r="D213" s="5">
         <v>155262593</v>
       </c>
       <c r="E213" s="5">
         <v>155364610</v>
       </c>
-      <c r="F213" s="11"/>
+      <c r="F213" s="34" t="s">
+        <v>230</v>
+      </c>
       <c r="G213" s="11"/>
-      <c r="H213" s="11"/>
+      <c r="H213" s="11">
+        <v>3</v>
+      </c>
       <c r="I213" s="2"/>
       <c r="J213" s="2"/>
       <c r="K213" s="2"/>
@@ -7502,20 +7897,28 @@
       <c r="V213" s="2"/>
     </row>
     <row r="214" spans="1:22" ht="15">
-      <c r="A214" s="27" t="s">
+      <c r="A214" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="B214" s="11"/>
-      <c r="C214" s="13"/>
+      <c r="B214" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C214" s="33" t="s">
+        <v>231</v>
+      </c>
       <c r="D214" s="5">
         <v>156184812</v>
       </c>
       <c r="E214" s="5">
         <v>156650711</v>
       </c>
-      <c r="F214" s="11"/>
+      <c r="F214" s="34" t="s">
+        <v>232</v>
+      </c>
       <c r="G214" s="11"/>
-      <c r="H214" s="11"/>
+      <c r="H214" s="11">
+        <v>0</v>
+      </c>
       <c r="I214" s="2"/>
       <c r="J214" s="2"/>
       <c r="K214" s="2"/>
@@ -7531,11 +7934,20 @@
       <c r="U214" s="2"/>
       <c r="V214" s="2"/>
     </row>
+    <row r="216" spans="1:22" ht="15.75" customHeight="1">
+      <c r="B216" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="C216" s="35" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit excel MODIFCANDO POR SEGUNDA ves el archivo excel
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="286">
   <si>
     <t>Localización</t>
   </si>
@@ -835,6 +835,48 @@
   </si>
   <si>
     <t>bbbbbbbbbbbbbbbbbbbbb</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>x7</t>
   </si>
 </sst>
 </file>
@@ -923,7 +965,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -957,6 +999,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF9F9F9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1034,7 +1082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1103,6 +1151,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1323,8 +1380,8 @@
   </sheetPr>
   <dimension ref="A1:V216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1382,8 +1439,12 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>279</v>
+      </c>
       <c r="D3" s="5">
         <v>32091689</v>
       </c>
@@ -1412,8 +1473,12 @@
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="41" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>280</v>
+      </c>
       <c r="D4" s="5">
         <v>32837131</v>
       </c>
@@ -1442,8 +1507,12 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="41" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>281</v>
+      </c>
       <c r="D5" s="5">
         <v>33089112</v>
       </c>
@@ -1472,8 +1541,12 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>282</v>
+      </c>
       <c r="D6" s="5">
         <v>33764252</v>
       </c>
@@ -1502,8 +1575,12 @@
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>283</v>
+      </c>
       <c r="D7" s="5">
         <v>33810174</v>
       </c>
@@ -1532,8 +1609,12 @@
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>284</v>
+      </c>
       <c r="D8" s="5">
         <v>33882149</v>
       </c>
@@ -1562,8 +1643,12 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>285</v>
+      </c>
       <c r="D9" s="5">
         <v>34199383</v>
       </c>
@@ -1592,7 +1677,7 @@
       <c r="A10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="13"/>
       <c r="D10" s="5">
         <v>34235896</v>
@@ -1622,7 +1707,7 @@
       <c r="A11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="11"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="13"/>
       <c r="D11" s="5">
         <v>34811253</v>
@@ -1652,7 +1737,7 @@
       <c r="A12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="11"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="12"/>
       <c r="D12" s="5">
         <v>34826096</v>
@@ -1682,7 +1767,7 @@
       <c r="A13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="11"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="14"/>
       <c r="D13" s="5">
         <v>34857740</v>
@@ -1712,7 +1797,7 @@
       <c r="A14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="11"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="13"/>
       <c r="D14" s="5">
         <v>34864860</v>
@@ -1742,7 +1827,7 @@
       <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="14"/>
       <c r="D15" s="5">
         <v>34960381</v>
@@ -1772,7 +1857,7 @@
       <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="13"/>
       <c r="D16" s="5">
         <v>34994565</v>

</xml_diff>

<commit_message>
APRENDI A EDITAR EL TEXTO DE REPOSITORIO DE MI COMPAÑERO
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -965,7 +965,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1005,6 +1005,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,7 +1088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1143,14 +1149,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1160,6 +1158,16 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1175,6 +1183,231 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1120140</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1432560" y="1813560"/>
+          <a:ext cx="2948940" cy="2171700"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1043940</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1501140</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Triángulo isósceles 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2004060" y="2164080"/>
+          <a:ext cx="457200" cy="464820"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2133600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Triángulo isósceles 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3093720" y="2217420"/>
+          <a:ext cx="457200" cy="464820"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1249680</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2209800" y="2994660"/>
+          <a:ext cx="1257300" cy="510540"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedUpArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1381,7 +1614,7 @@
   <dimension ref="A1:V216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1399,15 +1632,15 @@
       <c r="A1" s="25"/>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
+      <c r="E1" s="40"/>
+      <c r="F1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -1439,10 +1672,10 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="38" t="s">
         <v>279</v>
       </c>
       <c r="D3" s="5">
@@ -1451,9 +1684,9 @@
       <c r="E3" s="5">
         <v>32091761</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1473,10 +1706,10 @@
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="38" t="s">
         <v>280</v>
       </c>
       <c r="D4" s="5">
@@ -1485,9 +1718,9 @@
       <c r="E4" s="5">
         <v>32838076</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1507,10 +1740,10 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="38" t="s">
         <v>281</v>
       </c>
       <c r="D5" s="5">
@@ -1519,9 +1752,9 @@
       <c r="E5" s="5">
         <v>33090132</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1541,10 +1774,10 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="38" t="s">
         <v>282</v>
       </c>
       <c r="D6" s="5">
@@ -1553,9 +1786,9 @@
       <c r="E6" s="5">
         <v>33768221</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1575,10 +1808,10 @@
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="38" t="s">
         <v>283</v>
       </c>
       <c r="D7" s="5">
@@ -1587,9 +1820,9 @@
       <c r="E7" s="5">
         <v>33811741</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1609,10 +1842,10 @@
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="38" t="s">
         <v>284</v>
       </c>
       <c r="D8" s="5">
@@ -1621,9 +1854,9 @@
       <c r="E8" s="5">
         <v>33934641</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1643,10 +1876,10 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="38" t="s">
         <v>285</v>
       </c>
       <c r="D9" s="5">
@@ -1677,7 +1910,7 @@
       <c r="A10" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="40"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="13"/>
       <c r="D10" s="5">
         <v>34235896</v>
@@ -1707,7 +1940,7 @@
       <c r="A11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="40"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="13"/>
       <c r="D11" s="5">
         <v>34811253</v>
@@ -1737,7 +1970,7 @@
       <c r="A12" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="40"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="12"/>
       <c r="D12" s="5">
         <v>34826096</v>
@@ -1767,7 +2000,7 @@
       <c r="A13" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="40"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="14"/>
       <c r="D13" s="5">
         <v>34857740</v>
@@ -1797,7 +2030,7 @@
       <c r="A14" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="40"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="13"/>
       <c r="D14" s="5">
         <v>34864860</v>
@@ -1827,7 +2060,7 @@
       <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="40"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="14"/>
       <c r="D15" s="5">
         <v>34960381</v>
@@ -1857,7 +2090,7 @@
       <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="13"/>
       <c r="D16" s="5">
         <v>34994565</v>
@@ -8044,5 +8277,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
editando mi primer archivo excel del directorio
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUAN CARLOS DIAZ\Desktop\pc2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelly\Desktop\pc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7754F4D4-4DA8-4A3D-9BEC-DC12E4990799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9012" windowHeight="7560"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C1" sheetId="2" r:id="rId1"/>
@@ -882,7 +883,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15">
     <font>
       <sz val="10"/>
@@ -1088,7 +1089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1158,6 +1159,8 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1166,8 +1169,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,7 +1205,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvPr id="3" name="Elipse 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1256,7 +1265,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Triángulo isósceles 3"/>
+        <xdr:cNvPr id="4" name="Triángulo isósceles 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1310,7 +1325,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Triángulo isósceles 4"/>
+        <xdr:cNvPr id="5" name="Triángulo isósceles 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1364,7 +1385,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5"/>
+        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1607,24 +1634,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:V216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1632,15 +1659,15 @@
       <c r="A1" s="25"/>
       <c r="B1" s="25"/>
       <c r="C1" s="25"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -1668,7 +1695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14.4">
+    <row r="3" spans="1:22" ht="15">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1684,9 +1711,9 @@
       <c r="E3" s="5">
         <v>32091761</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1702,7 +1729,7 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="14.4">
+    <row r="4" spans="1:22" ht="15">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1718,9 +1745,9 @@
       <c r="E4" s="5">
         <v>32838076</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1736,7 +1763,7 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" ht="14.4">
+    <row r="5" spans="1:22" ht="15">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1752,9 +1779,9 @@
       <c r="E5" s="5">
         <v>33090132</v>
       </c>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1770,7 +1797,7 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="14.4">
+    <row r="6" spans="1:22" ht="15">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1786,9 +1813,9 @@
       <c r="E6" s="5">
         <v>33768221</v>
       </c>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1804,7 +1831,7 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="14.4">
+    <row r="7" spans="1:22" ht="15">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1820,9 +1847,9 @@
       <c r="E7" s="5">
         <v>33811741</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1838,7 +1865,7 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="14.4">
+    <row r="8" spans="1:22" ht="15">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -1854,9 +1881,9 @@
       <c r="E8" s="5">
         <v>33934641</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1872,7 +1899,7 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="14.4">
+    <row r="9" spans="1:22" ht="15">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -1918,8 +1945,10 @@
       <c r="E10" s="5">
         <v>34251973</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="F10" s="45">
+        <v>2</v>
+      </c>
+      <c r="G10" s="45"/>
       <c r="H10" s="11"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1936,7 +1965,7 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="14.4">
+    <row r="11" spans="1:22" ht="15">
       <c r="A11" s="26" t="s">
         <v>18</v>
       </c>
@@ -1948,8 +1977,8 @@
       <c r="E11" s="5">
         <v>34812505</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="11"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1966,7 +1995,7 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="14.4">
+    <row r="12" spans="1:22" ht="15">
       <c r="A12" s="26" t="s">
         <v>19</v>
       </c>
@@ -1978,8 +2007,8 @@
       <c r="E12" s="5">
         <v>34855603</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="11"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1996,7 +2025,7 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="14.4">
+    <row r="13" spans="1:22" ht="15">
       <c r="A13" s="26" t="s">
         <v>20</v>
       </c>
@@ -2008,8 +2037,8 @@
       <c r="E13" s="5">
         <v>34864667</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="11"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2026,7 +2055,7 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="14.4">
+    <row r="14" spans="1:22" ht="15">
       <c r="A14" s="26" t="s">
         <v>21</v>
       </c>
@@ -2038,8 +2067,8 @@
       <c r="E14" s="5">
         <v>34953982</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
       <c r="H14" s="11"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2056,7 +2085,7 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="14.4">
+    <row r="15" spans="1:22" ht="15">
       <c r="A15" s="26" t="s">
         <v>22</v>
       </c>
@@ -2068,8 +2097,8 @@
       <c r="E15" s="5">
         <v>34968544</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="4"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2086,7 +2115,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="14.4">
+    <row r="16" spans="1:22" ht="15">
       <c r="A16" s="26" t="s">
         <v>23</v>
       </c>
@@ -2098,8 +2127,8 @@
       <c r="E16" s="5">
         <v>34996018</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="4"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2116,7 +2145,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" ht="14.4">
+    <row r="17" spans="1:22" ht="15">
       <c r="A17" s="26" t="s">
         <v>24</v>
       </c>
@@ -2146,7 +2175,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22" ht="14.4">
+    <row r="18" spans="1:22" ht="15">
       <c r="A18" s="26" t="s">
         <v>25</v>
       </c>
@@ -2176,7 +2205,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" ht="14.4">
+    <row r="19" spans="1:22" ht="15">
       <c r="A19" s="26" t="s">
         <v>26</v>
       </c>
@@ -2206,7 +2235,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" ht="14.4">
+    <row r="20" spans="1:22" ht="15">
       <c r="A20" s="26" t="s">
         <v>27</v>
       </c>
@@ -2236,7 +2265,7 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="1:22" ht="14.4">
+    <row r="21" spans="1:22" ht="15">
       <c r="A21" s="26" t="s">
         <v>28</v>
       </c>
@@ -2266,7 +2295,7 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:22" ht="14.4">
+    <row r="22" spans="1:22" ht="15">
       <c r="A22" s="26" t="s">
         <v>29</v>
       </c>
@@ -2296,7 +2325,7 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="1:22" ht="14.4">
+    <row r="23" spans="1:22" ht="15">
       <c r="A23" s="26" t="s">
         <v>30</v>
       </c>
@@ -2326,7 +2355,7 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22" ht="14.4">
+    <row r="24" spans="1:22" ht="15">
       <c r="A24" s="26" t="s">
         <v>31</v>
       </c>
@@ -2356,7 +2385,7 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22" ht="14.4">
+    <row r="25" spans="1:22" ht="15">
       <c r="A25" s="26" t="s">
         <v>32</v>
       </c>
@@ -2386,7 +2415,7 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:22" ht="14.4">
+    <row r="26" spans="1:22" ht="15">
       <c r="A26" s="26" t="s">
         <v>33</v>
       </c>
@@ -2416,7 +2445,7 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:22" ht="14.4">
+    <row r="27" spans="1:22" ht="15">
       <c r="A27" s="26" t="s">
         <v>34</v>
       </c>
@@ -2446,7 +2475,7 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:22" ht="14.4">
+    <row r="28" spans="1:22" ht="15">
       <c r="A28" s="26" t="s">
         <v>35</v>
       </c>
@@ -2476,7 +2505,7 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:22" ht="14.4">
+    <row r="29" spans="1:22" ht="15">
       <c r="A29" s="26" t="s">
         <v>36</v>
       </c>
@@ -2506,7 +2535,7 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="1:22" ht="14.4">
+    <row r="30" spans="1:22" ht="15">
       <c r="A30" s="26" t="s">
         <v>37</v>
       </c>
@@ -2536,7 +2565,7 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:22" ht="14.4">
+    <row r="31" spans="1:22" ht="15">
       <c r="A31" s="26" t="s">
         <v>38</v>
       </c>
@@ -2566,7 +2595,7 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:22" ht="14.4">
+    <row r="32" spans="1:22" ht="15">
       <c r="A32" s="26" t="s">
         <v>39</v>
       </c>
@@ -2596,7 +2625,7 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:22" ht="14.4">
+    <row r="33" spans="1:22" ht="15">
       <c r="A33" s="26" t="s">
         <v>40</v>
       </c>
@@ -2626,7 +2655,7 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:22" ht="14.4">
+    <row r="34" spans="1:22" ht="15">
       <c r="A34" s="26" t="s">
         <v>41</v>
       </c>
@@ -2656,7 +2685,7 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="1:22" ht="14.4">
+    <row r="35" spans="1:22" ht="15">
       <c r="A35" s="26" t="s">
         <v>42</v>
       </c>
@@ -2686,7 +2715,7 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:22" ht="14.4">
+    <row r="36" spans="1:22" ht="15">
       <c r="A36" s="26" t="s">
         <v>43</v>
       </c>
@@ -2716,7 +2745,7 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="1:22" ht="14.4">
+    <row r="37" spans="1:22" ht="15">
       <c r="A37" s="26" t="s">
         <v>44</v>
       </c>
@@ -2746,7 +2775,7 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
     </row>
-    <row r="38" spans="1:22" ht="14.4">
+    <row r="38" spans="1:22" ht="15">
       <c r="A38" s="26" t="s">
         <v>45</v>
       </c>
@@ -2776,7 +2805,7 @@
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
     </row>
-    <row r="39" spans="1:22" ht="14.4">
+    <row r="39" spans="1:22" ht="15">
       <c r="A39" s="26" t="s">
         <v>46</v>
       </c>
@@ -2806,7 +2835,7 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" ht="14.4">
+    <row r="40" spans="1:22" ht="15">
       <c r="A40" s="26" t="s">
         <v>47</v>
       </c>
@@ -2836,7 +2865,7 @@
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:22" ht="14.4">
+    <row r="41" spans="1:22" ht="15">
       <c r="A41" s="26" t="s">
         <v>48</v>
       </c>
@@ -2866,7 +2895,7 @@
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:22" ht="14.4">
+    <row r="42" spans="1:22" ht="15">
       <c r="A42" s="26" t="s">
         <v>49</v>
       </c>
@@ -2896,7 +2925,7 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:22" ht="14.4">
+    <row r="43" spans="1:22" ht="15">
       <c r="A43" s="26" t="s">
         <v>50</v>
       </c>
@@ -2926,7 +2955,7 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:22" ht="14.4">
+    <row r="44" spans="1:22" ht="15">
       <c r="A44" s="26" t="s">
         <v>51</v>
       </c>
@@ -2956,7 +2985,7 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:22" ht="14.4">
+    <row r="45" spans="1:22" ht="15">
       <c r="A45" s="26" t="s">
         <v>52</v>
       </c>
@@ -2986,7 +3015,7 @@
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="1:22" ht="14.4">
+    <row r="46" spans="1:22" ht="15">
       <c r="A46" s="26" t="s">
         <v>53</v>
       </c>
@@ -3016,7 +3045,7 @@
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="1:22" ht="14.4">
+    <row r="47" spans="1:22" ht="15">
       <c r="A47" s="26" t="s">
         <v>54</v>
       </c>
@@ -3046,7 +3075,7 @@
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="1:22" ht="14.4">
+    <row r="48" spans="1:22" ht="15">
       <c r="A48" s="26" t="s">
         <v>55</v>
       </c>
@@ -3076,7 +3105,7 @@
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
     </row>
-    <row r="49" spans="1:22" ht="14.4">
+    <row r="49" spans="1:22" ht="15">
       <c r="A49" s="26" t="s">
         <v>56</v>
       </c>
@@ -3106,7 +3135,7 @@
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
     </row>
-    <row r="50" spans="1:22" ht="14.4">
+    <row r="50" spans="1:22" ht="15">
       <c r="A50" s="26" t="s">
         <v>57</v>
       </c>
@@ -3136,7 +3165,7 @@
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
     </row>
-    <row r="51" spans="1:22" ht="14.4">
+    <row r="51" spans="1:22" ht="15">
       <c r="A51" s="26" t="s">
         <v>58</v>
       </c>
@@ -3166,7 +3195,7 @@
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
     </row>
-    <row r="52" spans="1:22" ht="14.4">
+    <row r="52" spans="1:22" ht="15">
       <c r="A52" s="26" t="s">
         <v>59</v>
       </c>
@@ -3196,7 +3225,7 @@
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
     </row>
-    <row r="53" spans="1:22" ht="14.4">
+    <row r="53" spans="1:22" ht="15">
       <c r="A53" s="26" t="s">
         <v>60</v>
       </c>
@@ -3226,7 +3255,7 @@
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
     </row>
-    <row r="54" spans="1:22" ht="14.4">
+    <row r="54" spans="1:22" ht="15">
       <c r="A54" s="26" t="s">
         <v>61</v>
       </c>
@@ -3256,7 +3285,7 @@
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
     </row>
-    <row r="55" spans="1:22" ht="14.4">
+    <row r="55" spans="1:22" ht="15">
       <c r="A55" s="26" t="s">
         <v>62</v>
       </c>
@@ -3286,7 +3315,7 @@
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
     </row>
-    <row r="56" spans="1:22" ht="14.4">
+    <row r="56" spans="1:22" ht="15">
       <c r="A56" s="26" t="s">
         <v>63</v>
       </c>
@@ -3316,7 +3345,7 @@
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
     </row>
-    <row r="57" spans="1:22" ht="14.4">
+    <row r="57" spans="1:22" ht="15">
       <c r="A57" s="26" t="s">
         <v>64</v>
       </c>
@@ -3346,7 +3375,7 @@
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
     </row>
-    <row r="58" spans="1:22" ht="14.4">
+    <row r="58" spans="1:22" ht="15">
       <c r="A58" s="26" t="s">
         <v>65</v>
       </c>
@@ -3376,7 +3405,7 @@
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
     </row>
-    <row r="59" spans="1:22" ht="14.4">
+    <row r="59" spans="1:22" ht="15">
       <c r="A59" s="26" t="s">
         <v>66</v>
       </c>
@@ -3406,7 +3435,7 @@
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
     </row>
-    <row r="60" spans="1:22" ht="14.4">
+    <row r="60" spans="1:22" ht="15">
       <c r="A60" s="26" t="s">
         <v>67</v>
       </c>
@@ -3436,7 +3465,7 @@
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
     </row>
-    <row r="61" spans="1:22" ht="14.4">
+    <row r="61" spans="1:22" ht="15">
       <c r="A61" s="26" t="s">
         <v>68</v>
       </c>
@@ -3466,7 +3495,7 @@
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
     </row>
-    <row r="62" spans="1:22" ht="14.4">
+    <row r="62" spans="1:22" ht="15">
       <c r="A62" s="26" t="s">
         <v>69</v>
       </c>
@@ -3496,7 +3525,7 @@
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
     </row>
-    <row r="63" spans="1:22" ht="14.4">
+    <row r="63" spans="1:22" ht="15">
       <c r="A63" s="26" t="s">
         <v>70</v>
       </c>
@@ -3526,7 +3555,7 @@
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
     </row>
-    <row r="64" spans="1:22" ht="14.4">
+    <row r="64" spans="1:22" ht="15">
       <c r="A64" s="26" t="s">
         <v>71</v>
       </c>
@@ -3556,7 +3585,7 @@
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
     </row>
-    <row r="65" spans="1:22" ht="14.4">
+    <row r="65" spans="1:22" ht="15">
       <c r="A65" s="26" t="s">
         <v>72</v>
       </c>
@@ -3586,7 +3615,7 @@
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
     </row>
-    <row r="66" spans="1:22" ht="14.4">
+    <row r="66" spans="1:22" ht="15">
       <c r="A66" s="26" t="s">
         <v>73</v>
       </c>
@@ -3616,7 +3645,7 @@
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
     </row>
-    <row r="67" spans="1:22" ht="14.4">
+    <row r="67" spans="1:22" ht="15">
       <c r="A67" s="26" t="s">
         <v>74</v>
       </c>
@@ -3646,7 +3675,7 @@
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
     </row>
-    <row r="68" spans="1:22" ht="14.4">
+    <row r="68" spans="1:22" ht="15">
       <c r="A68" s="26" t="s">
         <v>75</v>
       </c>
@@ -3676,7 +3705,7 @@
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
     </row>
-    <row r="69" spans="1:22" ht="14.4">
+    <row r="69" spans="1:22" ht="15">
       <c r="A69" s="26" t="s">
         <v>76</v>
       </c>
@@ -3706,7 +3735,7 @@
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
     </row>
-    <row r="70" spans="1:22" ht="14.4">
+    <row r="70" spans="1:22" ht="15">
       <c r="A70" s="26" t="s">
         <v>77</v>
       </c>
@@ -3736,7 +3765,7 @@
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
     </row>
-    <row r="71" spans="1:22" ht="14.4">
+    <row r="71" spans="1:22" ht="15">
       <c r="A71" s="26" t="s">
         <v>78</v>
       </c>
@@ -3766,7 +3795,7 @@
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
     </row>
-    <row r="72" spans="1:22" ht="14.4">
+    <row r="72" spans="1:22" ht="15">
       <c r="A72" s="26" t="s">
         <v>79</v>
       </c>
@@ -3796,7 +3825,7 @@
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
     </row>
-    <row r="73" spans="1:22" ht="14.4">
+    <row r="73" spans="1:22" ht="15">
       <c r="A73" s="26" t="s">
         <v>80</v>
       </c>
@@ -3826,7 +3855,7 @@
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
     </row>
-    <row r="74" spans="1:22" ht="14.4">
+    <row r="74" spans="1:22" ht="15">
       <c r="A74" s="26" t="s">
         <v>81</v>
       </c>
@@ -3856,7 +3885,7 @@
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
     </row>
-    <row r="75" spans="1:22" ht="14.4">
+    <row r="75" spans="1:22" ht="15">
       <c r="A75" s="26" t="s">
         <v>82</v>
       </c>
@@ -3886,7 +3915,7 @@
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
     </row>
-    <row r="76" spans="1:22" ht="14.4">
+    <row r="76" spans="1:22" ht="15">
       <c r="A76" s="26" t="s">
         <v>83</v>
       </c>
@@ -3916,7 +3945,7 @@
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
     </row>
-    <row r="77" spans="1:22" ht="14.4">
+    <row r="77" spans="1:22" ht="15">
       <c r="A77" s="26" t="s">
         <v>84</v>
       </c>
@@ -3946,7 +3975,7 @@
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
     </row>
-    <row r="78" spans="1:22" ht="14.4">
+    <row r="78" spans="1:22" ht="15">
       <c r="A78" s="26" t="s">
         <v>85</v>
       </c>
@@ -3976,7 +4005,7 @@
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
     </row>
-    <row r="79" spans="1:22" ht="14.4">
+    <row r="79" spans="1:22" ht="15">
       <c r="A79" s="26" t="s">
         <v>86</v>
       </c>
@@ -4006,7 +4035,7 @@
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
     </row>
-    <row r="80" spans="1:22" ht="14.4">
+    <row r="80" spans="1:22" ht="15">
       <c r="A80" s="26" t="s">
         <v>87</v>
       </c>
@@ -4036,7 +4065,7 @@
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
     </row>
-    <row r="81" spans="1:22" ht="14.4">
+    <row r="81" spans="1:22" ht="15">
       <c r="A81" s="26" t="s">
         <v>88</v>
       </c>
@@ -4066,7 +4095,7 @@
       <c r="U81" s="2"/>
       <c r="V81" s="2"/>
     </row>
-    <row r="82" spans="1:22" ht="14.4">
+    <row r="82" spans="1:22" ht="15">
       <c r="A82" s="26" t="s">
         <v>89</v>
       </c>
@@ -4096,7 +4125,7 @@
       <c r="U82" s="2"/>
       <c r="V82" s="2"/>
     </row>
-    <row r="83" spans="1:22" ht="14.4">
+    <row r="83" spans="1:22" ht="15">
       <c r="A83" s="26" t="s">
         <v>90</v>
       </c>
@@ -4126,7 +4155,7 @@
       <c r="U83" s="2"/>
       <c r="V83" s="2"/>
     </row>
-    <row r="84" spans="1:22" ht="14.4">
+    <row r="84" spans="1:22" ht="15">
       <c r="A84" s="26" t="s">
         <v>91</v>
       </c>
@@ -4156,7 +4185,7 @@
       <c r="U84" s="2"/>
       <c r="V84" s="2"/>
     </row>
-    <row r="85" spans="1:22" ht="14.4">
+    <row r="85" spans="1:22" ht="15">
       <c r="A85" s="26" t="s">
         <v>92</v>
       </c>
@@ -4186,7 +4215,7 @@
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
     </row>
-    <row r="86" spans="1:22" ht="14.4">
+    <row r="86" spans="1:22" ht="15">
       <c r="A86" s="26" t="s">
         <v>93</v>
       </c>
@@ -4216,7 +4245,7 @@
       <c r="U86" s="2"/>
       <c r="V86" s="2"/>
     </row>
-    <row r="87" spans="1:22" ht="14.4">
+    <row r="87" spans="1:22" ht="15">
       <c r="A87" s="26" t="s">
         <v>94</v>
       </c>
@@ -4246,7 +4275,7 @@
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
     </row>
-    <row r="88" spans="1:22" ht="14.4">
+    <row r="88" spans="1:22" ht="15">
       <c r="A88" s="26" t="s">
         <v>95</v>
       </c>
@@ -4276,7 +4305,7 @@
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
     </row>
-    <row r="89" spans="1:22" ht="14.4">
+    <row r="89" spans="1:22" ht="15">
       <c r="A89" s="26" t="s">
         <v>96</v>
       </c>
@@ -4306,7 +4335,7 @@
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>
     </row>
-    <row r="90" spans="1:22" ht="14.4">
+    <row r="90" spans="1:22" ht="15">
       <c r="A90" s="26" t="s">
         <v>97</v>
       </c>
@@ -4336,7 +4365,7 @@
       <c r="U90" s="2"/>
       <c r="V90" s="2"/>
     </row>
-    <row r="91" spans="1:22" ht="14.4">
+    <row r="91" spans="1:22" ht="15">
       <c r="A91" s="26" t="s">
         <v>98</v>
       </c>
@@ -4366,7 +4395,7 @@
       <c r="U91" s="2"/>
       <c r="V91" s="2"/>
     </row>
-    <row r="92" spans="1:22" ht="14.4">
+    <row r="92" spans="1:22" ht="15">
       <c r="A92" s="26" t="s">
         <v>99</v>
       </c>
@@ -4400,7 +4429,7 @@
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
     </row>
-    <row r="93" spans="1:22" ht="14.4">
+    <row r="93" spans="1:22" ht="15">
       <c r="A93" s="26" t="s">
         <v>100</v>
       </c>
@@ -4430,7 +4459,7 @@
       <c r="U93" s="2"/>
       <c r="V93" s="2"/>
     </row>
-    <row r="94" spans="1:22" ht="14.4">
+    <row r="94" spans="1:22" ht="15">
       <c r="A94" s="26" t="s">
         <v>101</v>
       </c>
@@ -4460,7 +4489,7 @@
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
     </row>
-    <row r="95" spans="1:22" ht="14.4">
+    <row r="95" spans="1:22" ht="15">
       <c r="A95" s="26" t="s">
         <v>102</v>
       </c>
@@ -4490,7 +4519,7 @@
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
     </row>
-    <row r="96" spans="1:22" ht="14.4">
+    <row r="96" spans="1:22" ht="15">
       <c r="A96" s="26" t="s">
         <v>103</v>
       </c>
@@ -4520,7 +4549,7 @@
       <c r="U96" s="2"/>
       <c r="V96" s="2"/>
     </row>
-    <row r="97" spans="1:22" ht="14.4">
+    <row r="97" spans="1:22" ht="15">
       <c r="A97" s="26" t="s">
         <v>104</v>
       </c>
@@ -4550,7 +4579,7 @@
       <c r="U97" s="2"/>
       <c r="V97" s="2"/>
     </row>
-    <row r="98" spans="1:22" ht="14.4">
+    <row r="98" spans="1:22" ht="15">
       <c r="A98" s="26" t="s">
         <v>105</v>
       </c>
@@ -4580,7 +4609,7 @@
       <c r="U98" s="2"/>
       <c r="V98" s="2"/>
     </row>
-    <row r="99" spans="1:22" ht="14.4">
+    <row r="99" spans="1:22" ht="15">
       <c r="A99" s="26" t="s">
         <v>106</v>
       </c>
@@ -4610,7 +4639,7 @@
       <c r="U99" s="2"/>
       <c r="V99" s="2"/>
     </row>
-    <row r="100" spans="1:22" ht="14.4">
+    <row r="100" spans="1:22" ht="15">
       <c r="A100" s="26" t="s">
         <v>107</v>
       </c>
@@ -4640,7 +4669,7 @@
       <c r="U100" s="2"/>
       <c r="V100" s="2"/>
     </row>
-    <row r="101" spans="1:22" ht="14.4">
+    <row r="101" spans="1:22" ht="15">
       <c r="A101" s="26" t="s">
         <v>108</v>
       </c>
@@ -4670,7 +4699,7 @@
       <c r="U101" s="2"/>
       <c r="V101" s="2"/>
     </row>
-    <row r="102" spans="1:22" ht="14.4">
+    <row r="102" spans="1:22" ht="15">
       <c r="A102" s="26" t="s">
         <v>109</v>
       </c>
@@ -4700,7 +4729,7 @@
       <c r="U102" s="2"/>
       <c r="V102" s="2"/>
     </row>
-    <row r="103" spans="1:22" ht="14.4">
+    <row r="103" spans="1:22" ht="15">
       <c r="A103" s="26" t="s">
         <v>110</v>
       </c>
@@ -4730,7 +4759,7 @@
       <c r="U103" s="2"/>
       <c r="V103" s="2"/>
     </row>
-    <row r="104" spans="1:22" ht="14.4">
+    <row r="104" spans="1:22" ht="15">
       <c r="A104" s="26" t="s">
         <v>111</v>
       </c>
@@ -4760,7 +4789,7 @@
       <c r="U104" s="2"/>
       <c r="V104" s="2"/>
     </row>
-    <row r="105" spans="1:22" ht="14.4">
+    <row r="105" spans="1:22" ht="15">
       <c r="A105" s="26" t="s">
         <v>112</v>
       </c>
@@ -4790,7 +4819,7 @@
       <c r="U105" s="2"/>
       <c r="V105" s="2"/>
     </row>
-    <row r="106" spans="1:22" ht="14.4">
+    <row r="106" spans="1:22" ht="15">
       <c r="A106" s="26" t="s">
         <v>113</v>
       </c>
@@ -4820,7 +4849,7 @@
       <c r="U106" s="2"/>
       <c r="V106" s="2"/>
     </row>
-    <row r="107" spans="1:22" ht="14.4">
+    <row r="107" spans="1:22" ht="15">
       <c r="A107" s="26" t="s">
         <v>114</v>
       </c>
@@ -4850,7 +4879,7 @@
       <c r="U107" s="2"/>
       <c r="V107" s="2"/>
     </row>
-    <row r="108" spans="1:22" ht="14.4">
+    <row r="108" spans="1:22" ht="15">
       <c r="A108" s="26" t="s">
         <v>115</v>
       </c>
@@ -4880,7 +4909,7 @@
       <c r="U108" s="2"/>
       <c r="V108" s="2"/>
     </row>
-    <row r="109" spans="1:22" ht="14.4">
+    <row r="109" spans="1:22" ht="15">
       <c r="A109" s="26" t="s">
         <v>116</v>
       </c>
@@ -4910,7 +4939,7 @@
       <c r="U109" s="2"/>
       <c r="V109" s="2"/>
     </row>
-    <row r="110" spans="1:22" ht="14.4">
+    <row r="110" spans="1:22" ht="15">
       <c r="A110" s="26" t="s">
         <v>117</v>
       </c>
@@ -4940,7 +4969,7 @@
       <c r="U110" s="2"/>
       <c r="V110" s="2"/>
     </row>
-    <row r="111" spans="1:22" ht="14.4">
+    <row r="111" spans="1:22" ht="15">
       <c r="A111" s="26" t="s">
         <v>118</v>
       </c>
@@ -4970,7 +4999,7 @@
       <c r="U111" s="2"/>
       <c r="V111" s="2"/>
     </row>
-    <row r="112" spans="1:22" ht="14.4">
+    <row r="112" spans="1:22" ht="15">
       <c r="A112" s="26" t="s">
         <v>119</v>
       </c>
@@ -5000,7 +5029,7 @@
       <c r="U112" s="2"/>
       <c r="V112" s="2"/>
     </row>
-    <row r="113" spans="1:22" ht="14.4">
+    <row r="113" spans="1:22" ht="15">
       <c r="A113" s="26" t="s">
         <v>120</v>
       </c>
@@ -5030,7 +5059,7 @@
       <c r="U113" s="2"/>
       <c r="V113" s="2"/>
     </row>
-    <row r="114" spans="1:22" ht="14.4">
+    <row r="114" spans="1:22" ht="15">
       <c r="A114" s="26" t="s">
         <v>121</v>
       </c>
@@ -5060,7 +5089,7 @@
       <c r="U114" s="2"/>
       <c r="V114" s="2"/>
     </row>
-    <row r="115" spans="1:22" ht="14.4">
+    <row r="115" spans="1:22" ht="15">
       <c r="A115" s="26" t="s">
         <v>122</v>
       </c>
@@ -5090,7 +5119,7 @@
       <c r="U115" s="2"/>
       <c r="V115" s="2"/>
     </row>
-    <row r="116" spans="1:22" ht="14.4">
+    <row r="116" spans="1:22" ht="15">
       <c r="A116" s="26" t="s">
         <v>123</v>
       </c>
@@ -5120,7 +5149,7 @@
       <c r="U116" s="2"/>
       <c r="V116" s="2"/>
     </row>
-    <row r="117" spans="1:22" ht="14.4">
+    <row r="117" spans="1:22" ht="15">
       <c r="A117" s="26" t="s">
         <v>124</v>
       </c>
@@ -5150,7 +5179,7 @@
       <c r="U117" s="2"/>
       <c r="V117" s="2"/>
     </row>
-    <row r="118" spans="1:22" ht="14.4">
+    <row r="118" spans="1:22" ht="15">
       <c r="A118" s="26" t="s">
         <v>125</v>
       </c>
@@ -5180,7 +5209,7 @@
       <c r="U118" s="2"/>
       <c r="V118" s="2"/>
     </row>
-    <row r="119" spans="1:22" ht="14.4">
+    <row r="119" spans="1:22" ht="15">
       <c r="A119" s="26" t="s">
         <v>126</v>
       </c>
@@ -5210,7 +5239,7 @@
       <c r="U119" s="2"/>
       <c r="V119" s="2"/>
     </row>
-    <row r="120" spans="1:22" ht="14.4">
+    <row r="120" spans="1:22" ht="15">
       <c r="A120" s="26" t="s">
         <v>127</v>
       </c>
@@ -5240,7 +5269,7 @@
       <c r="U120" s="2"/>
       <c r="V120" s="2"/>
     </row>
-    <row r="121" spans="1:22" ht="14.4">
+    <row r="121" spans="1:22" ht="15">
       <c r="A121" s="26" t="s">
         <v>10</v>
       </c>
@@ -5270,7 +5299,7 @@
       <c r="U121" s="2"/>
       <c r="V121" s="2"/>
     </row>
-    <row r="122" spans="1:22" ht="14.4">
+    <row r="122" spans="1:22" ht="15">
       <c r="A122" s="26" t="s">
         <v>128</v>
       </c>
@@ -5300,7 +5329,7 @@
       <c r="U122" s="2"/>
       <c r="V122" s="2"/>
     </row>
-    <row r="123" spans="1:22" ht="14.4">
+    <row r="123" spans="1:22" ht="15">
       <c r="A123" s="26" t="s">
         <v>129</v>
       </c>
@@ -5330,7 +5359,7 @@
       <c r="U123" s="2"/>
       <c r="V123" s="2"/>
     </row>
-    <row r="124" spans="1:22" ht="14.4">
+    <row r="124" spans="1:22" ht="15">
       <c r="A124" s="26" t="s">
         <v>130</v>
       </c>
@@ -5360,7 +5389,7 @@
       <c r="U124" s="2"/>
       <c r="V124" s="2"/>
     </row>
-    <row r="125" spans="1:22" ht="14.4">
+    <row r="125" spans="1:22" ht="15">
       <c r="A125" s="26" t="s">
         <v>131</v>
       </c>
@@ -5390,7 +5419,7 @@
       <c r="U125" s="2"/>
       <c r="V125" s="2"/>
     </row>
-    <row r="126" spans="1:22" ht="14.4">
+    <row r="126" spans="1:22" ht="15">
       <c r="A126" s="26" t="s">
         <v>132</v>
       </c>
@@ -5420,7 +5449,7 @@
       <c r="U126" s="2"/>
       <c r="V126" s="2"/>
     </row>
-    <row r="127" spans="1:22" ht="14.4">
+    <row r="127" spans="1:22" ht="15">
       <c r="A127" s="26" t="s">
         <v>133</v>
       </c>
@@ -5450,7 +5479,7 @@
       <c r="U127" s="2"/>
       <c r="V127" s="2"/>
     </row>
-    <row r="128" spans="1:22" ht="14.4">
+    <row r="128" spans="1:22" ht="15">
       <c r="A128" s="26" t="s">
         <v>134</v>
       </c>
@@ -5480,7 +5509,7 @@
       <c r="U128" s="2"/>
       <c r="V128" s="2"/>
     </row>
-    <row r="129" spans="1:22" ht="14.4">
+    <row r="129" spans="1:22" ht="15">
       <c r="A129" s="26" t="s">
         <v>135</v>
       </c>
@@ -5510,7 +5539,7 @@
       <c r="U129" s="2"/>
       <c r="V129" s="2"/>
     </row>
-    <row r="130" spans="1:22" ht="14.4">
+    <row r="130" spans="1:22" ht="15">
       <c r="A130" s="26" t="s">
         <v>136</v>
       </c>
@@ -5540,7 +5569,7 @@
       <c r="U130" s="2"/>
       <c r="V130" s="2"/>
     </row>
-    <row r="131" spans="1:22" ht="14.4">
+    <row r="131" spans="1:22" ht="15">
       <c r="A131" s="26" t="s">
         <v>137</v>
       </c>
@@ -5570,7 +5599,7 @@
       <c r="U131" s="2"/>
       <c r="V131" s="2"/>
     </row>
-    <row r="132" spans="1:22" ht="14.4">
+    <row r="132" spans="1:22" ht="15">
       <c r="A132" s="26" t="s">
         <v>138</v>
       </c>
@@ -5600,7 +5629,7 @@
       <c r="U132" s="2"/>
       <c r="V132" s="2"/>
     </row>
-    <row r="133" spans="1:22" ht="14.4">
+    <row r="133" spans="1:22" ht="15">
       <c r="A133" s="26" t="s">
         <v>139</v>
       </c>
@@ -5630,7 +5659,7 @@
       <c r="U133" s="2"/>
       <c r="V133" s="2"/>
     </row>
-    <row r="134" spans="1:22" ht="14.4">
+    <row r="134" spans="1:22" ht="15">
       <c r="A134" s="26" t="s">
         <v>140</v>
       </c>
@@ -5660,7 +5689,7 @@
       <c r="U134" s="2"/>
       <c r="V134" s="2"/>
     </row>
-    <row r="135" spans="1:22" ht="14.4">
+    <row r="135" spans="1:22" ht="15">
       <c r="A135" s="26" t="s">
         <v>141</v>
       </c>
@@ -5690,7 +5719,7 @@
       <c r="U135" s="2"/>
       <c r="V135" s="2"/>
     </row>
-    <row r="136" spans="1:22" ht="14.4">
+    <row r="136" spans="1:22" ht="15">
       <c r="A136" s="26" t="s">
         <v>142</v>
       </c>
@@ -5720,7 +5749,7 @@
       <c r="U136" s="2"/>
       <c r="V136" s="2"/>
     </row>
-    <row r="137" spans="1:22" ht="14.4">
+    <row r="137" spans="1:22" ht="15">
       <c r="A137" s="26" t="s">
         <v>143</v>
       </c>
@@ -5750,7 +5779,7 @@
       <c r="U137" s="2"/>
       <c r="V137" s="2"/>
     </row>
-    <row r="138" spans="1:22" ht="14.4">
+    <row r="138" spans="1:22" ht="15">
       <c r="A138" s="26" t="s">
         <v>144</v>
       </c>
@@ -5780,7 +5809,7 @@
       <c r="U138" s="2"/>
       <c r="V138" s="2"/>
     </row>
-    <row r="139" spans="1:22" ht="14.4">
+    <row r="139" spans="1:22" ht="15">
       <c r="A139" s="26" t="s">
         <v>145</v>
       </c>
@@ -5810,7 +5839,7 @@
       <c r="U139" s="2"/>
       <c r="V139" s="2"/>
     </row>
-    <row r="140" spans="1:22" ht="14.4">
+    <row r="140" spans="1:22" ht="15">
       <c r="A140" s="26" t="s">
         <v>146</v>
       </c>
@@ -5840,7 +5869,7 @@
       <c r="U140" s="2"/>
       <c r="V140" s="2"/>
     </row>
-    <row r="141" spans="1:22" ht="14.4">
+    <row r="141" spans="1:22" ht="15">
       <c r="A141" s="26" t="s">
         <v>147</v>
       </c>
@@ -5870,7 +5899,7 @@
       <c r="U141" s="2"/>
       <c r="V141" s="2"/>
     </row>
-    <row r="142" spans="1:22" ht="14.4">
+    <row r="142" spans="1:22" ht="15">
       <c r="A142" s="26" t="s">
         <v>148</v>
       </c>
@@ -5900,7 +5929,7 @@
       <c r="U142" s="2"/>
       <c r="V142" s="2"/>
     </row>
-    <row r="143" spans="1:22" ht="14.4">
+    <row r="143" spans="1:22" ht="15">
       <c r="A143" s="26" t="s">
         <v>149</v>
       </c>
@@ -5930,7 +5959,7 @@
       <c r="U143" s="2"/>
       <c r="V143" s="2"/>
     </row>
-    <row r="144" spans="1:22" ht="14.4">
+    <row r="144" spans="1:22" ht="15">
       <c r="A144" s="26" t="s">
         <v>150</v>
       </c>
@@ -5960,7 +5989,7 @@
       <c r="U144" s="2"/>
       <c r="V144" s="2"/>
     </row>
-    <row r="145" spans="1:22" ht="14.4">
+    <row r="145" spans="1:22" ht="15">
       <c r="A145" s="26" t="s">
         <v>151</v>
       </c>
@@ -5990,7 +6019,7 @@
       <c r="U145" s="2"/>
       <c r="V145" s="2"/>
     </row>
-    <row r="146" spans="1:22" ht="14.4">
+    <row r="146" spans="1:22" ht="15">
       <c r="A146" s="26" t="s">
         <v>152</v>
       </c>
@@ -6020,7 +6049,7 @@
       <c r="U146" s="2"/>
       <c r="V146" s="2"/>
     </row>
-    <row r="147" spans="1:22" ht="14.4">
+    <row r="147" spans="1:22" ht="15">
       <c r="A147" s="26" t="s">
         <v>153</v>
       </c>
@@ -6050,7 +6079,7 @@
       <c r="U147" s="2"/>
       <c r="V147" s="2"/>
     </row>
-    <row r="148" spans="1:22" ht="14.4">
+    <row r="148" spans="1:22" ht="15">
       <c r="A148" s="26" t="s">
         <v>154</v>
       </c>
@@ -6080,7 +6109,7 @@
       <c r="U148" s="2"/>
       <c r="V148" s="2"/>
     </row>
-    <row r="149" spans="1:22" ht="14.4">
+    <row r="149" spans="1:22" ht="15">
       <c r="A149" s="26" t="s">
         <v>155</v>
       </c>
@@ -6110,7 +6139,7 @@
       <c r="U149" s="2"/>
       <c r="V149" s="2"/>
     </row>
-    <row r="150" spans="1:22" ht="15" thickBot="1">
+    <row r="150" spans="1:22" thickBot="1">
       <c r="A150" s="26" t="s">
         <v>156</v>
       </c>
@@ -6178,7 +6207,7 @@
       <c r="U151" s="2"/>
       <c r="V151" s="2"/>
     </row>
-    <row r="152" spans="1:22" ht="14.4">
+    <row r="152" spans="1:22" ht="15">
       <c r="A152" s="26" t="s">
         <v>158</v>
       </c>
@@ -6208,7 +6237,7 @@
       <c r="U152" s="2"/>
       <c r="V152" s="2"/>
     </row>
-    <row r="153" spans="1:22" ht="14.4">
+    <row r="153" spans="1:22" ht="15">
       <c r="A153" s="26" t="s">
         <v>159</v>
       </c>
@@ -6238,7 +6267,7 @@
       <c r="U153" s="2"/>
       <c r="V153" s="2"/>
     </row>
-    <row r="154" spans="1:22" ht="14.4">
+    <row r="154" spans="1:22" ht="15">
       <c r="A154" s="26" t="s">
         <v>160</v>
       </c>
@@ -6268,7 +6297,7 @@
       <c r="U154" s="2"/>
       <c r="V154" s="2"/>
     </row>
-    <row r="155" spans="1:22" ht="14.4">
+    <row r="155" spans="1:22" ht="15">
       <c r="A155" s="26" t="s">
         <v>161</v>
       </c>
@@ -6298,7 +6327,7 @@
       <c r="U155" s="2"/>
       <c r="V155" s="2"/>
     </row>
-    <row r="156" spans="1:22" ht="14.4">
+    <row r="156" spans="1:22" ht="15">
       <c r="A156" s="26" t="s">
         <v>162</v>
       </c>
@@ -6328,7 +6357,7 @@
       <c r="U156" s="2"/>
       <c r="V156" s="2"/>
     </row>
-    <row r="157" spans="1:22" ht="14.4">
+    <row r="157" spans="1:22" ht="15">
       <c r="A157" s="26" t="s">
         <v>163</v>
       </c>
@@ -6358,7 +6387,7 @@
       <c r="U157" s="2"/>
       <c r="V157" s="2"/>
     </row>
-    <row r="158" spans="1:22" ht="14.4">
+    <row r="158" spans="1:22" ht="15">
       <c r="A158" s="26" t="s">
         <v>164</v>
       </c>
@@ -6388,7 +6417,7 @@
       <c r="U158" s="2"/>
       <c r="V158" s="2"/>
     </row>
-    <row r="159" spans="1:22" ht="14.4">
+    <row r="159" spans="1:22" ht="15">
       <c r="A159" s="26" t="s">
         <v>165</v>
       </c>
@@ -6418,7 +6447,7 @@
       <c r="U159" s="2"/>
       <c r="V159" s="2"/>
     </row>
-    <row r="160" spans="1:22" ht="14.4">
+    <row r="160" spans="1:22" ht="15">
       <c r="A160" s="26" t="s">
         <v>166</v>
       </c>
@@ -6448,7 +6477,7 @@
       <c r="U160" s="2"/>
       <c r="V160" s="2"/>
     </row>
-    <row r="161" spans="1:22" ht="14.4">
+    <row r="161" spans="1:22" ht="15">
       <c r="A161" s="26" t="s">
         <v>167</v>
       </c>
@@ -6478,7 +6507,7 @@
       <c r="U161" s="2"/>
       <c r="V161" s="2"/>
     </row>
-    <row r="162" spans="1:22" ht="14.4">
+    <row r="162" spans="1:22" ht="15">
       <c r="A162" s="26" t="s">
         <v>168</v>
       </c>
@@ -6508,7 +6537,7 @@
       <c r="U162" s="2"/>
       <c r="V162" s="2"/>
     </row>
-    <row r="163" spans="1:22" ht="14.4">
+    <row r="163" spans="1:22" ht="15">
       <c r="A163" s="26" t="s">
         <v>169</v>
       </c>
@@ -6538,7 +6567,7 @@
       <c r="U163" s="2"/>
       <c r="V163" s="2"/>
     </row>
-    <row r="164" spans="1:22" ht="14.4">
+    <row r="164" spans="1:22" ht="15">
       <c r="A164" s="26" t="s">
         <v>170</v>
       </c>
@@ -6568,7 +6597,7 @@
       <c r="U164" s="2"/>
       <c r="V164" s="2"/>
     </row>
-    <row r="165" spans="1:22" ht="14.4">
+    <row r="165" spans="1:22" ht="15">
       <c r="A165" s="26" t="s">
         <v>171</v>
       </c>
@@ -6598,7 +6627,7 @@
       <c r="U165" s="2"/>
       <c r="V165" s="2"/>
     </row>
-    <row r="166" spans="1:22" ht="14.4">
+    <row r="166" spans="1:22" ht="15">
       <c r="A166" s="26" t="s">
         <v>172</v>
       </c>
@@ -6628,7 +6657,7 @@
       <c r="U166" s="2"/>
       <c r="V166" s="2"/>
     </row>
-    <row r="167" spans="1:22" ht="14.4">
+    <row r="167" spans="1:22" ht="15">
       <c r="A167" s="26" t="s">
         <v>173</v>
       </c>
@@ -6658,7 +6687,7 @@
       <c r="U167" s="2"/>
       <c r="V167" s="2"/>
     </row>
-    <row r="168" spans="1:22" ht="14.4">
+    <row r="168" spans="1:22" ht="15">
       <c r="A168" s="26" t="s">
         <v>174</v>
       </c>
@@ -6688,7 +6717,7 @@
       <c r="U168" s="2"/>
       <c r="V168" s="2"/>
     </row>
-    <row r="169" spans="1:22" ht="14.4">
+    <row r="169" spans="1:22" ht="15">
       <c r="A169" s="26" t="s">
         <v>175</v>
       </c>
@@ -6718,7 +6747,7 @@
       <c r="U169" s="2"/>
       <c r="V169" s="2"/>
     </row>
-    <row r="170" spans="1:22" ht="14.4">
+    <row r="170" spans="1:22" ht="15">
       <c r="A170" s="26" t="s">
         <v>176</v>
       </c>
@@ -6748,7 +6777,7 @@
       <c r="U170" s="2"/>
       <c r="V170" s="2"/>
     </row>
-    <row r="171" spans="1:22" ht="14.4">
+    <row r="171" spans="1:22" ht="15">
       <c r="A171" s="26" t="s">
         <v>177</v>
       </c>
@@ -6778,7 +6807,7 @@
       <c r="U171" s="2"/>
       <c r="V171" s="2"/>
     </row>
-    <row r="172" spans="1:22" ht="14.4">
+    <row r="172" spans="1:22" ht="15">
       <c r="A172" s="26" t="s">
         <v>178</v>
       </c>
@@ -6808,7 +6837,7 @@
       <c r="U172" s="2"/>
       <c r="V172" s="2"/>
     </row>
-    <row r="173" spans="1:22" ht="14.4">
+    <row r="173" spans="1:22" ht="15">
       <c r="A173" s="26" t="s">
         <v>179</v>
       </c>
@@ -6838,7 +6867,7 @@
       <c r="U173" s="2"/>
       <c r="V173" s="2"/>
     </row>
-    <row r="174" spans="1:22" ht="14.4">
+    <row r="174" spans="1:22" ht="15">
       <c r="A174" s="26" t="s">
         <v>180</v>
       </c>
@@ -6868,7 +6897,7 @@
       <c r="U174" s="2"/>
       <c r="V174" s="2"/>
     </row>
-    <row r="175" spans="1:22" ht="14.4">
+    <row r="175" spans="1:22" ht="15">
       <c r="A175" s="26" t="s">
         <v>181</v>
       </c>
@@ -6898,7 +6927,7 @@
       <c r="U175" s="2"/>
       <c r="V175" s="2"/>
     </row>
-    <row r="176" spans="1:22" ht="14.4">
+    <row r="176" spans="1:22" ht="15">
       <c r="A176" s="26" t="s">
         <v>182</v>
       </c>
@@ -6928,7 +6957,7 @@
       <c r="U176" s="2"/>
       <c r="V176" s="2"/>
     </row>
-    <row r="177" spans="1:22" ht="14.4">
+    <row r="177" spans="1:22" ht="15">
       <c r="A177" s="26" t="s">
         <v>183</v>
       </c>
@@ -6958,7 +6987,7 @@
       <c r="U177" s="2"/>
       <c r="V177" s="2"/>
     </row>
-    <row r="178" spans="1:22" ht="14.4">
+    <row r="178" spans="1:22" ht="15">
       <c r="A178" s="26" t="s">
         <v>184</v>
       </c>
@@ -6988,7 +7017,7 @@
       <c r="U178" s="2"/>
       <c r="V178" s="2"/>
     </row>
-    <row r="179" spans="1:22" ht="14.4">
+    <row r="179" spans="1:22" ht="15">
       <c r="A179" s="26" t="s">
         <v>185</v>
       </c>
@@ -7018,7 +7047,7 @@
       <c r="U179" s="2"/>
       <c r="V179" s="2"/>
     </row>
-    <row r="180" spans="1:22" ht="14.4">
+    <row r="180" spans="1:22" ht="15">
       <c r="A180" s="26" t="s">
         <v>186</v>
       </c>
@@ -7048,7 +7077,7 @@
       <c r="U180" s="2"/>
       <c r="V180" s="2"/>
     </row>
-    <row r="181" spans="1:22" ht="14.4">
+    <row r="181" spans="1:22" ht="15">
       <c r="A181" s="26" t="s">
         <v>187</v>
       </c>
@@ -7078,7 +7107,7 @@
       <c r="U181" s="2"/>
       <c r="V181" s="2"/>
     </row>
-    <row r="182" spans="1:22" ht="14.4">
+    <row r="182" spans="1:22" ht="15">
       <c r="A182" s="26" t="s">
         <v>188</v>
       </c>
@@ -7108,7 +7137,7 @@
       <c r="U182" s="2"/>
       <c r="V182" s="2"/>
     </row>
-    <row r="183" spans="1:22" ht="14.4">
+    <row r="183" spans="1:22" ht="15">
       <c r="A183" s="26" t="s">
         <v>189</v>
       </c>
@@ -7138,7 +7167,7 @@
       <c r="U183" s="2"/>
       <c r="V183" s="2"/>
     </row>
-    <row r="184" spans="1:22" ht="15" thickBot="1">
+    <row r="184" spans="1:22" thickBot="1">
       <c r="A184" s="26" t="s">
         <v>190</v>
       </c>
@@ -7168,7 +7197,7 @@
       <c r="U184" s="2"/>
       <c r="V184" s="2"/>
     </row>
-    <row r="185" spans="1:22" ht="15.6" thickBot="1">
+    <row r="185" spans="1:22" thickBot="1">
       <c r="A185" s="29" t="s">
         <v>191</v>
       </c>
@@ -7204,7 +7233,7 @@
       <c r="U185" s="2"/>
       <c r="V185" s="2"/>
     </row>
-    <row r="186" spans="1:22" ht="15.6" thickBot="1">
+    <row r="186" spans="1:22" thickBot="1">
       <c r="A186" s="29" t="s">
         <v>192</v>
       </c>
@@ -7242,7 +7271,7 @@
       <c r="U186" s="2"/>
       <c r="V186" s="2"/>
     </row>
-    <row r="187" spans="1:22" ht="15.6" thickBot="1">
+    <row r="187" spans="1:22" thickBot="1">
       <c r="A187" s="29" t="s">
         <v>193</v>
       </c>
@@ -7280,7 +7309,7 @@
       <c r="U187" s="2"/>
       <c r="V187" s="2"/>
     </row>
-    <row r="188" spans="1:22" ht="15.6" thickBot="1">
+    <row r="188" spans="1:22" thickBot="1">
       <c r="A188" s="29" t="s">
         <v>194</v>
       </c>
@@ -7318,7 +7347,7 @@
       <c r="U188" s="2"/>
       <c r="V188" s="2"/>
     </row>
-    <row r="189" spans="1:22" ht="15.6" thickBot="1">
+    <row r="189" spans="1:22" thickBot="1">
       <c r="A189" s="29" t="s">
         <v>195</v>
       </c>
@@ -7394,7 +7423,7 @@
       <c r="U190" s="2"/>
       <c r="V190" s="2"/>
     </row>
-    <row r="191" spans="1:22" ht="14.4">
+    <row r="191" spans="1:22" ht="15">
       <c r="A191" s="29" t="s">
         <v>197</v>
       </c>
@@ -7424,7 +7453,7 @@
       <c r="U191" s="2"/>
       <c r="V191" s="2"/>
     </row>
-    <row r="192" spans="1:22" ht="14.4">
+    <row r="192" spans="1:22" ht="15">
       <c r="A192" s="29" t="s">
         <v>198</v>
       </c>
@@ -7462,7 +7491,7 @@
       <c r="U192" s="2"/>
       <c r="V192" s="2"/>
     </row>
-    <row r="193" spans="1:22" ht="14.4">
+    <row r="193" spans="1:22" ht="15">
       <c r="A193" s="29" t="s">
         <v>199</v>
       </c>
@@ -7500,7 +7529,7 @@
       <c r="U193" s="2"/>
       <c r="V193" s="2"/>
     </row>
-    <row r="194" spans="1:22" ht="14.4">
+    <row r="194" spans="1:22" ht="15">
       <c r="A194" s="29" t="s">
         <v>200</v>
       </c>
@@ -7536,7 +7565,7 @@
       <c r="U194" s="2"/>
       <c r="V194" s="2"/>
     </row>
-    <row r="195" spans="1:22" ht="14.4">
+    <row r="195" spans="1:22" ht="15">
       <c r="A195" s="29" t="s">
         <v>201</v>
       </c>
@@ -7574,7 +7603,7 @@
       <c r="U195" s="2"/>
       <c r="V195" s="2"/>
     </row>
-    <row r="196" spans="1:22" ht="14.4">
+    <row r="196" spans="1:22" ht="15">
       <c r="A196" s="29" t="s">
         <v>202</v>
       </c>
@@ -7612,7 +7641,7 @@
       <c r="U196" s="2"/>
       <c r="V196" s="2"/>
     </row>
-    <row r="197" spans="1:22" ht="14.4">
+    <row r="197" spans="1:22" ht="15">
       <c r="A197" s="29" t="s">
         <v>203</v>
       </c>
@@ -7650,7 +7679,7 @@
       <c r="U197" s="2"/>
       <c r="V197" s="2"/>
     </row>
-    <row r="198" spans="1:22" ht="14.4">
+    <row r="198" spans="1:22" ht="15">
       <c r="A198" s="26" t="s">
         <v>204</v>
       </c>
@@ -7688,7 +7717,7 @@
       <c r="U198" s="2"/>
       <c r="V198" s="2"/>
     </row>
-    <row r="199" spans="1:22" ht="14.4">
+    <row r="199" spans="1:22" ht="15">
       <c r="A199" s="29" t="s">
         <v>205</v>
       </c>
@@ -7764,7 +7793,7 @@
       <c r="U200" s="2"/>
       <c r="V200" s="2"/>
     </row>
-    <row r="201" spans="1:22" ht="14.4">
+    <row r="201" spans="1:22" ht="15">
       <c r="A201" s="29" t="s">
         <v>207</v>
       </c>
@@ -7794,7 +7823,7 @@
       <c r="U201" s="2"/>
       <c r="V201" s="2"/>
     </row>
-    <row r="202" spans="1:22" ht="14.4">
+    <row r="202" spans="1:22" ht="15">
       <c r="A202" s="29" t="s">
         <v>208</v>
       </c>
@@ -7824,7 +7853,7 @@
       <c r="U202" s="2"/>
       <c r="V202" s="2"/>
     </row>
-    <row r="203" spans="1:22" ht="14.4">
+    <row r="203" spans="1:22" ht="15">
       <c r="A203" s="29" t="s">
         <v>209</v>
       </c>
@@ -7862,7 +7891,7 @@
       <c r="U203" s="2"/>
       <c r="V203" s="2"/>
     </row>
-    <row r="204" spans="1:22" ht="14.4">
+    <row r="204" spans="1:22" ht="15">
       <c r="A204" s="29" t="s">
         <v>210</v>
       </c>
@@ -7900,7 +7929,7 @@
       <c r="U204" s="2"/>
       <c r="V204" s="2"/>
     </row>
-    <row r="205" spans="1:22" ht="15" thickBot="1">
+    <row r="205" spans="1:22" thickBot="1">
       <c r="A205" s="29" t="s">
         <v>211</v>
       </c>
@@ -7976,7 +8005,7 @@
       <c r="U206" s="2"/>
       <c r="V206" s="2"/>
     </row>
-    <row r="207" spans="1:22" ht="14.4">
+    <row r="207" spans="1:22" ht="15">
       <c r="A207" s="29" t="s">
         <v>213</v>
       </c>
@@ -8012,7 +8041,7 @@
       <c r="U207" s="2"/>
       <c r="V207" s="2"/>
     </row>
-    <row r="208" spans="1:22" ht="15" thickBot="1">
+    <row r="208" spans="1:22" thickBot="1">
       <c r="A208" s="29" t="s">
         <v>214</v>
       </c>
@@ -8042,7 +8071,7 @@
       <c r="U208" s="2"/>
       <c r="V208" s="2"/>
     </row>
-    <row r="209" spans="1:22" ht="15.6" thickBot="1">
+    <row r="209" spans="1:22" thickBot="1">
       <c r="A209" s="29" t="s">
         <v>215</v>
       </c>
@@ -8118,7 +8147,7 @@
       <c r="U210" s="2"/>
       <c r="V210" s="2"/>
     </row>
-    <row r="211" spans="1:22" ht="14.4">
+    <row r="211" spans="1:22" ht="15">
       <c r="A211" s="29" t="s">
         <v>217</v>
       </c>
@@ -8156,7 +8185,7 @@
       <c r="U211" s="2"/>
       <c r="V211" s="2"/>
     </row>
-    <row r="212" spans="1:22" ht="15" thickBot="1">
+    <row r="212" spans="1:22" thickBot="1">
       <c r="A212" s="29" t="s">
         <v>218</v>
       </c>
@@ -8224,7 +8253,7 @@
       <c r="U213" s="2"/>
       <c r="V213" s="2"/>
     </row>
-    <row r="214" spans="1:22" ht="14.4">
+    <row r="214" spans="1:22" ht="15">
       <c r="A214" s="29" t="s">
         <v>220</v>
       </c>
@@ -8276,7 +8305,7 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sigo editando mi archivo excel GRUPAL :)
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelly\Desktop\pc2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUAN CARLOS DIAZ\Desktop\pc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CBBFD7-7210-47B4-8D76-A7EFD4CA4E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9012" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="C1" sheetId="2" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="301">
   <si>
     <t>Localización</t>
   </si>
@@ -878,13 +877,58 @@
   </si>
   <si>
     <t>x7</t>
+  </si>
+  <si>
+    <t>terminado</t>
+  </si>
+  <si>
+    <t>ATP Binding Cassette Subfamily C Member 5</t>
+  </si>
+  <si>
+    <t>25,22</t>
+  </si>
+  <si>
+    <t>Presenilin Associated Rhomboid Like</t>
+  </si>
+  <si>
+    <t>51,64</t>
+  </si>
+  <si>
+    <t>MAP6 Domain Containing 1</t>
+  </si>
+  <si>
+    <t>YEATS Domain Containing 2</t>
+  </si>
+  <si>
+    <t>Kelch Like Family Member 24</t>
+  </si>
+  <si>
+    <t>28,40</t>
+  </si>
+  <si>
+    <t>27,17</t>
+  </si>
+  <si>
+    <t>10,8</t>
+  </si>
+  <si>
+    <t>Kelch Like Family Member 6</t>
+  </si>
+  <si>
+    <t>9,9</t>
+  </si>
+  <si>
+    <t>MCF.2 Cell Line Derived Transforming Sequence-Like 2</t>
+  </si>
+  <si>
+    <t>4,3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -894,31 +938,26 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -929,19 +968,16 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF444444"/>
       <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -973,8 +1009,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1020,12 +1074,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1103,7 +1151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1136,9 +1184,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1175,8 +1220,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1185,8 +1228,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1221,13 +1273,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Elipse 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Elipse 2"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1269,66 +1315,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2133600</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Triángulo isósceles 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3093720" y="2217420"/>
-          <a:ext cx="457200" cy="464820"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>1249680</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
@@ -1341,13 +1327,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1385,6 +1365,168 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1173480</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1615440</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Elipse 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2133600" y="2255520"/>
+          <a:ext cx="441960" cy="396240"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2232660</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Elipse 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3192780" y="2286000"/>
+          <a:ext cx="441960" cy="396240"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1564949</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28459</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2082899</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>144069</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Acorde 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="18150062">
+          <a:off x="2451919" y="3256289"/>
+          <a:ext cx="664250" cy="517950"/>
+        </a:xfrm>
+        <a:prstGeom prst="chord">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1590,40 +1732,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:V216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="43" t="s">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -1641,24 +1783,24 @@
       <c r="E2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15">
+    <row r="3" spans="1:22" ht="14.4">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="37" t="s">
         <v>279</v>
       </c>
       <c r="D3" s="5">
@@ -1667,9 +1809,9 @@
       <c r="E3" s="5">
         <v>32091761</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1685,14 +1827,14 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="15">
+    <row r="4" spans="1:22" ht="14.4">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>280</v>
       </c>
       <c r="D4" s="5">
@@ -1701,9 +1843,9 @@
       <c r="E4" s="5">
         <v>32838076</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1719,14 +1861,14 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" ht="15">
+    <row r="5" spans="1:22" ht="14.4">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="37" t="s">
         <v>281</v>
       </c>
       <c r="D5" s="5">
@@ -1735,9 +1877,9 @@
       <c r="E5" s="5">
         <v>33090132</v>
       </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1753,14 +1895,14 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="15">
+    <row r="6" spans="1:22" ht="14.4">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="37" t="s">
         <v>282</v>
       </c>
       <c r="D6" s="5">
@@ -1769,9 +1911,9 @@
       <c r="E6" s="5">
         <v>33768221</v>
       </c>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1787,14 +1929,14 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="15">
+    <row r="7" spans="1:22" ht="14.4">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="37" t="s">
         <v>283</v>
       </c>
       <c r="D7" s="5">
@@ -1803,9 +1945,9 @@
       <c r="E7" s="5">
         <v>33811741</v>
       </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1821,14 +1963,14 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="15">
+    <row r="8" spans="1:22" ht="14.4">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>284</v>
       </c>
       <c r="D8" s="5">
@@ -1837,9 +1979,9 @@
       <c r="E8" s="5">
         <v>33934641</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1855,14 +1997,14 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="15">
+    <row r="9" spans="1:22" ht="14.4">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="37" t="s">
         <v>285</v>
       </c>
       <c r="D9" s="5">
@@ -1890,10 +2032,10 @@
       <c r="V9" s="2"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="13"/>
       <c r="D10" s="5">
         <v>34235896</v>
@@ -1901,10 +2043,8 @@
       <c r="E10" s="5">
         <v>34251973</v>
       </c>
-      <c r="F10" s="41">
-        <v>2</v>
-      </c>
-      <c r="G10" s="41"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1921,11 +2061,11 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="15">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:22" ht="14.4">
+      <c r="A11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="36"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="13"/>
       <c r="D11" s="5">
         <v>34811253</v>
@@ -1933,8 +2073,8 @@
       <c r="E11" s="5">
         <v>34812505</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1951,11 +2091,11 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="15">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:22" ht="14.4">
+      <c r="A12" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="36"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="12"/>
       <c r="D12" s="5">
         <v>34826096</v>
@@ -1963,8 +2103,8 @@
       <c r="E12" s="5">
         <v>34855603</v>
       </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1981,11 +2121,11 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="15">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:22" ht="14.4">
+      <c r="A13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="14"/>
       <c r="D13" s="5">
         <v>34857740</v>
@@ -1993,8 +2133,8 @@
       <c r="E13" s="5">
         <v>34864667</v>
       </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -2011,11 +2151,11 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="15">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:22" ht="14.4">
+      <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="36"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="13"/>
       <c r="D14" s="5">
         <v>34864860</v>
@@ -2023,8 +2163,8 @@
       <c r="E14" s="5">
         <v>34953982</v>
       </c>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -2041,11 +2181,11 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="15">
-      <c r="A15" s="26" t="s">
+    <row r="15" spans="1:22" ht="14.4">
+      <c r="A15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="14"/>
       <c r="D15" s="5">
         <v>34960381</v>
@@ -2053,8 +2193,8 @@
       <c r="E15" s="5">
         <v>34968544</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -2071,11 +2211,11 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="15">
-      <c r="A16" s="26" t="s">
+    <row r="16" spans="1:22" ht="14.4">
+      <c r="A16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="36"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="13"/>
       <c r="D16" s="5">
         <v>34994565</v>
@@ -2083,8 +2223,8 @@
       <c r="E16" s="5">
         <v>34996018</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -2101,8 +2241,8 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" ht="15">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:22" ht="14.4">
+      <c r="A17" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B17" s="11"/>
@@ -2131,8 +2271,8 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22" ht="15">
-      <c r="A18" s="26" t="s">
+    <row r="18" spans="1:22" ht="14.4">
+      <c r="A18" s="25" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="4"/>
@@ -2143,8 +2283,8 @@
       <c r="E18" s="5">
         <v>69418230</v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -2161,8 +2301,8 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" ht="15">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:22" ht="14.4">
+      <c r="A19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="11"/>
@@ -2173,8 +2313,8 @@
       <c r="E19" s="5">
         <v>69586809</v>
       </c>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -2191,8 +2331,8 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" ht="15">
-      <c r="A20" s="26" t="s">
+    <row r="20" spans="1:22" ht="14.4">
+      <c r="A20" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="11"/>
@@ -2203,8 +2343,8 @@
       <c r="E20" s="5">
         <v>69708647</v>
       </c>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -2221,8 +2361,8 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="1:22" ht="15">
-      <c r="A21" s="26" t="s">
+    <row r="21" spans="1:22" ht="14.4">
+      <c r="A21" s="25" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="11"/>
@@ -2233,8 +2373,8 @@
       <c r="E21" s="5">
         <v>69826032</v>
       </c>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -2251,8 +2391,8 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:22" ht="15">
-      <c r="A22" s="26" t="s">
+    <row r="22" spans="1:22" ht="14.4">
+      <c r="A22" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="11"/>
@@ -2263,8 +2403,8 @@
       <c r="E22" s="5">
         <v>69933388</v>
       </c>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2281,8 +2421,8 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="1:22" ht="15">
-      <c r="A23" s="26" t="s">
+    <row r="23" spans="1:22" ht="14.4">
+      <c r="A23" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="16"/>
@@ -2293,8 +2433,8 @@
       <c r="E23" s="5">
         <v>69941662</v>
       </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2311,8 +2451,8 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22" ht="15">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:22" ht="14.4">
+      <c r="A24" s="25" t="s">
         <v>31</v>
       </c>
       <c r="B24" s="16"/>
@@ -2323,8 +2463,8 @@
       <c r="E24" s="5">
         <v>69990604</v>
       </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2341,8 +2481,8 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22" ht="15">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:22" ht="14.4">
+      <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="16"/>
@@ -2353,8 +2493,8 @@
       <c r="E25" s="5">
         <v>70101362</v>
       </c>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2371,8 +2511,8 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:22" ht="15">
-      <c r="A26" s="26" t="s">
+    <row r="26" spans="1:22" ht="14.4">
+      <c r="A26" s="25" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="16"/>
@@ -2383,8 +2523,8 @@
       <c r="E26" s="5">
         <v>70139011</v>
       </c>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2401,8 +2541,8 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:22" ht="15">
-      <c r="A27" s="26" t="s">
+    <row r="27" spans="1:22" ht="14.4">
+      <c r="A27" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="16"/>
@@ -2413,8 +2553,8 @@
       <c r="E27" s="5">
         <v>70202391</v>
       </c>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2431,8 +2571,8 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:22" ht="15">
-      <c r="A28" s="26" t="s">
+    <row r="28" spans="1:22" ht="14.4">
+      <c r="A28" s="25" t="s">
         <v>35</v>
       </c>
       <c r="B28" s="16"/>
@@ -2443,8 +2583,8 @@
       <c r="E28" s="5">
         <v>70241268</v>
       </c>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2461,8 +2601,8 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:22" ht="15">
-      <c r="A29" s="26" t="s">
+    <row r="29" spans="1:22" ht="14.4">
+      <c r="A29" s="25" t="s">
         <v>36</v>
       </c>
       <c r="B29" s="16"/>
@@ -2491,8 +2631,8 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="1:22" ht="15">
-      <c r="A30" s="26" t="s">
+    <row r="30" spans="1:22" ht="14.4">
+      <c r="A30" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B30" s="16"/>
@@ -2521,8 +2661,8 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:22" ht="15">
-      <c r="A31" s="26" t="s">
+    <row r="31" spans="1:22" ht="14.4">
+      <c r="A31" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B31" s="16"/>
@@ -2551,8 +2691,8 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:22" ht="15">
-      <c r="A32" s="26" t="s">
+    <row r="32" spans="1:22" ht="14.4">
+      <c r="A32" s="25" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="16"/>
@@ -2581,8 +2721,8 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:22" ht="15">
-      <c r="A33" s="26" t="s">
+    <row r="33" spans="1:22" ht="14.4">
+      <c r="A33" s="25" t="s">
         <v>40</v>
       </c>
       <c r="B33" s="16"/>
@@ -2611,8 +2751,8 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:22" ht="15">
-      <c r="A34" s="26" t="s">
+    <row r="34" spans="1:22" ht="14.4">
+      <c r="A34" s="25" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="16"/>
@@ -2641,8 +2781,8 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="1:22" ht="15">
-      <c r="A35" s="26" t="s">
+    <row r="35" spans="1:22" ht="14.4">
+      <c r="A35" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="11"/>
@@ -2671,8 +2811,8 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:22" ht="15">
-      <c r="A36" s="26" t="s">
+    <row r="36" spans="1:22" ht="14.4">
+      <c r="A36" s="25" t="s">
         <v>43</v>
       </c>
       <c r="B36" s="16"/>
@@ -2701,8 +2841,8 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="1:22" ht="15">
-      <c r="A37" s="26" t="s">
+    <row r="37" spans="1:22" ht="14.4">
+      <c r="A37" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="16"/>
@@ -2731,8 +2871,8 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
     </row>
-    <row r="38" spans="1:22" ht="15">
-      <c r="A38" s="26" t="s">
+    <row r="38" spans="1:22" ht="14.4">
+      <c r="A38" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="11"/>
@@ -2761,8 +2901,8 @@
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
     </row>
-    <row r="39" spans="1:22" ht="15">
-      <c r="A39" s="26" t="s">
+    <row r="39" spans="1:22" ht="14.4">
+      <c r="A39" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11"/>
@@ -2791,8 +2931,8 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" ht="15">
-      <c r="A40" s="26" t="s">
+    <row r="40" spans="1:22" ht="14.4">
+      <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B40" s="16"/>
@@ -2821,8 +2961,8 @@
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:22" ht="15">
-      <c r="A41" s="26" t="s">
+    <row r="41" spans="1:22" ht="14.4">
+      <c r="A41" s="25" t="s">
         <v>48</v>
       </c>
       <c r="B41" s="16"/>
@@ -2851,8 +2991,8 @@
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:22" ht="15">
-      <c r="A42" s="26" t="s">
+    <row r="42" spans="1:22" ht="14.4">
+      <c r="A42" s="25" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="16"/>
@@ -2881,8 +3021,8 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:22" ht="15">
-      <c r="A43" s="26" t="s">
+    <row r="43" spans="1:22" ht="14.4">
+      <c r="A43" s="25" t="s">
         <v>50</v>
       </c>
       <c r="B43" s="16"/>
@@ -2911,8 +3051,8 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:22" ht="15">
-      <c r="A44" s="26" t="s">
+    <row r="44" spans="1:22" ht="14.4">
+      <c r="A44" s="25" t="s">
         <v>51</v>
       </c>
       <c r="B44" s="11"/>
@@ -2941,8 +3081,8 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:22" ht="15">
-      <c r="A45" s="26" t="s">
+    <row r="45" spans="1:22" ht="14.4">
+      <c r="A45" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="16"/>
@@ -2971,8 +3111,8 @@
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="1:22" ht="15">
-      <c r="A46" s="26" t="s">
+    <row r="46" spans="1:22" ht="14.4">
+      <c r="A46" s="25" t="s">
         <v>53</v>
       </c>
       <c r="B46" s="16"/>
@@ -3001,8 +3141,8 @@
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="1:22" ht="15">
-      <c r="A47" s="26" t="s">
+    <row r="47" spans="1:22" ht="14.4">
+      <c r="A47" s="25" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="16"/>
@@ -3031,8 +3171,8 @@
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="1:22" ht="15">
-      <c r="A48" s="26" t="s">
+    <row r="48" spans="1:22" ht="14.4">
+      <c r="A48" s="25" t="s">
         <v>55</v>
       </c>
       <c r="B48" s="16"/>
@@ -3061,8 +3201,8 @@
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
     </row>
-    <row r="49" spans="1:22" ht="15">
-      <c r="A49" s="26" t="s">
+    <row r="49" spans="1:22" ht="14.4">
+      <c r="A49" s="25" t="s">
         <v>56</v>
       </c>
       <c r="B49" s="11"/>
@@ -3091,8 +3231,8 @@
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
     </row>
-    <row r="50" spans="1:22" ht="15">
-      <c r="A50" s="26" t="s">
+    <row r="50" spans="1:22" ht="14.4">
+      <c r="A50" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="16"/>
@@ -3121,8 +3261,8 @@
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
     </row>
-    <row r="51" spans="1:22" ht="15">
-      <c r="A51" s="26" t="s">
+    <row r="51" spans="1:22" ht="14.4">
+      <c r="A51" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B51" s="16"/>
@@ -3151,8 +3291,8 @@
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
     </row>
-    <row r="52" spans="1:22" ht="15">
-      <c r="A52" s="26" t="s">
+    <row r="52" spans="1:22" ht="14.4">
+      <c r="A52" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B52" s="16"/>
@@ -3181,8 +3321,8 @@
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
     </row>
-    <row r="53" spans="1:22" ht="15">
-      <c r="A53" s="26" t="s">
+    <row r="53" spans="1:22" ht="14.4">
+      <c r="A53" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B53" s="11"/>
@@ -3211,8 +3351,8 @@
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
     </row>
-    <row r="54" spans="1:22" ht="15">
-      <c r="A54" s="26" t="s">
+    <row r="54" spans="1:22" ht="14.4">
+      <c r="A54" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B54" s="16"/>
@@ -3241,8 +3381,8 @@
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
     </row>
-    <row r="55" spans="1:22" ht="15">
-      <c r="A55" s="26" t="s">
+    <row r="55" spans="1:22" ht="14.4">
+      <c r="A55" s="25" t="s">
         <v>62</v>
       </c>
       <c r="B55" s="16"/>
@@ -3271,8 +3411,8 @@
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
     </row>
-    <row r="56" spans="1:22" ht="15">
-      <c r="A56" s="26" t="s">
+    <row r="56" spans="1:22" ht="14.4">
+      <c r="A56" s="25" t="s">
         <v>63</v>
       </c>
       <c r="B56" s="16"/>
@@ -3301,8 +3441,8 @@
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
     </row>
-    <row r="57" spans="1:22" ht="15">
-      <c r="A57" s="26" t="s">
+    <row r="57" spans="1:22" ht="14.4">
+      <c r="A57" s="25" t="s">
         <v>64</v>
       </c>
       <c r="B57" s="16"/>
@@ -3331,8 +3471,8 @@
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
     </row>
-    <row r="58" spans="1:22" ht="15">
-      <c r="A58" s="26" t="s">
+    <row r="58" spans="1:22" ht="14.4">
+      <c r="A58" s="25" t="s">
         <v>65</v>
       </c>
       <c r="B58" s="11"/>
@@ -3361,8 +3501,8 @@
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
     </row>
-    <row r="59" spans="1:22" ht="15">
-      <c r="A59" s="26" t="s">
+    <row r="59" spans="1:22" ht="14.4">
+      <c r="A59" s="25" t="s">
         <v>66</v>
       </c>
       <c r="B59" s="16"/>
@@ -3391,8 +3531,8 @@
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
     </row>
-    <row r="60" spans="1:22" ht="15">
-      <c r="A60" s="26" t="s">
+    <row r="60" spans="1:22" ht="14.4">
+      <c r="A60" s="25" t="s">
         <v>67</v>
       </c>
       <c r="B60" s="16"/>
@@ -3421,8 +3561,8 @@
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
     </row>
-    <row r="61" spans="1:22" ht="15">
-      <c r="A61" s="26" t="s">
+    <row r="61" spans="1:22" ht="14.4">
+      <c r="A61" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B61" s="11"/>
@@ -3451,8 +3591,8 @@
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
     </row>
-    <row r="62" spans="1:22" ht="15">
-      <c r="A62" s="26" t="s">
+    <row r="62" spans="1:22" ht="14.4">
+      <c r="A62" s="25" t="s">
         <v>69</v>
       </c>
       <c r="B62" s="16"/>
@@ -3481,8 +3621,8 @@
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
     </row>
-    <row r="63" spans="1:22" ht="15">
-      <c r="A63" s="26" t="s">
+    <row r="63" spans="1:22" ht="14.4">
+      <c r="A63" s="25" t="s">
         <v>70</v>
       </c>
       <c r="B63" s="11"/>
@@ -3511,8 +3651,8 @@
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
     </row>
-    <row r="64" spans="1:22" ht="15">
-      <c r="A64" s="26" t="s">
+    <row r="64" spans="1:22" ht="14.4">
+      <c r="A64" s="25" t="s">
         <v>71</v>
       </c>
       <c r="B64" s="16"/>
@@ -3541,8 +3681,8 @@
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
     </row>
-    <row r="65" spans="1:22" ht="15">
-      <c r="A65" s="26" t="s">
+    <row r="65" spans="1:22" ht="14.4">
+      <c r="A65" s="25" t="s">
         <v>72</v>
       </c>
       <c r="B65" s="16"/>
@@ -3571,8 +3711,8 @@
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
     </row>
-    <row r="66" spans="1:22" ht="15">
-      <c r="A66" s="26" t="s">
+    <row r="66" spans="1:22" ht="14.4">
+      <c r="A66" s="25" t="s">
         <v>73</v>
       </c>
       <c r="B66" s="16"/>
@@ -3601,8 +3741,8 @@
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
     </row>
-    <row r="67" spans="1:22" ht="15">
-      <c r="A67" s="26" t="s">
+    <row r="67" spans="1:22" ht="14.4">
+      <c r="A67" s="25" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="16"/>
@@ -3631,8 +3771,8 @@
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
     </row>
-    <row r="68" spans="1:22" ht="15">
-      <c r="A68" s="26" t="s">
+    <row r="68" spans="1:22" ht="14.4">
+      <c r="A68" s="25" t="s">
         <v>75</v>
       </c>
       <c r="B68" s="16"/>
@@ -3661,8 +3801,8 @@
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
     </row>
-    <row r="69" spans="1:22" ht="15">
-      <c r="A69" s="26" t="s">
+    <row r="69" spans="1:22" ht="14.4">
+      <c r="A69" s="25" t="s">
         <v>76</v>
       </c>
       <c r="B69" s="16"/>
@@ -3691,8 +3831,8 @@
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
     </row>
-    <row r="70" spans="1:22" ht="15">
-      <c r="A70" s="26" t="s">
+    <row r="70" spans="1:22" ht="14.4">
+      <c r="A70" s="25" t="s">
         <v>77</v>
       </c>
       <c r="B70" s="16"/>
@@ -3721,8 +3861,8 @@
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
     </row>
-    <row r="71" spans="1:22" ht="15">
-      <c r="A71" s="26" t="s">
+    <row r="71" spans="1:22" ht="14.4">
+      <c r="A71" s="25" t="s">
         <v>78</v>
       </c>
       <c r="B71" s="16"/>
@@ -3751,8 +3891,8 @@
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
     </row>
-    <row r="72" spans="1:22" ht="15">
-      <c r="A72" s="26" t="s">
+    <row r="72" spans="1:22" ht="14.4">
+      <c r="A72" s="25" t="s">
         <v>79</v>
       </c>
       <c r="B72" s="4"/>
@@ -3781,8 +3921,8 @@
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
     </row>
-    <row r="73" spans="1:22" ht="15">
-      <c r="A73" s="26" t="s">
+    <row r="73" spans="1:22" ht="14.4">
+      <c r="A73" s="25" t="s">
         <v>80</v>
       </c>
       <c r="B73" s="16"/>
@@ -3811,8 +3951,8 @@
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
     </row>
-    <row r="74" spans="1:22" ht="15">
-      <c r="A74" s="26" t="s">
+    <row r="74" spans="1:22" ht="14.4">
+      <c r="A74" s="25" t="s">
         <v>81</v>
       </c>
       <c r="B74" s="16"/>
@@ -3841,8 +3981,8 @@
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
     </row>
-    <row r="75" spans="1:22" ht="15">
-      <c r="A75" s="26" t="s">
+    <row r="75" spans="1:22" ht="14.4">
+      <c r="A75" s="25" t="s">
         <v>82</v>
       </c>
       <c r="B75" s="16"/>
@@ -3871,8 +4011,8 @@
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
     </row>
-    <row r="76" spans="1:22" ht="15">
-      <c r="A76" s="26" t="s">
+    <row r="76" spans="1:22" ht="14.4">
+      <c r="A76" s="25" t="s">
         <v>83</v>
       </c>
       <c r="B76" s="16"/>
@@ -3901,8 +4041,8 @@
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
     </row>
-    <row r="77" spans="1:22" ht="15">
-      <c r="A77" s="26" t="s">
+    <row r="77" spans="1:22" ht="14.4">
+      <c r="A77" s="25" t="s">
         <v>84</v>
       </c>
       <c r="B77" s="16"/>
@@ -3931,8 +4071,8 @@
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
     </row>
-    <row r="78" spans="1:22" ht="15">
-      <c r="A78" s="26" t="s">
+    <row r="78" spans="1:22" ht="14.4">
+      <c r="A78" s="25" t="s">
         <v>85</v>
       </c>
       <c r="B78" s="4"/>
@@ -3961,8 +4101,8 @@
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
     </row>
-    <row r="79" spans="1:22" ht="15">
-      <c r="A79" s="26" t="s">
+    <row r="79" spans="1:22" ht="14.4">
+      <c r="A79" s="25" t="s">
         <v>86</v>
       </c>
       <c r="B79" s="4"/>
@@ -3991,8 +4131,8 @@
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
     </row>
-    <row r="80" spans="1:22" ht="15">
-      <c r="A80" s="26" t="s">
+    <row r="80" spans="1:22" ht="14.4">
+      <c r="A80" s="25" t="s">
         <v>87</v>
       </c>
       <c r="B80" s="4"/>
@@ -4021,8 +4161,8 @@
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
     </row>
-    <row r="81" spans="1:22" ht="15">
-      <c r="A81" s="26" t="s">
+    <row r="81" spans="1:22" ht="14.4">
+      <c r="A81" s="25" t="s">
         <v>88</v>
       </c>
       <c r="B81" s="16"/>
@@ -4051,8 +4191,8 @@
       <c r="U81" s="2"/>
       <c r="V81" s="2"/>
     </row>
-    <row r="82" spans="1:22" ht="15">
-      <c r="A82" s="26" t="s">
+    <row r="82" spans="1:22" ht="14.4">
+      <c r="A82" s="25" t="s">
         <v>89</v>
       </c>
       <c r="B82" s="16"/>
@@ -4081,8 +4221,8 @@
       <c r="U82" s="2"/>
       <c r="V82" s="2"/>
     </row>
-    <row r="83" spans="1:22" ht="15">
-      <c r="A83" s="26" t="s">
+    <row r="83" spans="1:22" ht="14.4">
+      <c r="A83" s="25" t="s">
         <v>90</v>
       </c>
       <c r="B83" s="16"/>
@@ -4111,8 +4251,8 @@
       <c r="U83" s="2"/>
       <c r="V83" s="2"/>
     </row>
-    <row r="84" spans="1:22" ht="15">
-      <c r="A84" s="26" t="s">
+    <row r="84" spans="1:22" ht="14.4">
+      <c r="A84" s="25" t="s">
         <v>91</v>
       </c>
       <c r="B84" s="16"/>
@@ -4141,8 +4281,8 @@
       <c r="U84" s="2"/>
       <c r="V84" s="2"/>
     </row>
-    <row r="85" spans="1:22" ht="15">
-      <c r="A85" s="26" t="s">
+    <row r="85" spans="1:22" ht="14.4">
+      <c r="A85" s="25" t="s">
         <v>92</v>
       </c>
       <c r="B85" s="4"/>
@@ -4171,8 +4311,8 @@
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
     </row>
-    <row r="86" spans="1:22" ht="15">
-      <c r="A86" s="26" t="s">
+    <row r="86" spans="1:22" ht="14.4">
+      <c r="A86" s="25" t="s">
         <v>93</v>
       </c>
       <c r="B86" s="16"/>
@@ -4201,8 +4341,8 @@
       <c r="U86" s="2"/>
       <c r="V86" s="2"/>
     </row>
-    <row r="87" spans="1:22" ht="15">
-      <c r="A87" s="26" t="s">
+    <row r="87" spans="1:22" ht="14.4">
+      <c r="A87" s="25" t="s">
         <v>94</v>
       </c>
       <c r="B87" s="16"/>
@@ -4231,8 +4371,8 @@
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
     </row>
-    <row r="88" spans="1:22" ht="15">
-      <c r="A88" s="26" t="s">
+    <row r="88" spans="1:22" ht="14.4">
+      <c r="A88" s="25" t="s">
         <v>95</v>
       </c>
       <c r="B88" s="16"/>
@@ -4261,8 +4401,8 @@
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
     </row>
-    <row r="89" spans="1:22" ht="15">
-      <c r="A89" s="26" t="s">
+    <row r="89" spans="1:22" ht="14.4">
+      <c r="A89" s="25" t="s">
         <v>96</v>
       </c>
       <c r="B89" s="16"/>
@@ -4291,8 +4431,8 @@
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>
     </row>
-    <row r="90" spans="1:22" ht="15">
-      <c r="A90" s="26" t="s">
+    <row r="90" spans="1:22" ht="14.4">
+      <c r="A90" s="25" t="s">
         <v>97</v>
       </c>
       <c r="B90" s="16"/>
@@ -4321,8 +4461,8 @@
       <c r="U90" s="2"/>
       <c r="V90" s="2"/>
     </row>
-    <row r="91" spans="1:22" ht="15">
-      <c r="A91" s="26" t="s">
+    <row r="91" spans="1:22" ht="14.4">
+      <c r="A91" s="25" t="s">
         <v>98</v>
       </c>
       <c r="B91" s="16"/>
@@ -4351,8 +4491,8 @@
       <c r="U91" s="2"/>
       <c r="V91" s="2"/>
     </row>
-    <row r="92" spans="1:22" ht="15">
-      <c r="A92" s="26" t="s">
+    <row r="92" spans="1:22" ht="14.4">
+      <c r="A92" s="25" t="s">
         <v>99</v>
       </c>
       <c r="B92" s="16" t="s">
@@ -4385,8 +4525,8 @@
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
     </row>
-    <row r="93" spans="1:22" ht="15">
-      <c r="A93" s="26" t="s">
+    <row r="93" spans="1:22" ht="14.4">
+      <c r="A93" s="25" t="s">
         <v>100</v>
       </c>
       <c r="B93" s="16"/>
@@ -4415,8 +4555,8 @@
       <c r="U93" s="2"/>
       <c r="V93" s="2"/>
     </row>
-    <row r="94" spans="1:22" ht="15">
-      <c r="A94" s="26" t="s">
+    <row r="94" spans="1:22" ht="14.4">
+      <c r="A94" s="25" t="s">
         <v>101</v>
       </c>
       <c r="B94" s="16"/>
@@ -4445,8 +4585,8 @@
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
     </row>
-    <row r="95" spans="1:22" ht="15">
-      <c r="A95" s="26" t="s">
+    <row r="95" spans="1:22" ht="14.4">
+      <c r="A95" s="25" t="s">
         <v>102</v>
       </c>
       <c r="B95" s="16"/>
@@ -4475,8 +4615,8 @@
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
     </row>
-    <row r="96" spans="1:22" ht="15">
-      <c r="A96" s="26" t="s">
+    <row r="96" spans="1:22" ht="14.4">
+      <c r="A96" s="25" t="s">
         <v>103</v>
       </c>
       <c r="B96" s="16"/>
@@ -4505,8 +4645,8 @@
       <c r="U96" s="2"/>
       <c r="V96" s="2"/>
     </row>
-    <row r="97" spans="1:22" ht="15">
-      <c r="A97" s="26" t="s">
+    <row r="97" spans="1:22" ht="14.4">
+      <c r="A97" s="25" t="s">
         <v>104</v>
       </c>
       <c r="B97" s="4"/>
@@ -4535,8 +4675,8 @@
       <c r="U97" s="2"/>
       <c r="V97" s="2"/>
     </row>
-    <row r="98" spans="1:22" ht="15">
-      <c r="A98" s="26" t="s">
+    <row r="98" spans="1:22" ht="14.4">
+      <c r="A98" s="25" t="s">
         <v>105</v>
       </c>
       <c r="B98" s="4"/>
@@ -4565,8 +4705,8 @@
       <c r="U98" s="2"/>
       <c r="V98" s="2"/>
     </row>
-    <row r="99" spans="1:22" ht="15">
-      <c r="A99" s="26" t="s">
+    <row r="99" spans="1:22" ht="14.4">
+      <c r="A99" s="25" t="s">
         <v>106</v>
       </c>
       <c r="B99" s="4"/>
@@ -4595,8 +4735,8 @@
       <c r="U99" s="2"/>
       <c r="V99" s="2"/>
     </row>
-    <row r="100" spans="1:22" ht="15">
-      <c r="A100" s="26" t="s">
+    <row r="100" spans="1:22" ht="14.4">
+      <c r="A100" s="25" t="s">
         <v>107</v>
       </c>
       <c r="B100" s="4"/>
@@ -4625,22 +4765,34 @@
       <c r="U100" s="2"/>
       <c r="V100" s="2"/>
     </row>
-    <row r="101" spans="1:22" ht="15">
-      <c r="A101" s="26" t="s">
+    <row r="101" spans="1:22" ht="14.4">
+      <c r="A101" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B101" s="4"/>
-      <c r="C101" s="17"/>
-      <c r="D101" s="5">
+      <c r="B101" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" s="44">
         <v>82792580</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E101" s="44">
         <v>82811159</v>
       </c>
-      <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="2"/>
+      <c r="F101" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G101" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H101" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="I101" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
@@ -4655,22 +4807,32 @@
       <c r="U101" s="2"/>
       <c r="V101" s="2"/>
     </row>
-    <row r="102" spans="1:22" ht="15">
-      <c r="A102" s="26" t="s">
+    <row r="102" spans="1:22" ht="14.4">
+      <c r="A102" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B102" s="16"/>
-      <c r="C102" s="14"/>
+      <c r="B102" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="C102" s="48" t="s">
+        <v>287</v>
+      </c>
       <c r="D102" s="5">
         <v>82810850</v>
       </c>
       <c r="E102" s="5">
         <v>82893600</v>
       </c>
-      <c r="F102" s="11"/>
+      <c r="F102" s="29" t="s">
+        <v>288</v>
+      </c>
       <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="2"/>
+      <c r="H102" s="11">
+        <v>12</v>
+      </c>
+      <c r="I102" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
@@ -4685,8 +4847,8 @@
       <c r="U102" s="2"/>
       <c r="V102" s="2"/>
     </row>
-    <row r="103" spans="1:22" ht="15">
-      <c r="A103" s="26" t="s">
+    <row r="103" spans="1:22" ht="14.4">
+      <c r="A103" s="28" t="s">
         <v>110</v>
       </c>
       <c r="B103" s="4"/>
@@ -4700,7 +4862,9 @@
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
-      <c r="I103" s="2"/>
+      <c r="I103" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
@@ -4715,22 +4879,32 @@
       <c r="U103" s="2"/>
       <c r="V103" s="2"/>
     </row>
-    <row r="104" spans="1:22" ht="15">
-      <c r="A104" s="26" t="s">
+    <row r="104" spans="1:22" ht="16.8">
+      <c r="A104" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B104" s="16"/>
-      <c r="C104" s="15"/>
+      <c r="B104" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="C104" s="47" t="s">
+        <v>289</v>
+      </c>
       <c r="D104" s="5">
         <v>82931563</v>
       </c>
       <c r="E104" s="5">
         <v>82985019</v>
       </c>
-      <c r="F104" s="11"/>
+      <c r="F104" s="29" t="s">
+        <v>290</v>
+      </c>
       <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
-      <c r="I104" s="2"/>
+      <c r="H104" s="11">
+        <v>0</v>
+      </c>
+      <c r="I104" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
@@ -4745,22 +4919,32 @@
       <c r="U104" s="2"/>
       <c r="V104" s="2"/>
     </row>
-    <row r="105" spans="1:22" ht="15">
-      <c r="A105" s="26" t="s">
+    <row r="105" spans="1:22" ht="14.4">
+      <c r="A105" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B105" s="16"/>
-      <c r="C105" s="19"/>
+      <c r="B105" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C105" s="47" t="s">
+        <v>291</v>
+      </c>
       <c r="D105" s="5">
         <v>82988294</v>
       </c>
       <c r="E105" s="5">
         <v>82995755</v>
       </c>
-      <c r="F105" s="11"/>
+      <c r="F105" s="29" t="s">
+        <v>296</v>
+      </c>
       <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
-      <c r="I105" s="2"/>
+      <c r="H105" s="11">
+        <v>3</v>
+      </c>
+      <c r="I105" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
@@ -4775,22 +4959,32 @@
       <c r="U105" s="2"/>
       <c r="V105" s="2"/>
     </row>
-    <row r="106" spans="1:22" ht="15">
-      <c r="A106" s="26" t="s">
+    <row r="106" spans="1:22" ht="14.4">
+      <c r="A106" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B106" s="16"/>
-      <c r="C106" s="15"/>
+      <c r="B106" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C106" s="47" t="s">
+        <v>292</v>
+      </c>
       <c r="D106" s="5">
         <v>82997831</v>
       </c>
       <c r="E106" s="5">
         <v>83104794</v>
       </c>
-      <c r="F106" s="11"/>
+      <c r="F106" s="29" t="s">
+        <v>295</v>
+      </c>
       <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="2"/>
+      <c r="H106" s="11">
+        <v>3</v>
+      </c>
+      <c r="I106" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
@@ -4805,8 +4999,8 @@
       <c r="U106" s="2"/>
       <c r="V106" s="2"/>
     </row>
-    <row r="107" spans="1:22" ht="15">
-      <c r="A107" s="26" t="s">
+    <row r="107" spans="1:22" ht="14.4">
+      <c r="A107" s="28" t="s">
         <v>114</v>
       </c>
       <c r="B107" s="4"/>
@@ -4820,7 +5014,9 @@
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
-      <c r="I107" s="2"/>
+      <c r="I107" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
@@ -4835,22 +5031,32 @@
       <c r="U107" s="2"/>
       <c r="V107" s="2"/>
     </row>
-    <row r="108" spans="1:22" ht="15">
-      <c r="A108" s="26" t="s">
+    <row r="108" spans="1:22" ht="14.4">
+      <c r="A108" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B108" s="16"/>
-      <c r="C108" s="15"/>
+      <c r="B108" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C108" s="47" t="s">
+        <v>293</v>
+      </c>
       <c r="D108" s="5">
         <v>83132206</v>
       </c>
       <c r="E108" s="5">
         <v>83168823</v>
       </c>
-      <c r="F108" s="11"/>
+      <c r="F108" s="29" t="s">
+        <v>294</v>
+      </c>
       <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="2"/>
+      <c r="H108" s="11">
+        <v>3</v>
+      </c>
+      <c r="I108" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
@@ -4865,8 +5071,8 @@
       <c r="U108" s="2"/>
       <c r="V108" s="2"/>
     </row>
-    <row r="109" spans="1:22" ht="15">
-      <c r="A109" s="26" t="s">
+    <row r="109" spans="1:22" ht="14.4">
+      <c r="A109" s="28" t="s">
         <v>116</v>
       </c>
       <c r="B109" s="4"/>
@@ -4880,7 +5086,9 @@
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
-      <c r="I109" s="2"/>
+      <c r="I109" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
@@ -4895,22 +5103,32 @@
       <c r="U109" s="2"/>
       <c r="V109" s="2"/>
     </row>
-    <row r="110" spans="1:22" ht="15">
-      <c r="A110" s="26" t="s">
+    <row r="110" spans="1:22" ht="14.4">
+      <c r="A110" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B110" s="16"/>
-      <c r="C110" s="14"/>
+      <c r="B110" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C110" s="47" t="s">
+        <v>297</v>
+      </c>
       <c r="D110" s="5">
         <v>83232769</v>
       </c>
       <c r="E110" s="5">
         <v>83289469</v>
       </c>
-      <c r="F110" s="11"/>
+      <c r="F110" s="29" t="s">
+        <v>298</v>
+      </c>
       <c r="G110" s="11"/>
-      <c r="H110" s="11"/>
-      <c r="I110" s="2"/>
+      <c r="H110" s="11">
+        <v>0</v>
+      </c>
+      <c r="I110" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
@@ -4925,8 +5143,8 @@
       <c r="U110" s="2"/>
       <c r="V110" s="2"/>
     </row>
-    <row r="111" spans="1:22" ht="15">
-      <c r="A111" s="26" t="s">
+    <row r="111" spans="1:22" ht="14.4">
+      <c r="A111" s="28" t="s">
         <v>118</v>
       </c>
       <c r="B111" s="4"/>
@@ -4940,7 +5158,9 @@
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="2"/>
+      <c r="I111" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
@@ -4955,22 +5175,30 @@
       <c r="U111" s="2"/>
       <c r="V111" s="2"/>
     </row>
-    <row r="112" spans="1:22" ht="15">
-      <c r="A112" s="26" t="s">
+    <row r="112" spans="1:22" ht="14.4">
+      <c r="A112" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="B112" s="16"/>
-      <c r="C112" s="15"/>
+      <c r="B112" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="C112" s="47" t="s">
+        <v>299</v>
+      </c>
       <c r="D112" s="5">
         <v>83333199</v>
       </c>
       <c r="E112" s="5">
         <v>83613814</v>
       </c>
-      <c r="F112" s="11"/>
+      <c r="F112" s="29" t="s">
+        <v>300</v>
+      </c>
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
-      <c r="I112" s="2"/>
+      <c r="I112" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
@@ -4985,8 +5213,8 @@
       <c r="U112" s="2"/>
       <c r="V112" s="2"/>
     </row>
-    <row r="113" spans="1:22" ht="15">
-      <c r="A113" s="26" t="s">
+    <row r="113" spans="1:22" ht="14.4">
+      <c r="A113" s="28" t="s">
         <v>120</v>
       </c>
       <c r="B113" s="4"/>
@@ -5000,7 +5228,9 @@
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="2"/>
+      <c r="I113" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
@@ -5015,8 +5245,8 @@
       <c r="U113" s="2"/>
       <c r="V113" s="2"/>
     </row>
-    <row r="114" spans="1:22" ht="15">
-      <c r="A114" s="26" t="s">
+    <row r="114" spans="1:22" ht="14.4">
+      <c r="A114" s="28" t="s">
         <v>121</v>
       </c>
       <c r="B114" s="4"/>
@@ -5030,7 +5260,9 @@
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
-      <c r="I114" s="2"/>
+      <c r="I114" s="46" t="s">
+        <v>286</v>
+      </c>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
@@ -5045,8 +5277,8 @@
       <c r="U114" s="2"/>
       <c r="V114" s="2"/>
     </row>
-    <row r="115" spans="1:22" ht="15">
-      <c r="A115" s="26" t="s">
+    <row r="115" spans="1:22" ht="14.4">
+      <c r="A115" s="25" t="s">
         <v>122</v>
       </c>
       <c r="B115" s="16"/>
@@ -5075,8 +5307,8 @@
       <c r="U115" s="2"/>
       <c r="V115" s="2"/>
     </row>
-    <row r="116" spans="1:22" ht="15">
-      <c r="A116" s="26" t="s">
+    <row r="116" spans="1:22" ht="14.4">
+      <c r="A116" s="25" t="s">
         <v>123</v>
       </c>
       <c r="B116" s="4"/>
@@ -5105,8 +5337,8 @@
       <c r="U116" s="2"/>
       <c r="V116" s="2"/>
     </row>
-    <row r="117" spans="1:22" ht="15">
-      <c r="A117" s="26" t="s">
+    <row r="117" spans="1:22" ht="14.4">
+      <c r="A117" s="25" t="s">
         <v>124</v>
       </c>
       <c r="B117" s="16"/>
@@ -5135,8 +5367,8 @@
       <c r="U117" s="2"/>
       <c r="V117" s="2"/>
     </row>
-    <row r="118" spans="1:22" ht="15">
-      <c r="A118" s="26" t="s">
+    <row r="118" spans="1:22" ht="14.4">
+      <c r="A118" s="25" t="s">
         <v>125</v>
       </c>
       <c r="B118" s="16"/>
@@ -5165,8 +5397,8 @@
       <c r="U118" s="2"/>
       <c r="V118" s="2"/>
     </row>
-    <row r="119" spans="1:22" ht="15">
-      <c r="A119" s="26" t="s">
+    <row r="119" spans="1:22" ht="14.4">
+      <c r="A119" s="25" t="s">
         <v>126</v>
       </c>
       <c r="B119" s="16"/>
@@ -5195,8 +5427,8 @@
       <c r="U119" s="2"/>
       <c r="V119" s="2"/>
     </row>
-    <row r="120" spans="1:22" ht="15">
-      <c r="A120" s="26" t="s">
+    <row r="120" spans="1:22" ht="14.4">
+      <c r="A120" s="25" t="s">
         <v>127</v>
       </c>
       <c r="B120" s="16"/>
@@ -5225,8 +5457,8 @@
       <c r="U120" s="2"/>
       <c r="V120" s="2"/>
     </row>
-    <row r="121" spans="1:22" ht="15">
-      <c r="A121" s="26" t="s">
+    <row r="121" spans="1:22" ht="14.4">
+      <c r="A121" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B121" s="4"/>
@@ -5255,12 +5487,12 @@
       <c r="U121" s="2"/>
       <c r="V121" s="2"/>
     </row>
-    <row r="122" spans="1:22" ht="15">
-      <c r="A122" s="26" t="s">
+    <row r="122" spans="1:22" ht="14.4">
+      <c r="A122" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B122" s="20"/>
-      <c r="C122" s="20"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
       <c r="D122" s="5">
         <v>95470430</v>
       </c>
@@ -5285,8 +5517,8 @@
       <c r="U122" s="2"/>
       <c r="V122" s="2"/>
     </row>
-    <row r="123" spans="1:22" ht="15">
-      <c r="A123" s="26" t="s">
+    <row r="123" spans="1:22" ht="14.4">
+      <c r="A123" s="25" t="s">
         <v>129</v>
       </c>
       <c r="B123" s="16"/>
@@ -5315,8 +5547,8 @@
       <c r="U123" s="2"/>
       <c r="V123" s="2"/>
     </row>
-    <row r="124" spans="1:22" ht="15">
-      <c r="A124" s="26" t="s">
+    <row r="124" spans="1:22" ht="14.4">
+      <c r="A124" s="25" t="s">
         <v>130</v>
       </c>
       <c r="B124" s="16"/>
@@ -5345,12 +5577,12 @@
       <c r="U124" s="2"/>
       <c r="V124" s="2"/>
     </row>
-    <row r="125" spans="1:22" ht="15">
-      <c r="A125" s="26" t="s">
+    <row r="125" spans="1:22" ht="14.4">
+      <c r="A125" s="25" t="s">
         <v>131</v>
       </c>
       <c r="B125" s="11"/>
-      <c r="C125" s="20"/>
+      <c r="C125" s="19"/>
       <c r="D125" s="5">
         <v>96059361</v>
       </c>
@@ -5375,8 +5607,8 @@
       <c r="U125" s="2"/>
       <c r="V125" s="2"/>
     </row>
-    <row r="126" spans="1:22" ht="15">
-      <c r="A126" s="26" t="s">
+    <row r="126" spans="1:22" ht="14.4">
+      <c r="A126" s="25" t="s">
         <v>132</v>
       </c>
       <c r="B126" s="16"/>
@@ -5405,8 +5637,8 @@
       <c r="U126" s="2"/>
       <c r="V126" s="2"/>
     </row>
-    <row r="127" spans="1:22" ht="15">
-      <c r="A127" s="26" t="s">
+    <row r="127" spans="1:22" ht="14.4">
+      <c r="A127" s="25" t="s">
         <v>133</v>
       </c>
       <c r="B127" s="16"/>
@@ -5435,8 +5667,8 @@
       <c r="U127" s="2"/>
       <c r="V127" s="2"/>
     </row>
-    <row r="128" spans="1:22" ht="15">
-      <c r="A128" s="26" t="s">
+    <row r="128" spans="1:22" ht="14.4">
+      <c r="A128" s="25" t="s">
         <v>134</v>
       </c>
       <c r="B128" s="16"/>
@@ -5465,8 +5697,8 @@
       <c r="U128" s="2"/>
       <c r="V128" s="2"/>
     </row>
-    <row r="129" spans="1:22" ht="15">
-      <c r="A129" s="26" t="s">
+    <row r="129" spans="1:22" ht="14.4">
+      <c r="A129" s="25" t="s">
         <v>135</v>
       </c>
       <c r="B129" s="16"/>
@@ -5495,8 +5727,8 @@
       <c r="U129" s="2"/>
       <c r="V129" s="2"/>
     </row>
-    <row r="130" spans="1:22" ht="15">
-      <c r="A130" s="26" t="s">
+    <row r="130" spans="1:22" ht="14.4">
+      <c r="A130" s="25" t="s">
         <v>136</v>
       </c>
       <c r="B130" s="16"/>
@@ -5525,8 +5757,8 @@
       <c r="U130" s="2"/>
       <c r="V130" s="2"/>
     </row>
-    <row r="131" spans="1:22" ht="15">
-      <c r="A131" s="26" t="s">
+    <row r="131" spans="1:22" ht="14.4">
+      <c r="A131" s="25" t="s">
         <v>137</v>
       </c>
       <c r="B131" s="16"/>
@@ -5555,8 +5787,8 @@
       <c r="U131" s="2"/>
       <c r="V131" s="2"/>
     </row>
-    <row r="132" spans="1:22" ht="15">
-      <c r="A132" s="26" t="s">
+    <row r="132" spans="1:22" ht="14.4">
+      <c r="A132" s="25" t="s">
         <v>138</v>
       </c>
       <c r="B132" s="16"/>
@@ -5585,8 +5817,8 @@
       <c r="U132" s="2"/>
       <c r="V132" s="2"/>
     </row>
-    <row r="133" spans="1:22" ht="15">
-      <c r="A133" s="26" t="s">
+    <row r="133" spans="1:22" ht="14.4">
+      <c r="A133" s="25" t="s">
         <v>139</v>
       </c>
       <c r="B133" s="1"/>
@@ -5615,8 +5847,8 @@
       <c r="U133" s="2"/>
       <c r="V133" s="2"/>
     </row>
-    <row r="134" spans="1:22" ht="15">
-      <c r="A134" s="26" t="s">
+    <row r="134" spans="1:22" ht="14.4">
+      <c r="A134" s="25" t="s">
         <v>140</v>
       </c>
       <c r="B134" s="16"/>
@@ -5645,8 +5877,8 @@
       <c r="U134" s="2"/>
       <c r="V134" s="2"/>
     </row>
-    <row r="135" spans="1:22" ht="15">
-      <c r="A135" s="26" t="s">
+    <row r="135" spans="1:22" ht="14.4">
+      <c r="A135" s="25" t="s">
         <v>141</v>
       </c>
       <c r="B135" s="1"/>
@@ -5675,8 +5907,8 @@
       <c r="U135" s="2"/>
       <c r="V135" s="2"/>
     </row>
-    <row r="136" spans="1:22" ht="15">
-      <c r="A136" s="26" t="s">
+    <row r="136" spans="1:22" ht="14.4">
+      <c r="A136" s="25" t="s">
         <v>142</v>
       </c>
       <c r="B136" s="11"/>
@@ -5705,8 +5937,8 @@
       <c r="U136" s="2"/>
       <c r="V136" s="2"/>
     </row>
-    <row r="137" spans="1:22" ht="15">
-      <c r="A137" s="26" t="s">
+    <row r="137" spans="1:22" ht="14.4">
+      <c r="A137" s="25" t="s">
         <v>143</v>
       </c>
       <c r="B137" s="16"/>
@@ -5735,8 +5967,8 @@
       <c r="U137" s="2"/>
       <c r="V137" s="2"/>
     </row>
-    <row r="138" spans="1:22" ht="15">
-      <c r="A138" s="26" t="s">
+    <row r="138" spans="1:22" ht="14.4">
+      <c r="A138" s="25" t="s">
         <v>144</v>
       </c>
       <c r="B138" s="16"/>
@@ -5765,8 +5997,8 @@
       <c r="U138" s="2"/>
       <c r="V138" s="2"/>
     </row>
-    <row r="139" spans="1:22" ht="15">
-      <c r="A139" s="26" t="s">
+    <row r="139" spans="1:22" ht="14.4">
+      <c r="A139" s="25" t="s">
         <v>145</v>
       </c>
       <c r="B139" s="16"/>
@@ -5795,8 +6027,8 @@
       <c r="U139" s="2"/>
       <c r="V139" s="2"/>
     </row>
-    <row r="140" spans="1:22" ht="15">
-      <c r="A140" s="26" t="s">
+    <row r="140" spans="1:22" ht="14.4">
+      <c r="A140" s="25" t="s">
         <v>146</v>
       </c>
       <c r="B140" s="16"/>
@@ -5825,12 +6057,12 @@
       <c r="U140" s="2"/>
       <c r="V140" s="2"/>
     </row>
-    <row r="141" spans="1:22" ht="15">
-      <c r="A141" s="26" t="s">
+    <row r="141" spans="1:22" ht="14.4">
+      <c r="A141" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="B141" s="21"/>
-      <c r="C141" s="21"/>
+      <c r="B141" s="20"/>
+      <c r="C141" s="20"/>
       <c r="D141" s="5">
         <v>97084201</v>
       </c>
@@ -5855,8 +6087,8 @@
       <c r="U141" s="2"/>
       <c r="V141" s="2"/>
     </row>
-    <row r="142" spans="1:22" ht="15">
-      <c r="A142" s="26" t="s">
+    <row r="142" spans="1:22" ht="14.4">
+      <c r="A142" s="25" t="s">
         <v>148</v>
       </c>
       <c r="B142" s="16"/>
@@ -5885,12 +6117,12 @@
       <c r="U142" s="2"/>
       <c r="V142" s="2"/>
     </row>
-    <row r="143" spans="1:22" ht="15">
-      <c r="A143" s="26" t="s">
+    <row r="143" spans="1:22" ht="14.4">
+      <c r="A143" s="25" t="s">
         <v>149</v>
       </c>
       <c r="B143" s="16"/>
-      <c r="C143" s="20"/>
+      <c r="C143" s="19"/>
       <c r="D143" s="5">
         <v>97109423</v>
       </c>
@@ -5915,12 +6147,12 @@
       <c r="U143" s="2"/>
       <c r="V143" s="2"/>
     </row>
-    <row r="144" spans="1:22" ht="15">
-      <c r="A144" s="26" t="s">
+    <row r="144" spans="1:22" ht="14.4">
+      <c r="A144" s="25" t="s">
         <v>150</v>
       </c>
       <c r="B144" s="16"/>
-      <c r="C144" s="20"/>
+      <c r="C144" s="19"/>
       <c r="D144" s="5">
         <v>97126904</v>
       </c>
@@ -5945,12 +6177,12 @@
       <c r="U144" s="2"/>
       <c r="V144" s="2"/>
     </row>
-    <row r="145" spans="1:22" ht="15">
-      <c r="A145" s="26" t="s">
+    <row r="145" spans="1:22" ht="14.4">
+      <c r="A145" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="B145" s="21"/>
-      <c r="C145" s="21"/>
+      <c r="B145" s="20"/>
+      <c r="C145" s="20"/>
       <c r="D145" s="5">
         <v>97128891</v>
       </c>
@@ -5975,12 +6207,12 @@
       <c r="U145" s="2"/>
       <c r="V145" s="2"/>
     </row>
-    <row r="146" spans="1:22" ht="15">
-      <c r="A146" s="26" t="s">
+    <row r="146" spans="1:22" ht="14.4">
+      <c r="A146" s="25" t="s">
         <v>152</v>
       </c>
       <c r="B146" s="11"/>
-      <c r="C146" s="22"/>
+      <c r="C146" s="21"/>
       <c r="D146" s="5">
         <v>97218753</v>
       </c>
@@ -6005,12 +6237,12 @@
       <c r="U146" s="2"/>
       <c r="V146" s="2"/>
     </row>
-    <row r="147" spans="1:22" ht="15">
-      <c r="A147" s="26" t="s">
+    <row r="147" spans="1:22" ht="14.4">
+      <c r="A147" s="25" t="s">
         <v>153</v>
       </c>
       <c r="B147" s="11"/>
-      <c r="C147" s="20"/>
+      <c r="C147" s="19"/>
       <c r="D147" s="5">
         <v>108869996</v>
       </c>
@@ -6035,8 +6267,8 @@
       <c r="U147" s="2"/>
       <c r="V147" s="2"/>
     </row>
-    <row r="148" spans="1:22" ht="15">
-      <c r="A148" s="26" t="s">
+    <row r="148" spans="1:22" ht="14.4">
+      <c r="A148" s="25" t="s">
         <v>154</v>
       </c>
       <c r="B148" s="16"/>
@@ -6065,8 +6297,8 @@
       <c r="U148" s="2"/>
       <c r="V148" s="2"/>
     </row>
-    <row r="149" spans="1:22" ht="15">
-      <c r="A149" s="26" t="s">
+    <row r="149" spans="1:22" ht="14.4">
+      <c r="A149" s="25" t="s">
         <v>155</v>
       </c>
       <c r="B149" s="16"/>
@@ -6095,8 +6327,8 @@
       <c r="U149" s="2"/>
       <c r="V149" s="2"/>
     </row>
-    <row r="150" spans="1:22" thickBot="1">
-      <c r="A150" s="26" t="s">
+    <row r="150" spans="1:22" ht="15" thickBot="1">
+      <c r="A150" s="25" t="s">
         <v>156</v>
       </c>
       <c r="B150" s="4"/>
@@ -6126,13 +6358,13 @@
       <c r="V150" s="2"/>
     </row>
     <row r="151" spans="1:22" ht="15">
-      <c r="A151" s="26" t="s">
+      <c r="A151" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="B151" s="28" t="s">
+      <c r="B151" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C151" s="27" t="s">
+      <c r="C151" s="26" t="s">
         <v>221</v>
       </c>
       <c r="D151" s="5">
@@ -6141,7 +6373,7 @@
       <c r="E151" s="5">
         <v>109711074</v>
       </c>
-      <c r="F151" s="28" t="s">
+      <c r="F151" s="27" t="s">
         <v>224</v>
       </c>
       <c r="G151" s="4"/>
@@ -6163,8 +6395,8 @@
       <c r="U151" s="2"/>
       <c r="V151" s="2"/>
     </row>
-    <row r="152" spans="1:22" ht="15">
-      <c r="A152" s="26" t="s">
+    <row r="152" spans="1:22" ht="14.4">
+      <c r="A152" s="25" t="s">
         <v>158</v>
       </c>
       <c r="B152" s="4"/>
@@ -6193,8 +6425,8 @@
       <c r="U152" s="2"/>
       <c r="V152" s="2"/>
     </row>
-    <row r="153" spans="1:22" ht="15">
-      <c r="A153" s="26" t="s">
+    <row r="153" spans="1:22" ht="14.4">
+      <c r="A153" s="25" t="s">
         <v>159</v>
       </c>
       <c r="B153" s="4"/>
@@ -6223,8 +6455,8 @@
       <c r="U153" s="2"/>
       <c r="V153" s="2"/>
     </row>
-    <row r="154" spans="1:22" ht="15">
-      <c r="A154" s="26" t="s">
+    <row r="154" spans="1:22" ht="14.4">
+      <c r="A154" s="25" t="s">
         <v>160</v>
       </c>
       <c r="B154" s="4"/>
@@ -6253,8 +6485,8 @@
       <c r="U154" s="2"/>
       <c r="V154" s="2"/>
     </row>
-    <row r="155" spans="1:22" ht="15">
-      <c r="A155" s="26" t="s">
+    <row r="155" spans="1:22" ht="14.4">
+      <c r="A155" s="25" t="s">
         <v>161</v>
       </c>
       <c r="B155" s="4"/>
@@ -6283,8 +6515,8 @@
       <c r="U155" s="2"/>
       <c r="V155" s="2"/>
     </row>
-    <row r="156" spans="1:22" ht="15">
-      <c r="A156" s="26" t="s">
+    <row r="156" spans="1:22" ht="14.4">
+      <c r="A156" s="25" t="s">
         <v>162</v>
       </c>
       <c r="B156" s="4"/>
@@ -6313,8 +6545,8 @@
       <c r="U156" s="2"/>
       <c r="V156" s="2"/>
     </row>
-    <row r="157" spans="1:22" ht="15">
-      <c r="A157" s="26" t="s">
+    <row r="157" spans="1:22" ht="14.4">
+      <c r="A157" s="25" t="s">
         <v>163</v>
       </c>
       <c r="B157" s="4"/>
@@ -6343,8 +6575,8 @@
       <c r="U157" s="2"/>
       <c r="V157" s="2"/>
     </row>
-    <row r="158" spans="1:22" ht="15">
-      <c r="A158" s="26" t="s">
+    <row r="158" spans="1:22" ht="14.4">
+      <c r="A158" s="25" t="s">
         <v>164</v>
       </c>
       <c r="B158" s="4"/>
@@ -6373,16 +6605,16 @@
       <c r="U158" s="2"/>
       <c r="V158" s="2"/>
     </row>
-    <row r="159" spans="1:22" ht="15">
-      <c r="A159" s="26" t="s">
+    <row r="159" spans="1:22" ht="14.4">
+      <c r="A159" s="25" t="s">
         <v>165</v>
       </c>
       <c r="B159" s="6"/>
       <c r="C159" s="7"/>
-      <c r="D159" s="23">
+      <c r="D159" s="22">
         <v>113460909</v>
       </c>
-      <c r="E159" s="23">
+      <c r="E159" s="22">
         <v>113465343</v>
       </c>
       <c r="F159" s="4"/>
@@ -6403,16 +6635,16 @@
       <c r="U159" s="2"/>
       <c r="V159" s="2"/>
     </row>
-    <row r="160" spans="1:22" ht="15">
-      <c r="A160" s="26" t="s">
+    <row r="160" spans="1:22" ht="14.4">
+      <c r="A160" s="25" t="s">
         <v>166</v>
       </c>
       <c r="B160" s="6"/>
       <c r="C160" s="7"/>
-      <c r="D160" s="23">
+      <c r="D160" s="22">
         <v>114039627</v>
       </c>
-      <c r="E160" s="23">
+      <c r="E160" s="22">
         <v>114044419</v>
       </c>
       <c r="F160" s="4"/>
@@ -6433,16 +6665,16 @@
       <c r="U160" s="2"/>
       <c r="V160" s="2"/>
     </row>
-    <row r="161" spans="1:22" ht="15">
-      <c r="A161" s="26" t="s">
+    <row r="161" spans="1:22" ht="14.4">
+      <c r="A161" s="25" t="s">
         <v>167</v>
       </c>
       <c r="B161" s="6"/>
       <c r="C161" s="7"/>
-      <c r="D161" s="23">
+      <c r="D161" s="22">
         <v>114205077</v>
       </c>
-      <c r="E161" s="23">
+      <c r="E161" s="22">
         <v>114214900</v>
       </c>
       <c r="F161" s="4"/>
@@ -6463,16 +6695,16 @@
       <c r="U161" s="2"/>
       <c r="V161" s="2"/>
     </row>
-    <row r="162" spans="1:22" ht="15">
-      <c r="A162" s="26" t="s">
+    <row r="162" spans="1:22" ht="14.4">
+      <c r="A162" s="25" t="s">
         <v>168</v>
       </c>
       <c r="B162" s="6"/>
       <c r="C162" s="7"/>
-      <c r="D162" s="23">
+      <c r="D162" s="22">
         <v>114567590</v>
       </c>
-      <c r="E162" s="23">
+      <c r="E162" s="22">
         <v>114574104</v>
       </c>
       <c r="F162" s="4"/>
@@ -6493,16 +6725,16 @@
       <c r="U162" s="2"/>
       <c r="V162" s="2"/>
     </row>
-    <row r="163" spans="1:22" ht="15">
-      <c r="A163" s="26" t="s">
+    <row r="163" spans="1:22" ht="14.4">
+      <c r="A163" s="25" t="s">
         <v>169</v>
       </c>
       <c r="B163" s="6"/>
       <c r="C163" s="7"/>
-      <c r="D163" s="23">
+      <c r="D163" s="22">
         <v>114638336</v>
       </c>
-      <c r="E163" s="23">
+      <c r="E163" s="22">
         <v>114643543</v>
       </c>
       <c r="F163" s="4"/>
@@ -6523,16 +6755,16 @@
       <c r="U163" s="2"/>
       <c r="V163" s="2"/>
     </row>
-    <row r="164" spans="1:22" ht="15">
-      <c r="A164" s="26" t="s">
+    <row r="164" spans="1:22" ht="14.4">
+      <c r="A164" s="25" t="s">
         <v>170</v>
       </c>
       <c r="B164" s="6"/>
       <c r="C164" s="7"/>
-      <c r="D164" s="23">
+      <c r="D164" s="22">
         <v>114974326</v>
       </c>
-      <c r="E164" s="23">
+      <c r="E164" s="22">
         <v>115192808</v>
       </c>
       <c r="F164" s="4"/>
@@ -6553,16 +6785,16 @@
       <c r="U164" s="2"/>
       <c r="V164" s="2"/>
     </row>
-    <row r="165" spans="1:22" ht="15">
-      <c r="A165" s="26" t="s">
+    <row r="165" spans="1:22" ht="14.4">
+      <c r="A165" s="25" t="s">
         <v>171</v>
       </c>
       <c r="B165" s="6"/>
       <c r="C165" s="7"/>
-      <c r="D165" s="23">
+      <c r="D165" s="22">
         <v>115334226</v>
       </c>
-      <c r="E165" s="23">
+      <c r="E165" s="22">
         <v>115335879</v>
       </c>
       <c r="F165" s="4"/>
@@ -6583,16 +6815,16 @@
       <c r="U165" s="2"/>
       <c r="V165" s="2"/>
     </row>
-    <row r="166" spans="1:22" ht="15">
-      <c r="A166" s="26" t="s">
+    <row r="166" spans="1:22" ht="14.4">
+      <c r="A166" s="25" t="s">
         <v>172</v>
       </c>
       <c r="B166" s="6"/>
       <c r="C166" s="7"/>
-      <c r="D166" s="23">
+      <c r="D166" s="22">
         <v>115626920</v>
       </c>
-      <c r="E166" s="23">
+      <c r="E166" s="22">
         <v>115636639</v>
       </c>
       <c r="F166" s="4"/>
@@ -6613,16 +6845,16 @@
       <c r="U166" s="2"/>
       <c r="V166" s="2"/>
     </row>
-    <row r="167" spans="1:22" ht="15">
-      <c r="A167" s="26" t="s">
+    <row r="167" spans="1:22" ht="14.4">
+      <c r="A167" s="25" t="s">
         <v>173</v>
       </c>
       <c r="B167" s="6"/>
       <c r="C167" s="7"/>
-      <c r="D167" s="23">
+      <c r="D167" s="22">
         <v>115725079</v>
       </c>
-      <c r="E167" s="23">
+      <c r="E167" s="22">
         <v>115746451</v>
       </c>
       <c r="F167" s="4"/>
@@ -6643,16 +6875,16 @@
       <c r="U167" s="2"/>
       <c r="V167" s="2"/>
     </row>
-    <row r="168" spans="1:22" ht="15">
-      <c r="A168" s="26" t="s">
+    <row r="168" spans="1:22" ht="14.4">
+      <c r="A168" s="25" t="s">
         <v>174</v>
       </c>
       <c r="B168" s="6"/>
       <c r="C168" s="7"/>
-      <c r="D168" s="23">
+      <c r="D168" s="22">
         <v>115759698</v>
       </c>
-      <c r="E168" s="23">
+      <c r="E168" s="22">
         <v>115774070</v>
       </c>
       <c r="F168" s="4"/>
@@ -6673,16 +6905,16 @@
       <c r="U168" s="2"/>
       <c r="V168" s="2"/>
     </row>
-    <row r="169" spans="1:22" ht="15">
-      <c r="A169" s="26" t="s">
+    <row r="169" spans="1:22" ht="14.4">
+      <c r="A169" s="25" t="s">
         <v>175</v>
       </c>
       <c r="B169" s="6"/>
       <c r="C169" s="7"/>
-      <c r="D169" s="23">
+      <c r="D169" s="22">
         <v>115761181</v>
       </c>
-      <c r="E169" s="23">
+      <c r="E169" s="22">
         <v>115761777</v>
       </c>
       <c r="F169" s="4"/>
@@ -6703,16 +6935,16 @@
       <c r="U169" s="2"/>
       <c r="V169" s="2"/>
     </row>
-    <row r="170" spans="1:22" ht="15">
-      <c r="A170" s="26" t="s">
+    <row r="170" spans="1:22" ht="14.4">
+      <c r="A170" s="25" t="s">
         <v>176</v>
       </c>
       <c r="B170" s="6"/>
       <c r="C170" s="7"/>
-      <c r="D170" s="23">
+      <c r="D170" s="22">
         <v>115795806</v>
       </c>
-      <c r="E170" s="23">
+      <c r="E170" s="22">
         <v>115830521</v>
       </c>
       <c r="F170" s="4"/>
@@ -6733,16 +6965,16 @@
       <c r="U170" s="2"/>
       <c r="V170" s="2"/>
     </row>
-    <row r="171" spans="1:22" ht="15">
-      <c r="A171" s="26" t="s">
+    <row r="171" spans="1:22" ht="14.4">
+      <c r="A171" s="25" t="s">
         <v>177</v>
       </c>
       <c r="B171" s="6"/>
       <c r="C171" s="7"/>
-      <c r="D171" s="23">
+      <c r="D171" s="22">
         <v>115895606</v>
       </c>
-      <c r="E171" s="23">
+      <c r="E171" s="22">
         <v>115924433</v>
       </c>
       <c r="F171" s="4"/>
@@ -6763,16 +6995,16 @@
       <c r="U171" s="2"/>
       <c r="V171" s="2"/>
     </row>
-    <row r="172" spans="1:22" ht="15">
-      <c r="A172" s="26" t="s">
+    <row r="172" spans="1:22" ht="14.4">
+      <c r="A172" s="25" t="s">
         <v>178</v>
       </c>
       <c r="B172" s="6"/>
       <c r="C172" s="7"/>
-      <c r="D172" s="23">
+      <c r="D172" s="22">
         <v>115940485</v>
       </c>
-      <c r="E172" s="23">
+      <c r="E172" s="22">
         <v>115948547</v>
       </c>
       <c r="F172" s="4"/>
@@ -6793,16 +7025,16 @@
       <c r="U172" s="2"/>
       <c r="V172" s="2"/>
     </row>
-    <row r="173" spans="1:22" ht="15">
-      <c r="A173" s="26" t="s">
+    <row r="173" spans="1:22" ht="14.4">
+      <c r="A173" s="25" t="s">
         <v>179</v>
       </c>
       <c r="B173" s="6"/>
       <c r="C173" s="7"/>
-      <c r="D173" s="23">
+      <c r="D173" s="22">
         <v>115952522</v>
       </c>
-      <c r="E173" s="23">
+      <c r="E173" s="22">
         <v>115953478</v>
       </c>
       <c r="F173" s="4"/>
@@ -6823,16 +7055,16 @@
       <c r="U173" s="2"/>
       <c r="V173" s="2"/>
     </row>
-    <row r="174" spans="1:22" ht="15">
-      <c r="A174" s="26" t="s">
+    <row r="174" spans="1:22" ht="14.4">
+      <c r="A174" s="25" t="s">
         <v>180</v>
       </c>
       <c r="B174" s="6"/>
       <c r="C174" s="7"/>
-      <c r="D174" s="23">
+      <c r="D174" s="22">
         <v>116180918</v>
       </c>
-      <c r="E174" s="23">
+      <c r="E174" s="22">
         <v>116185772</v>
       </c>
       <c r="F174" s="4"/>
@@ -6853,8 +7085,8 @@
       <c r="U174" s="2"/>
       <c r="V174" s="2"/>
     </row>
-    <row r="175" spans="1:22" ht="15">
-      <c r="A175" s="26" t="s">
+    <row r="175" spans="1:22" ht="14.4">
+      <c r="A175" s="25" t="s">
         <v>181</v>
       </c>
       <c r="B175" s="4"/>
@@ -6883,8 +7115,8 @@
       <c r="U175" s="2"/>
       <c r="V175" s="2"/>
     </row>
-    <row r="176" spans="1:22" ht="15">
-      <c r="A176" s="26" t="s">
+    <row r="176" spans="1:22" ht="14.4">
+      <c r="A176" s="25" t="s">
         <v>182</v>
       </c>
       <c r="B176" s="4"/>
@@ -6913,8 +7145,8 @@
       <c r="U176" s="2"/>
       <c r="V176" s="2"/>
     </row>
-    <row r="177" spans="1:22" ht="15">
-      <c r="A177" s="26" t="s">
+    <row r="177" spans="1:22" ht="14.4">
+      <c r="A177" s="25" t="s">
         <v>183</v>
       </c>
       <c r="B177" s="4"/>
@@ -6943,8 +7175,8 @@
       <c r="U177" s="2"/>
       <c r="V177" s="2"/>
     </row>
-    <row r="178" spans="1:22" ht="15">
-      <c r="A178" s="26" t="s">
+    <row r="178" spans="1:22" ht="14.4">
+      <c r="A178" s="25" t="s">
         <v>184</v>
       </c>
       <c r="B178" s="4"/>
@@ -6973,8 +7205,8 @@
       <c r="U178" s="2"/>
       <c r="V178" s="2"/>
     </row>
-    <row r="179" spans="1:22" ht="15">
-      <c r="A179" s="26" t="s">
+    <row r="179" spans="1:22" ht="14.4">
+      <c r="A179" s="25" t="s">
         <v>185</v>
       </c>
       <c r="B179" s="4"/>
@@ -7003,8 +7235,8 @@
       <c r="U179" s="2"/>
       <c r="V179" s="2"/>
     </row>
-    <row r="180" spans="1:22" ht="15">
-      <c r="A180" s="26" t="s">
+    <row r="180" spans="1:22" ht="14.4">
+      <c r="A180" s="25" t="s">
         <v>186</v>
       </c>
       <c r="B180" s="4"/>
@@ -7033,8 +7265,8 @@
       <c r="U180" s="2"/>
       <c r="V180" s="2"/>
     </row>
-    <row r="181" spans="1:22" ht="15">
-      <c r="A181" s="26" t="s">
+    <row r="181" spans="1:22" ht="14.4">
+      <c r="A181" s="25" t="s">
         <v>187</v>
       </c>
       <c r="B181" s="4"/>
@@ -7063,8 +7295,8 @@
       <c r="U181" s="2"/>
       <c r="V181" s="2"/>
     </row>
-    <row r="182" spans="1:22" ht="15">
-      <c r="A182" s="26" t="s">
+    <row r="182" spans="1:22" ht="14.4">
+      <c r="A182" s="25" t="s">
         <v>188</v>
       </c>
       <c r="B182" s="4"/>
@@ -7093,8 +7325,8 @@
       <c r="U182" s="2"/>
       <c r="V182" s="2"/>
     </row>
-    <row r="183" spans="1:22" ht="15">
-      <c r="A183" s="26" t="s">
+    <row r="183" spans="1:22" ht="14.4">
+      <c r="A183" s="25" t="s">
         <v>189</v>
       </c>
       <c r="B183" s="4"/>
@@ -7123,8 +7355,8 @@
       <c r="U183" s="2"/>
       <c r="V183" s="2"/>
     </row>
-    <row r="184" spans="1:22" thickBot="1">
-      <c r="A184" s="26" t="s">
+    <row r="184" spans="1:22" ht="15" thickBot="1">
+      <c r="A184" s="25" t="s">
         <v>190</v>
       </c>
       <c r="B184" s="4"/>
@@ -7153,14 +7385,14 @@
       <c r="U184" s="2"/>
       <c r="V184" s="2"/>
     </row>
-    <row r="185" spans="1:22" thickBot="1">
-      <c r="A185" s="29" t="s">
+    <row r="185" spans="1:22" ht="15.6" thickBot="1">
+      <c r="A185" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="B185" s="27" t="s">
+      <c r="B185" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C185" s="32" t="s">
+      <c r="C185" s="31" t="s">
         <v>235</v>
       </c>
       <c r="D185" s="5">
@@ -7189,14 +7421,14 @@
       <c r="U185" s="2"/>
       <c r="V185" s="2"/>
     </row>
-    <row r="186" spans="1:22" thickBot="1">
-      <c r="A186" s="29" t="s">
+    <row r="186" spans="1:22" ht="15.6" thickBot="1">
+      <c r="A186" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="B186" s="27" t="s">
+      <c r="B186" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C186" s="32" t="s">
+      <c r="C186" s="31" t="s">
         <v>236</v>
       </c>
       <c r="D186" s="5">
@@ -7205,7 +7437,7 @@
       <c r="E186" s="5">
         <v>144991569</v>
       </c>
-      <c r="F186" s="28" t="s">
+      <c r="F186" s="27" t="s">
         <v>237</v>
       </c>
       <c r="G186" s="4"/>
@@ -7227,14 +7459,14 @@
       <c r="U186" s="2"/>
       <c r="V186" s="2"/>
     </row>
-    <row r="187" spans="1:22" thickBot="1">
-      <c r="A187" s="29" t="s">
+    <row r="187" spans="1:22" ht="15.6" thickBot="1">
+      <c r="A187" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="B187" s="27" t="s">
+      <c r="B187" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C187" s="32" t="s">
+      <c r="C187" s="31" t="s">
         <v>238</v>
       </c>
       <c r="D187" s="5">
@@ -7243,7 +7475,7 @@
       <c r="E187" s="5">
         <v>145048712</v>
       </c>
-      <c r="F187" s="28" t="s">
+      <c r="F187" s="27" t="s">
         <v>239</v>
       </c>
       <c r="G187" s="4"/>
@@ -7265,14 +7497,14 @@
       <c r="U187" s="2"/>
       <c r="V187" s="2"/>
     </row>
-    <row r="188" spans="1:22" thickBot="1">
-      <c r="A188" s="29" t="s">
+    <row r="188" spans="1:22" ht="15.6" thickBot="1">
+      <c r="A188" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="B188" s="27" t="s">
+      <c r="B188" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C188" s="32" t="s">
+      <c r="C188" s="31" t="s">
         <v>240</v>
       </c>
       <c r="D188" s="5">
@@ -7281,7 +7513,7 @@
       <c r="E188" s="5">
         <v>145246309</v>
       </c>
-      <c r="F188" s="28" t="s">
+      <c r="F188" s="27" t="s">
         <v>241</v>
       </c>
       <c r="G188" s="4"/>
@@ -7303,14 +7535,14 @@
       <c r="U188" s="2"/>
       <c r="V188" s="2"/>
     </row>
-    <row r="189" spans="1:22" thickBot="1">
-      <c r="A189" s="29" t="s">
+    <row r="189" spans="1:22" ht="15.6" thickBot="1">
+      <c r="A189" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="B189" s="27" t="s">
+      <c r="B189" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C189" s="32" t="s">
+      <c r="C189" s="31" t="s">
         <v>242</v>
       </c>
       <c r="D189" s="5">
@@ -7319,7 +7551,7 @@
       <c r="E189" s="5">
         <v>145275187</v>
       </c>
-      <c r="F189" s="28" t="s">
+      <c r="F189" s="27" t="s">
         <v>243</v>
       </c>
       <c r="G189" s="4"/>
@@ -7342,13 +7574,13 @@
       <c r="V189" s="2"/>
     </row>
     <row r="190" spans="1:22" ht="15">
-      <c r="A190" s="29" t="s">
+      <c r="A190" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="B190" s="27" t="s">
+      <c r="B190" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C190" s="32" t="s">
+      <c r="C190" s="31" t="s">
         <v>244</v>
       </c>
       <c r="D190" s="5">
@@ -7357,7 +7589,7 @@
       <c r="E190" s="5">
         <v>145581973</v>
       </c>
-      <c r="F190" s="28" t="s">
+      <c r="F190" s="27" t="s">
         <v>245</v>
       </c>
       <c r="G190" s="4"/>
@@ -7379,8 +7611,8 @@
       <c r="U190" s="2"/>
       <c r="V190" s="2"/>
     </row>
-    <row r="191" spans="1:22" ht="15">
-      <c r="A191" s="29" t="s">
+    <row r="191" spans="1:22" ht="14.4">
+      <c r="A191" s="28" t="s">
         <v>197</v>
       </c>
       <c r="B191" s="4"/>
@@ -7409,14 +7641,14 @@
       <c r="U191" s="2"/>
       <c r="V191" s="2"/>
     </row>
-    <row r="192" spans="1:22" ht="15">
-      <c r="A192" s="29" t="s">
+    <row r="192" spans="1:22" ht="14.4">
+      <c r="A192" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="B192" s="28" t="s">
+      <c r="B192" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C192" s="32" t="s">
+      <c r="C192" s="31" t="s">
         <v>246</v>
       </c>
       <c r="D192" s="5">
@@ -7425,7 +7657,7 @@
       <c r="E192" s="5">
         <v>145652325</v>
       </c>
-      <c r="F192" s="33">
+      <c r="F192" s="32">
         <v>113159</v>
       </c>
       <c r="G192" s="4"/>
@@ -7447,14 +7679,14 @@
       <c r="U192" s="2"/>
       <c r="V192" s="2"/>
     </row>
-    <row r="193" spans="1:22" ht="15">
-      <c r="A193" s="29" t="s">
+    <row r="193" spans="1:22" ht="14.4">
+      <c r="A193" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="B193" s="28" t="s">
+      <c r="B193" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C193" s="32" t="s">
+      <c r="C193" s="31" t="s">
         <v>247</v>
       </c>
       <c r="D193" s="5">
@@ -7463,7 +7695,7 @@
       <c r="E193" s="5">
         <v>145799845</v>
       </c>
-      <c r="F193" s="33">
+      <c r="F193" s="32">
         <v>126165</v>
       </c>
       <c r="G193" s="4"/>
@@ -7485,14 +7717,14 @@
       <c r="U193" s="2"/>
       <c r="V193" s="2"/>
     </row>
-    <row r="194" spans="1:22" ht="15">
-      <c r="A194" s="29" t="s">
+    <row r="194" spans="1:22" ht="14.4">
+      <c r="A194" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="B194" s="28" t="s">
+      <c r="B194" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C194" s="32" t="s">
+      <c r="C194" s="31" t="s">
         <v>248</v>
       </c>
       <c r="D194" s="5">
@@ -7501,7 +7733,7 @@
       <c r="E194" s="5">
         <v>145824726</v>
       </c>
-      <c r="F194" s="28" t="s">
+      <c r="F194" s="27" t="s">
         <v>249</v>
       </c>
       <c r="G194" s="4"/>
@@ -7521,14 +7753,14 @@
       <c r="U194" s="2"/>
       <c r="V194" s="2"/>
     </row>
-    <row r="195" spans="1:22" ht="15">
-      <c r="A195" s="29" t="s">
+    <row r="195" spans="1:22" ht="14.4">
+      <c r="A195" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="B195" s="28" t="s">
+      <c r="B195" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C195" s="32" t="s">
+      <c r="C195" s="31" t="s">
         <v>250</v>
       </c>
       <c r="D195" s="5">
@@ -7559,14 +7791,14 @@
       <c r="U195" s="2"/>
       <c r="V195" s="2"/>
     </row>
-    <row r="196" spans="1:22" ht="15">
-      <c r="A196" s="29" t="s">
+    <row r="196" spans="1:22" ht="14.4">
+      <c r="A196" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="B196" s="28" t="s">
+      <c r="B196" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C196" s="32" t="s">
+      <c r="C196" s="31" t="s">
         <v>251</v>
       </c>
       <c r="D196" s="5">
@@ -7575,7 +7807,7 @@
       <c r="E196" s="5">
         <v>145883591</v>
       </c>
-      <c r="F196" s="28" t="s">
+      <c r="F196" s="27" t="s">
         <v>252</v>
       </c>
       <c r="G196" s="4"/>
@@ -7597,14 +7829,14 @@
       <c r="U196" s="2"/>
       <c r="V196" s="2"/>
     </row>
-    <row r="197" spans="1:22" ht="15">
-      <c r="A197" s="29" t="s">
+    <row r="197" spans="1:22" ht="14.4">
+      <c r="A197" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="B197" s="28" t="s">
+      <c r="B197" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C197" s="32" t="s">
+      <c r="C197" s="31" t="s">
         <v>253</v>
       </c>
       <c r="D197" s="5">
@@ -7613,7 +7845,7 @@
       <c r="E197" s="5">
         <v>145937594</v>
       </c>
-      <c r="F197" s="28" t="s">
+      <c r="F197" s="27" t="s">
         <v>254</v>
       </c>
       <c r="G197" s="4"/>
@@ -7635,14 +7867,14 @@
       <c r="U197" s="2"/>
       <c r="V197" s="2"/>
     </row>
-    <row r="198" spans="1:22" ht="15">
-      <c r="A198" s="26" t="s">
+    <row r="198" spans="1:22" ht="14.4">
+      <c r="A198" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="B198" s="28" t="s">
+      <c r="B198" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C198" s="32" t="s">
+      <c r="C198" s="31" t="s">
         <v>256</v>
       </c>
       <c r="D198" s="5">
@@ -7651,7 +7883,7 @@
       <c r="E198" s="5">
         <v>145945394</v>
       </c>
-      <c r="F198" s="28" t="s">
+      <c r="F198" s="27" t="s">
         <v>257</v>
       </c>
       <c r="G198" s="4"/>
@@ -7673,14 +7905,14 @@
       <c r="U198" s="2"/>
       <c r="V198" s="2"/>
     </row>
-    <row r="199" spans="1:22" ht="15">
-      <c r="A199" s="29" t="s">
+    <row r="199" spans="1:22" ht="14.4">
+      <c r="A199" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="B199" s="28" t="s">
+      <c r="B199" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C199" s="32" t="s">
+      <c r="C199" s="31" t="s">
         <v>255</v>
       </c>
       <c r="D199" s="5">
@@ -7712,13 +7944,13 @@
       <c r="V199" s="2"/>
     </row>
     <row r="200" spans="1:22" ht="15">
-      <c r="A200" s="26" t="s">
+      <c r="A200" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="B200" s="28" t="s">
+      <c r="B200" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C200" s="34" t="s">
+      <c r="C200" s="33" t="s">
         <v>258</v>
       </c>
       <c r="D200" s="5">
@@ -7727,7 +7959,7 @@
       <c r="E200" s="5">
         <v>146072360</v>
       </c>
-      <c r="F200" s="28" t="s">
+      <c r="F200" s="27" t="s">
         <v>234</v>
       </c>
       <c r="G200" s="4"/>
@@ -7749,8 +7981,8 @@
       <c r="U200" s="2"/>
       <c r="V200" s="2"/>
     </row>
-    <row r="201" spans="1:22" ht="15">
-      <c r="A201" s="29" t="s">
+    <row r="201" spans="1:22" ht="14.4">
+      <c r="A201" s="28" t="s">
         <v>207</v>
       </c>
       <c r="B201" s="4"/>
@@ -7779,8 +8011,8 @@
       <c r="U201" s="2"/>
       <c r="V201" s="2"/>
     </row>
-    <row r="202" spans="1:22" ht="15">
-      <c r="A202" s="29" t="s">
+    <row r="202" spans="1:22" ht="14.4">
+      <c r="A202" s="28" t="s">
         <v>208</v>
       </c>
       <c r="B202" s="4"/>
@@ -7809,14 +8041,14 @@
       <c r="U202" s="2"/>
       <c r="V202" s="2"/>
     </row>
-    <row r="203" spans="1:22" ht="15">
-      <c r="A203" s="29" t="s">
+    <row r="203" spans="1:22" ht="14.4">
+      <c r="A203" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="B203" s="28" t="s">
+      <c r="B203" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C203" s="32" t="s">
+      <c r="C203" s="31" t="s">
         <v>259</v>
       </c>
       <c r="D203" s="5">
@@ -7825,7 +8057,7 @@
       <c r="E203" s="5">
         <v>146195343</v>
       </c>
-      <c r="F203" s="28" t="s">
+      <c r="F203" s="27" t="s">
         <v>260</v>
       </c>
       <c r="G203" s="4"/>
@@ -7847,14 +8079,14 @@
       <c r="U203" s="2"/>
       <c r="V203" s="2"/>
     </row>
-    <row r="204" spans="1:22" ht="15">
-      <c r="A204" s="29" t="s">
+    <row r="204" spans="1:22" ht="14.4">
+      <c r="A204" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="B204" s="28" t="s">
+      <c r="B204" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C204" s="32" t="s">
+      <c r="C204" s="31" t="s">
         <v>261</v>
       </c>
       <c r="D204" s="5">
@@ -7863,7 +8095,7 @@
       <c r="E204" s="5">
         <v>146243445</v>
       </c>
-      <c r="F204" s="28" t="s">
+      <c r="F204" s="27" t="s">
         <v>262</v>
       </c>
       <c r="G204" s="4"/>
@@ -7885,14 +8117,14 @@
       <c r="U204" s="2"/>
       <c r="V204" s="2"/>
     </row>
-    <row r="205" spans="1:22" thickBot="1">
-      <c r="A205" s="29" t="s">
+    <row r="205" spans="1:22" ht="15" thickBot="1">
+      <c r="A205" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="B205" s="28" t="s">
+      <c r="B205" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C205" s="32" t="s">
+      <c r="C205" s="31" t="s">
         <v>263</v>
       </c>
       <c r="D205" s="5">
@@ -7901,7 +8133,7 @@
       <c r="E205" s="5">
         <v>146307587</v>
       </c>
-      <c r="F205" s="28" t="s">
+      <c r="F205" s="27" t="s">
         <v>264</v>
       </c>
       <c r="G205" s="4"/>
@@ -7924,13 +8156,13 @@
       <c r="V205" s="2"/>
     </row>
     <row r="206" spans="1:22" ht="15">
-      <c r="A206" s="29" t="s">
+      <c r="A206" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B206" s="28" t="s">
+      <c r="B206" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C206" s="27" t="s">
+      <c r="C206" s="26" t="s">
         <v>265</v>
       </c>
       <c r="D206" s="5">
@@ -7939,7 +8171,7 @@
       <c r="E206" s="5">
         <v>146480596</v>
       </c>
-      <c r="F206" s="28" t="s">
+      <c r="F206" s="27" t="s">
         <v>266</v>
       </c>
       <c r="G206" s="4"/>
@@ -7961,14 +8193,14 @@
       <c r="U206" s="2"/>
       <c r="V206" s="2"/>
     </row>
-    <row r="207" spans="1:22" ht="15">
-      <c r="A207" s="29" t="s">
+    <row r="207" spans="1:22" ht="14.4">
+      <c r="A207" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="B207" s="28" t="s">
+      <c r="B207" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C207" s="35" t="s">
+      <c r="C207" s="34" t="s">
         <v>267</v>
       </c>
       <c r="D207" s="5">
@@ -7997,12 +8229,12 @@
       <c r="U207" s="2"/>
       <c r="V207" s="2"/>
     </row>
-    <row r="208" spans="1:22" thickBot="1">
-      <c r="A208" s="29" t="s">
+    <row r="208" spans="1:22" ht="15" thickBot="1">
+      <c r="A208" s="28" t="s">
         <v>214</v>
       </c>
       <c r="B208" s="11"/>
-      <c r="C208" s="24"/>
+      <c r="C208" s="23"/>
       <c r="D208" s="5">
         <v>146768806</v>
       </c>
@@ -8027,14 +8259,14 @@
       <c r="U208" s="2"/>
       <c r="V208" s="2"/>
     </row>
-    <row r="209" spans="1:22" thickBot="1">
-      <c r="A209" s="29" t="s">
+    <row r="209" spans="1:22" ht="15.6" thickBot="1">
+      <c r="A209" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="B209" s="27" t="s">
+      <c r="B209" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C209" s="32" t="s">
+      <c r="C209" s="31" t="s">
         <v>268</v>
       </c>
       <c r="D209" s="5">
@@ -8043,7 +8275,7 @@
       <c r="E209" s="5">
         <v>153498961</v>
       </c>
-      <c r="F209" s="30" t="s">
+      <c r="F209" s="29" t="s">
         <v>269</v>
       </c>
       <c r="G209" s="11"/>
@@ -8066,13 +8298,13 @@
       <c r="V209" s="2"/>
     </row>
     <row r="210" spans="1:22" ht="15">
-      <c r="A210" s="29" t="s">
+      <c r="A210" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="B210" s="27" t="s">
+      <c r="B210" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C210" s="27" t="s">
+      <c r="C210" s="26" t="s">
         <v>233</v>
       </c>
       <c r="D210" s="5">
@@ -8081,7 +8313,7 @@
       <c r="E210" s="5">
         <v>153936148</v>
       </c>
-      <c r="F210" s="30" t="s">
+      <c r="F210" s="29" t="s">
         <v>234</v>
       </c>
       <c r="G210" s="11"/>
@@ -8103,14 +8335,14 @@
       <c r="U210" s="2"/>
       <c r="V210" s="2"/>
     </row>
-    <row r="211" spans="1:22" ht="15">
-      <c r="A211" s="29" t="s">
+    <row r="211" spans="1:22" ht="14.4">
+      <c r="A211" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="B211" s="30" t="s">
+      <c r="B211" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="C211" s="29" t="s">
+      <c r="C211" s="28" t="s">
         <v>227</v>
       </c>
       <c r="D211" s="5">
@@ -8119,7 +8351,7 @@
       <c r="E211" s="5">
         <v>154524620</v>
       </c>
-      <c r="F211" s="30" t="s">
+      <c r="F211" s="29" t="s">
         <v>228</v>
       </c>
       <c r="G211" s="11"/>
@@ -8141,8 +8373,8 @@
       <c r="U211" s="2"/>
       <c r="V211" s="2"/>
     </row>
-    <row r="212" spans="1:22" thickBot="1">
-      <c r="A212" s="29" t="s">
+    <row r="212" spans="1:22" ht="15" thickBot="1">
+      <c r="A212" s="28" t="s">
         <v>218</v>
       </c>
       <c r="B212" s="4"/>
@@ -8172,13 +8404,13 @@
       <c r="V212" s="2"/>
     </row>
     <row r="213" spans="1:22" ht="15">
-      <c r="A213" s="29" t="s">
+      <c r="A213" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="B213" s="30" t="s">
+      <c r="B213" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="C213" s="27" t="s">
+      <c r="C213" s="26" t="s">
         <v>229</v>
       </c>
       <c r="D213" s="5">
@@ -8187,7 +8419,7 @@
       <c r="E213" s="5">
         <v>155364610</v>
       </c>
-      <c r="F213" s="30" t="s">
+      <c r="F213" s="29" t="s">
         <v>230</v>
       </c>
       <c r="G213" s="11"/>
@@ -8209,14 +8441,14 @@
       <c r="U213" s="2"/>
       <c r="V213" s="2"/>
     </row>
-    <row r="214" spans="1:22" ht="15">
-      <c r="A214" s="29" t="s">
+    <row r="214" spans="1:22" ht="14.4">
+      <c r="A214" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="B214" s="30" t="s">
+      <c r="B214" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="C214" s="29" t="s">
+      <c r="C214" s="28" t="s">
         <v>231</v>
       </c>
       <c r="D214" s="5">
@@ -8225,7 +8457,7 @@
       <c r="E214" s="5">
         <v>156650711</v>
       </c>
-      <c r="F214" s="30" t="s">
+      <c r="F214" s="29" t="s">
         <v>232</v>
       </c>
       <c r="G214" s="11"/>
@@ -8248,10 +8480,10 @@
       <c r="V214" s="2"/>
     </row>
     <row r="216" spans="1:22" ht="15.75" customHeight="1">
-      <c r="B216" s="31" t="s">
+      <c r="B216" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="C216" s="31" t="s">
+      <c r="C216" s="30" t="s">
         <v>226</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Editando las filas del excel
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JUAN CARLOS DIAZ\Desktop\pc2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelly\Desktop\pc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0028E751-989D-46D8-9EA0-BABF82C74025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9012" windowHeight="7560"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C1" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="292">
   <si>
     <t>Localización</t>
   </si>
@@ -837,48 +838,6 @@
     <t>bbbbbbbbbbbbbbbbbbbbb</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a </t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>x1</t>
-  </si>
-  <si>
-    <t>x2</t>
-  </si>
-  <si>
-    <t>x3</t>
-  </si>
-  <si>
-    <t>x4</t>
-  </si>
-  <si>
-    <t>x5</t>
-  </si>
-  <si>
-    <t>x6</t>
-  </si>
-  <si>
-    <t>x7</t>
-  </si>
-  <si>
     <t>terminado</t>
   </si>
   <si>
@@ -922,12 +881,27 @@
   </si>
   <si>
     <t>4,3</t>
+  </si>
+  <si>
+    <t>Vestigial Like Family Member 3</t>
+  </si>
+  <si>
+    <t>Charged Multivesicular Body Protein 2B</t>
+  </si>
+  <si>
+    <t>POU Class 1 Homeobox 1</t>
+  </si>
+  <si>
+    <t>5-Hydroxytryptamine Receptor 1F</t>
+  </si>
+  <si>
+    <t>CGG Triplet Repeat Binding Protein 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18">
     <font>
       <sz val="10"/>
@@ -938,26 +912,31 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -968,16 +947,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF444444"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1073,7 +1055,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1212,22 +1194,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1239,6 +1205,22 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1261,25 +1243,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>310515</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1120140</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:colOff>958215</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>108585</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Elipse 2"/>
+        <xdr:cNvPr id="3" name="Elipse 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1432560" y="1813560"/>
-          <a:ext cx="2948940" cy="2171700"/>
+          <a:off x="1243965" y="2642235"/>
+          <a:ext cx="2886075" cy="2257425"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1317,23 +1305,29 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1249680</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5"/>
+        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2209800" y="2994660"/>
-          <a:ext cx="1257300" cy="510540"/>
+          <a:off x="2183130" y="3251835"/>
+          <a:ext cx="1194435" cy="525780"/>
         </a:xfrm>
         <a:prstGeom prst="curvedUpArrow">
           <a:avLst/>
@@ -1373,25 +1367,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1173480</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>1211580</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1615440</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>1653540</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Elipse 1"/>
+        <xdr:cNvPr id="2" name="Elipse 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2133600" y="2255520"/>
-          <a:ext cx="441960" cy="396240"/>
+          <a:off x="2145030" y="2767965"/>
+          <a:ext cx="441960" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1427,25 +1427,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2232660</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>2146935</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>287655</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Elipse 7"/>
+        <xdr:cNvPr id="8" name="Elipse 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3192780" y="2286000"/>
-          <a:ext cx="441960" cy="396240"/>
+          <a:off x="3080385" y="2779395"/>
+          <a:ext cx="379095" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1493,13 +1499,19 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Acorde 6"/>
+        <xdr:cNvPr id="7" name="Acorde 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="18150062">
-          <a:off x="2451919" y="3256289"/>
-          <a:ext cx="664250" cy="517950"/>
+          <a:off x="2413819" y="3380114"/>
+          <a:ext cx="687110" cy="517950"/>
         </a:xfrm>
         <a:prstGeom prst="chord">
           <a:avLst/>
@@ -1732,24 +1744,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:V216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1757,15 +1769,15 @@
       <c r="A1" s="24"/>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="42" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -1793,25 +1805,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="14.4">
+    <row r="3" spans="1:22" ht="15">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>273</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>279</v>
-      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="5">
         <v>32091689</v>
       </c>
       <c r="E3" s="5">
         <v>32091761</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1827,25 +1835,21 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
     </row>
-    <row r="4" spans="1:22" ht="14.4">
+    <row r="4" spans="1:22" ht="15">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>272</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>280</v>
-      </c>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="5">
         <v>32837131</v>
       </c>
       <c r="E4" s="5">
         <v>32838076</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1861,25 +1865,21 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
     </row>
-    <row r="5" spans="1:22" ht="14.4">
+    <row r="5" spans="1:22" ht="15">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>275</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>281</v>
-      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="5">
         <v>33089112</v>
       </c>
       <c r="E5" s="5">
         <v>33090132</v>
       </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1895,25 +1895,21 @@
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="14.4">
+    <row r="6" spans="1:22" ht="15">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>276</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>282</v>
-      </c>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="5">
         <v>33764252</v>
       </c>
       <c r="E6" s="5">
         <v>33768221</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1929,25 +1925,21 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="14.4">
+    <row r="7" spans="1:22" ht="15">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>277</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>283</v>
-      </c>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="5">
         <v>33810174</v>
       </c>
       <c r="E7" s="5">
         <v>33811741</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1963,15 +1955,15 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="14.4">
+    <row r="8" spans="1:22" ht="15">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>278</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>284</v>
+      <c r="B8" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>287</v>
       </c>
       <c r="D8" s="5">
         <v>33882149</v>
@@ -1979,9 +1971,9 @@
       <c r="E8" s="5">
         <v>33934641</v>
       </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1997,15 +1989,15 @@
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="14.4">
+    <row r="9" spans="1:22" ht="15">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>274</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>285</v>
+      <c r="B9" s="49" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>288</v>
       </c>
       <c r="D9" s="5">
         <v>34199383</v>
@@ -2035,8 +2027,12 @@
       <c r="A10" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="13"/>
+      <c r="B10" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>289</v>
+      </c>
       <c r="D10" s="5">
         <v>34235896</v>
       </c>
@@ -2061,12 +2057,16 @@
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="14.4">
+    <row r="11" spans="1:22" ht="15">
       <c r="A11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>290</v>
+      </c>
       <c r="D11" s="5">
         <v>34811253</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="14.4">
+    <row r="12" spans="1:22" ht="15">
       <c r="A12" s="25" t="s">
         <v>19</v>
       </c>
@@ -2121,12 +2121,16 @@
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
     </row>
-    <row r="13" spans="1:22" ht="14.4">
+    <row r="13" spans="1:22" ht="15">
       <c r="A13" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>291</v>
+      </c>
       <c r="D13" s="5">
         <v>34857740</v>
       </c>
@@ -2151,7 +2155,7 @@
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
     </row>
-    <row r="14" spans="1:22" ht="14.4">
+    <row r="14" spans="1:22" ht="15">
       <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
@@ -2181,7 +2185,7 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="14.4">
+    <row r="15" spans="1:22" ht="15">
       <c r="A15" s="25" t="s">
         <v>22</v>
       </c>
@@ -2211,7 +2215,7 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:22" ht="14.4">
+    <row r="16" spans="1:22" ht="15">
       <c r="A16" s="25" t="s">
         <v>23</v>
       </c>
@@ -2241,7 +2245,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
     </row>
-    <row r="17" spans="1:22" ht="14.4">
+    <row r="17" spans="1:22" ht="15">
       <c r="A17" s="25" t="s">
         <v>24</v>
       </c>
@@ -2271,7 +2275,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
     </row>
-    <row r="18" spans="1:22" ht="14.4">
+    <row r="18" spans="1:22" ht="15">
       <c r="A18" s="25" t="s">
         <v>25</v>
       </c>
@@ -2301,7 +2305,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
     </row>
-    <row r="19" spans="1:22" ht="14.4">
+    <row r="19" spans="1:22" ht="15">
       <c r="A19" s="25" t="s">
         <v>26</v>
       </c>
@@ -2331,7 +2335,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
     </row>
-    <row r="20" spans="1:22" ht="14.4">
+    <row r="20" spans="1:22" ht="15">
       <c r="A20" s="25" t="s">
         <v>27</v>
       </c>
@@ -2361,7 +2365,7 @@
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
     </row>
-    <row r="21" spans="1:22" ht="14.4">
+    <row r="21" spans="1:22" ht="15">
       <c r="A21" s="25" t="s">
         <v>28</v>
       </c>
@@ -2391,7 +2395,7 @@
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
     </row>
-    <row r="22" spans="1:22" ht="14.4">
+    <row r="22" spans="1:22" ht="15">
       <c r="A22" s="25" t="s">
         <v>29</v>
       </c>
@@ -2421,7 +2425,7 @@
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
     </row>
-    <row r="23" spans="1:22" ht="14.4">
+    <row r="23" spans="1:22" ht="15">
       <c r="A23" s="25" t="s">
         <v>30</v>
       </c>
@@ -2451,7 +2455,7 @@
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22" ht="14.4">
+    <row r="24" spans="1:22" ht="15">
       <c r="A24" s="25" t="s">
         <v>31</v>
       </c>
@@ -2481,7 +2485,7 @@
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
     </row>
-    <row r="25" spans="1:22" ht="14.4">
+    <row r="25" spans="1:22" ht="15">
       <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
@@ -2511,7 +2515,7 @@
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
     </row>
-    <row r="26" spans="1:22" ht="14.4">
+    <row r="26" spans="1:22" ht="15">
       <c r="A26" s="25" t="s">
         <v>33</v>
       </c>
@@ -2541,7 +2545,7 @@
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
     </row>
-    <row r="27" spans="1:22" ht="14.4">
+    <row r="27" spans="1:22" ht="15">
       <c r="A27" s="25" t="s">
         <v>34</v>
       </c>
@@ -2571,7 +2575,7 @@
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
     </row>
-    <row r="28" spans="1:22" ht="14.4">
+    <row r="28" spans="1:22" ht="15">
       <c r="A28" s="25" t="s">
         <v>35</v>
       </c>
@@ -2601,7 +2605,7 @@
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
     </row>
-    <row r="29" spans="1:22" ht="14.4">
+    <row r="29" spans="1:22" ht="15">
       <c r="A29" s="25" t="s">
         <v>36</v>
       </c>
@@ -2631,7 +2635,7 @@
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
     </row>
-    <row r="30" spans="1:22" ht="14.4">
+    <row r="30" spans="1:22" ht="15">
       <c r="A30" s="25" t="s">
         <v>37</v>
       </c>
@@ -2661,7 +2665,7 @@
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
     </row>
-    <row r="31" spans="1:22" ht="14.4">
+    <row r="31" spans="1:22" ht="15">
       <c r="A31" s="25" t="s">
         <v>38</v>
       </c>
@@ -2691,7 +2695,7 @@
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
     </row>
-    <row r="32" spans="1:22" ht="14.4">
+    <row r="32" spans="1:22" ht="15">
       <c r="A32" s="25" t="s">
         <v>39</v>
       </c>
@@ -2721,7 +2725,7 @@
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
     </row>
-    <row r="33" spans="1:22" ht="14.4">
+    <row r="33" spans="1:22" ht="15">
       <c r="A33" s="25" t="s">
         <v>40</v>
       </c>
@@ -2751,7 +2755,7 @@
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
     </row>
-    <row r="34" spans="1:22" ht="14.4">
+    <row r="34" spans="1:22" ht="15">
       <c r="A34" s="25" t="s">
         <v>41</v>
       </c>
@@ -2781,7 +2785,7 @@
       <c r="U34" s="2"/>
       <c r="V34" s="2"/>
     </row>
-    <row r="35" spans="1:22" ht="14.4">
+    <row r="35" spans="1:22" ht="15">
       <c r="A35" s="25" t="s">
         <v>42</v>
       </c>
@@ -2811,7 +2815,7 @@
       <c r="U35" s="2"/>
       <c r="V35" s="2"/>
     </row>
-    <row r="36" spans="1:22" ht="14.4">
+    <row r="36" spans="1:22" ht="15">
       <c r="A36" s="25" t="s">
         <v>43</v>
       </c>
@@ -2841,7 +2845,7 @@
       <c r="U36" s="2"/>
       <c r="V36" s="2"/>
     </row>
-    <row r="37" spans="1:22" ht="14.4">
+    <row r="37" spans="1:22" ht="15">
       <c r="A37" s="25" t="s">
         <v>44</v>
       </c>
@@ -2871,7 +2875,7 @@
       <c r="U37" s="2"/>
       <c r="V37" s="2"/>
     </row>
-    <row r="38" spans="1:22" ht="14.4">
+    <row r="38" spans="1:22" ht="15">
       <c r="A38" s="25" t="s">
         <v>45</v>
       </c>
@@ -2901,7 +2905,7 @@
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
     </row>
-    <row r="39" spans="1:22" ht="14.4">
+    <row r="39" spans="1:22" ht="15">
       <c r="A39" s="25" t="s">
         <v>46</v>
       </c>
@@ -2931,7 +2935,7 @@
       <c r="U39" s="2"/>
       <c r="V39" s="2"/>
     </row>
-    <row r="40" spans="1:22" ht="14.4">
+    <row r="40" spans="1:22" ht="15">
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
@@ -2961,7 +2965,7 @@
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="1:22" ht="14.4">
+    <row r="41" spans="1:22" ht="15">
       <c r="A41" s="25" t="s">
         <v>48</v>
       </c>
@@ -2991,7 +2995,7 @@
       <c r="U41" s="2"/>
       <c r="V41" s="2"/>
     </row>
-    <row r="42" spans="1:22" ht="14.4">
+    <row r="42" spans="1:22" ht="15">
       <c r="A42" s="25" t="s">
         <v>49</v>
       </c>
@@ -3021,7 +3025,7 @@
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:22" ht="14.4">
+    <row r="43" spans="1:22" ht="15">
       <c r="A43" s="25" t="s">
         <v>50</v>
       </c>
@@ -3051,7 +3055,7 @@
       <c r="U43" s="2"/>
       <c r="V43" s="2"/>
     </row>
-    <row r="44" spans="1:22" ht="14.4">
+    <row r="44" spans="1:22" ht="15">
       <c r="A44" s="25" t="s">
         <v>51</v>
       </c>
@@ -3081,7 +3085,7 @@
       <c r="U44" s="2"/>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:22" ht="14.4">
+    <row r="45" spans="1:22" ht="15">
       <c r="A45" s="25" t="s">
         <v>52</v>
       </c>
@@ -3111,7 +3115,7 @@
       <c r="U45" s="2"/>
       <c r="V45" s="2"/>
     </row>
-    <row r="46" spans="1:22" ht="14.4">
+    <row r="46" spans="1:22" ht="15">
       <c r="A46" s="25" t="s">
         <v>53</v>
       </c>
@@ -3141,7 +3145,7 @@
       <c r="U46" s="2"/>
       <c r="V46" s="2"/>
     </row>
-    <row r="47" spans="1:22" ht="14.4">
+    <row r="47" spans="1:22" ht="15">
       <c r="A47" s="25" t="s">
         <v>54</v>
       </c>
@@ -3171,7 +3175,7 @@
       <c r="U47" s="2"/>
       <c r="V47" s="2"/>
     </row>
-    <row r="48" spans="1:22" ht="14.4">
+    <row r="48" spans="1:22" ht="15">
       <c r="A48" s="25" t="s">
         <v>55</v>
       </c>
@@ -3201,7 +3205,7 @@
       <c r="U48" s="2"/>
       <c r="V48" s="2"/>
     </row>
-    <row r="49" spans="1:22" ht="14.4">
+    <row r="49" spans="1:22" ht="15">
       <c r="A49" s="25" t="s">
         <v>56</v>
       </c>
@@ -3231,7 +3235,7 @@
       <c r="U49" s="2"/>
       <c r="V49" s="2"/>
     </row>
-    <row r="50" spans="1:22" ht="14.4">
+    <row r="50" spans="1:22" ht="15">
       <c r="A50" s="25" t="s">
         <v>57</v>
       </c>
@@ -3261,7 +3265,7 @@
       <c r="U50" s="2"/>
       <c r="V50" s="2"/>
     </row>
-    <row r="51" spans="1:22" ht="14.4">
+    <row r="51" spans="1:22" ht="15">
       <c r="A51" s="25" t="s">
         <v>58</v>
       </c>
@@ -3291,7 +3295,7 @@
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
     </row>
-    <row r="52" spans="1:22" ht="14.4">
+    <row r="52" spans="1:22" ht="15">
       <c r="A52" s="25" t="s">
         <v>59</v>
       </c>
@@ -3321,7 +3325,7 @@
       <c r="U52" s="2"/>
       <c r="V52" s="2"/>
     </row>
-    <row r="53" spans="1:22" ht="14.4">
+    <row r="53" spans="1:22" ht="15">
       <c r="A53" s="25" t="s">
         <v>60</v>
       </c>
@@ -3351,7 +3355,7 @@
       <c r="U53" s="2"/>
       <c r="V53" s="2"/>
     </row>
-    <row r="54" spans="1:22" ht="14.4">
+    <row r="54" spans="1:22" ht="15">
       <c r="A54" s="25" t="s">
         <v>61</v>
       </c>
@@ -3381,7 +3385,7 @@
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
     </row>
-    <row r="55" spans="1:22" ht="14.4">
+    <row r="55" spans="1:22" ht="15">
       <c r="A55" s="25" t="s">
         <v>62</v>
       </c>
@@ -3411,7 +3415,7 @@
       <c r="U55" s="2"/>
       <c r="V55" s="2"/>
     </row>
-    <row r="56" spans="1:22" ht="14.4">
+    <row r="56" spans="1:22" ht="15">
       <c r="A56" s="25" t="s">
         <v>63</v>
       </c>
@@ -3441,7 +3445,7 @@
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
     </row>
-    <row r="57" spans="1:22" ht="14.4">
+    <row r="57" spans="1:22" ht="15">
       <c r="A57" s="25" t="s">
         <v>64</v>
       </c>
@@ -3471,7 +3475,7 @@
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
     </row>
-    <row r="58" spans="1:22" ht="14.4">
+    <row r="58" spans="1:22" ht="15">
       <c r="A58" s="25" t="s">
         <v>65</v>
       </c>
@@ -3501,7 +3505,7 @@
       <c r="U58" s="2"/>
       <c r="V58" s="2"/>
     </row>
-    <row r="59" spans="1:22" ht="14.4">
+    <row r="59" spans="1:22" ht="15">
       <c r="A59" s="25" t="s">
         <v>66</v>
       </c>
@@ -3531,7 +3535,7 @@
       <c r="U59" s="2"/>
       <c r="V59" s="2"/>
     </row>
-    <row r="60" spans="1:22" ht="14.4">
+    <row r="60" spans="1:22" ht="15">
       <c r="A60" s="25" t="s">
         <v>67</v>
       </c>
@@ -3561,7 +3565,7 @@
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
     </row>
-    <row r="61" spans="1:22" ht="14.4">
+    <row r="61" spans="1:22" ht="15">
       <c r="A61" s="25" t="s">
         <v>68</v>
       </c>
@@ -3591,7 +3595,7 @@
       <c r="U61" s="2"/>
       <c r="V61" s="2"/>
     </row>
-    <row r="62" spans="1:22" ht="14.4">
+    <row r="62" spans="1:22" ht="15">
       <c r="A62" s="25" t="s">
         <v>69</v>
       </c>
@@ -3621,7 +3625,7 @@
       <c r="U62" s="2"/>
       <c r="V62" s="2"/>
     </row>
-    <row r="63" spans="1:22" ht="14.4">
+    <row r="63" spans="1:22" ht="15">
       <c r="A63" s="25" t="s">
         <v>70</v>
       </c>
@@ -3651,7 +3655,7 @@
       <c r="U63" s="2"/>
       <c r="V63" s="2"/>
     </row>
-    <row r="64" spans="1:22" ht="14.4">
+    <row r="64" spans="1:22" ht="15">
       <c r="A64" s="25" t="s">
         <v>71</v>
       </c>
@@ -3681,7 +3685,7 @@
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
     </row>
-    <row r="65" spans="1:22" ht="14.4">
+    <row r="65" spans="1:22" ht="15">
       <c r="A65" s="25" t="s">
         <v>72</v>
       </c>
@@ -3711,7 +3715,7 @@
       <c r="U65" s="2"/>
       <c r="V65" s="2"/>
     </row>
-    <row r="66" spans="1:22" ht="14.4">
+    <row r="66" spans="1:22" ht="15">
       <c r="A66" s="25" t="s">
         <v>73</v>
       </c>
@@ -3741,7 +3745,7 @@
       <c r="U66" s="2"/>
       <c r="V66" s="2"/>
     </row>
-    <row r="67" spans="1:22" ht="14.4">
+    <row r="67" spans="1:22" ht="15">
       <c r="A67" s="25" t="s">
         <v>74</v>
       </c>
@@ -3771,7 +3775,7 @@
       <c r="U67" s="2"/>
       <c r="V67" s="2"/>
     </row>
-    <row r="68" spans="1:22" ht="14.4">
+    <row r="68" spans="1:22" ht="15">
       <c r="A68" s="25" t="s">
         <v>75</v>
       </c>
@@ -3801,7 +3805,7 @@
       <c r="U68" s="2"/>
       <c r="V68" s="2"/>
     </row>
-    <row r="69" spans="1:22" ht="14.4">
+    <row r="69" spans="1:22" ht="15">
       <c r="A69" s="25" t="s">
         <v>76</v>
       </c>
@@ -3831,7 +3835,7 @@
       <c r="U69" s="2"/>
       <c r="V69" s="2"/>
     </row>
-    <row r="70" spans="1:22" ht="14.4">
+    <row r="70" spans="1:22" ht="15">
       <c r="A70" s="25" t="s">
         <v>77</v>
       </c>
@@ -3861,7 +3865,7 @@
       <c r="U70" s="2"/>
       <c r="V70" s="2"/>
     </row>
-    <row r="71" spans="1:22" ht="14.4">
+    <row r="71" spans="1:22" ht="15">
       <c r="A71" s="25" t="s">
         <v>78</v>
       </c>
@@ -3891,7 +3895,7 @@
       <c r="U71" s="2"/>
       <c r="V71" s="2"/>
     </row>
-    <row r="72" spans="1:22" ht="14.4">
+    <row r="72" spans="1:22" ht="15">
       <c r="A72" s="25" t="s">
         <v>79</v>
       </c>
@@ -3921,7 +3925,7 @@
       <c r="U72" s="2"/>
       <c r="V72" s="2"/>
     </row>
-    <row r="73" spans="1:22" ht="14.4">
+    <row r="73" spans="1:22" ht="15">
       <c r="A73" s="25" t="s">
         <v>80</v>
       </c>
@@ -3951,7 +3955,7 @@
       <c r="U73" s="2"/>
       <c r="V73" s="2"/>
     </row>
-    <row r="74" spans="1:22" ht="14.4">
+    <row r="74" spans="1:22" ht="15">
       <c r="A74" s="25" t="s">
         <v>81</v>
       </c>
@@ -3981,7 +3985,7 @@
       <c r="U74" s="2"/>
       <c r="V74" s="2"/>
     </row>
-    <row r="75" spans="1:22" ht="14.4">
+    <row r="75" spans="1:22" ht="15">
       <c r="A75" s="25" t="s">
         <v>82</v>
       </c>
@@ -4011,7 +4015,7 @@
       <c r="U75" s="2"/>
       <c r="V75" s="2"/>
     </row>
-    <row r="76" spans="1:22" ht="14.4">
+    <row r="76" spans="1:22" ht="15">
       <c r="A76" s="25" t="s">
         <v>83</v>
       </c>
@@ -4041,7 +4045,7 @@
       <c r="U76" s="2"/>
       <c r="V76" s="2"/>
     </row>
-    <row r="77" spans="1:22" ht="14.4">
+    <row r="77" spans="1:22" ht="15">
       <c r="A77" s="25" t="s">
         <v>84</v>
       </c>
@@ -4071,7 +4075,7 @@
       <c r="U77" s="2"/>
       <c r="V77" s="2"/>
     </row>
-    <row r="78" spans="1:22" ht="14.4">
+    <row r="78" spans="1:22" ht="15">
       <c r="A78" s="25" t="s">
         <v>85</v>
       </c>
@@ -4101,7 +4105,7 @@
       <c r="U78" s="2"/>
       <c r="V78" s="2"/>
     </row>
-    <row r="79" spans="1:22" ht="14.4">
+    <row r="79" spans="1:22" ht="15">
       <c r="A79" s="25" t="s">
         <v>86</v>
       </c>
@@ -4131,7 +4135,7 @@
       <c r="U79" s="2"/>
       <c r="V79" s="2"/>
     </row>
-    <row r="80" spans="1:22" ht="14.4">
+    <row r="80" spans="1:22" ht="15">
       <c r="A80" s="25" t="s">
         <v>87</v>
       </c>
@@ -4161,7 +4165,7 @@
       <c r="U80" s="2"/>
       <c r="V80" s="2"/>
     </row>
-    <row r="81" spans="1:22" ht="14.4">
+    <row r="81" spans="1:22" ht="15">
       <c r="A81" s="25" t="s">
         <v>88</v>
       </c>
@@ -4191,7 +4195,7 @@
       <c r="U81" s="2"/>
       <c r="V81" s="2"/>
     </row>
-    <row r="82" spans="1:22" ht="14.4">
+    <row r="82" spans="1:22" ht="15">
       <c r="A82" s="25" t="s">
         <v>89</v>
       </c>
@@ -4221,7 +4225,7 @@
       <c r="U82" s="2"/>
       <c r="V82" s="2"/>
     </row>
-    <row r="83" spans="1:22" ht="14.4">
+    <row r="83" spans="1:22" ht="15">
       <c r="A83" s="25" t="s">
         <v>90</v>
       </c>
@@ -4251,7 +4255,7 @@
       <c r="U83" s="2"/>
       <c r="V83" s="2"/>
     </row>
-    <row r="84" spans="1:22" ht="14.4">
+    <row r="84" spans="1:22" ht="15">
       <c r="A84" s="25" t="s">
         <v>91</v>
       </c>
@@ -4281,7 +4285,7 @@
       <c r="U84" s="2"/>
       <c r="V84" s="2"/>
     </row>
-    <row r="85" spans="1:22" ht="14.4">
+    <row r="85" spans="1:22" ht="15">
       <c r="A85" s="25" t="s">
         <v>92</v>
       </c>
@@ -4311,7 +4315,7 @@
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
     </row>
-    <row r="86" spans="1:22" ht="14.4">
+    <row r="86" spans="1:22" ht="15">
       <c r="A86" s="25" t="s">
         <v>93</v>
       </c>
@@ -4341,7 +4345,7 @@
       <c r="U86" s="2"/>
       <c r="V86" s="2"/>
     </row>
-    <row r="87" spans="1:22" ht="14.4">
+    <row r="87" spans="1:22" ht="15">
       <c r="A87" s="25" t="s">
         <v>94</v>
       </c>
@@ -4371,7 +4375,7 @@
       <c r="U87" s="2"/>
       <c r="V87" s="2"/>
     </row>
-    <row r="88" spans="1:22" ht="14.4">
+    <row r="88" spans="1:22" ht="15">
       <c r="A88" s="25" t="s">
         <v>95</v>
       </c>
@@ -4401,7 +4405,7 @@
       <c r="U88" s="2"/>
       <c r="V88" s="2"/>
     </row>
-    <row r="89" spans="1:22" ht="14.4">
+    <row r="89" spans="1:22" ht="15">
       <c r="A89" s="25" t="s">
         <v>96</v>
       </c>
@@ -4431,7 +4435,7 @@
       <c r="U89" s="2"/>
       <c r="V89" s="2"/>
     </row>
-    <row r="90" spans="1:22" ht="14.4">
+    <row r="90" spans="1:22" ht="15">
       <c r="A90" s="25" t="s">
         <v>97</v>
       </c>
@@ -4461,7 +4465,7 @@
       <c r="U90" s="2"/>
       <c r="V90" s="2"/>
     </row>
-    <row r="91" spans="1:22" ht="14.4">
+    <row r="91" spans="1:22" ht="15">
       <c r="A91" s="25" t="s">
         <v>98</v>
       </c>
@@ -4491,7 +4495,7 @@
       <c r="U91" s="2"/>
       <c r="V91" s="2"/>
     </row>
-    <row r="92" spans="1:22" ht="14.4">
+    <row r="92" spans="1:22" ht="15">
       <c r="A92" s="25" t="s">
         <v>99</v>
       </c>
@@ -4525,7 +4529,7 @@
       <c r="U92" s="2"/>
       <c r="V92" s="2"/>
     </row>
-    <row r="93" spans="1:22" ht="14.4">
+    <row r="93" spans="1:22" ht="15">
       <c r="A93" s="25" t="s">
         <v>100</v>
       </c>
@@ -4555,7 +4559,7 @@
       <c r="U93" s="2"/>
       <c r="V93" s="2"/>
     </row>
-    <row r="94" spans="1:22" ht="14.4">
+    <row r="94" spans="1:22" ht="15">
       <c r="A94" s="25" t="s">
         <v>101</v>
       </c>
@@ -4585,7 +4589,7 @@
       <c r="U94" s="2"/>
       <c r="V94" s="2"/>
     </row>
-    <row r="95" spans="1:22" ht="14.4">
+    <row r="95" spans="1:22" ht="15">
       <c r="A95" s="25" t="s">
         <v>102</v>
       </c>
@@ -4615,7 +4619,7 @@
       <c r="U95" s="2"/>
       <c r="V95" s="2"/>
     </row>
-    <row r="96" spans="1:22" ht="14.4">
+    <row r="96" spans="1:22" ht="15">
       <c r="A96" s="25" t="s">
         <v>103</v>
       </c>
@@ -4645,7 +4649,7 @@
       <c r="U96" s="2"/>
       <c r="V96" s="2"/>
     </row>
-    <row r="97" spans="1:22" ht="14.4">
+    <row r="97" spans="1:22" ht="15">
       <c r="A97" s="25" t="s">
         <v>104</v>
       </c>
@@ -4675,7 +4679,7 @@
       <c r="U97" s="2"/>
       <c r="V97" s="2"/>
     </row>
-    <row r="98" spans="1:22" ht="14.4">
+    <row r="98" spans="1:22" ht="15">
       <c r="A98" s="25" t="s">
         <v>105</v>
       </c>
@@ -4705,7 +4709,7 @@
       <c r="U98" s="2"/>
       <c r="V98" s="2"/>
     </row>
-    <row r="99" spans="1:22" ht="14.4">
+    <row r="99" spans="1:22" ht="15">
       <c r="A99" s="25" t="s">
         <v>106</v>
       </c>
@@ -4735,7 +4739,7 @@
       <c r="U99" s="2"/>
       <c r="V99" s="2"/>
     </row>
-    <row r="100" spans="1:22" ht="14.4">
+    <row r="100" spans="1:22" ht="15">
       <c r="A100" s="25" t="s">
         <v>107</v>
       </c>
@@ -4765,33 +4769,33 @@
       <c r="U100" s="2"/>
       <c r="V100" s="2"/>
     </row>
-    <row r="101" spans="1:22" ht="14.4">
+    <row r="101" spans="1:22" ht="15">
       <c r="A101" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B101" s="49" t="s">
+      <c r="B101" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C101" s="49" t="s">
+      <c r="C101" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D101" s="44">
+      <c r="D101" s="36">
         <v>82792580</v>
       </c>
-      <c r="E101" s="44">
+      <c r="E101" s="36">
         <v>82811159</v>
       </c>
-      <c r="F101" s="45" t="s">
+      <c r="F101" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G101" s="45" t="s">
+      <c r="G101" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H101" s="45" t="s">
+      <c r="H101" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="I101" s="46" t="s">
-        <v>286</v>
+      <c r="I101" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
@@ -4807,15 +4811,15 @@
       <c r="U101" s="2"/>
       <c r="V101" s="2"/>
     </row>
-    <row r="102" spans="1:22" ht="14.4">
+    <row r="102" spans="1:22" ht="15">
       <c r="A102" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B102" s="48" t="s">
+      <c r="B102" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="C102" s="48" t="s">
-        <v>287</v>
+      <c r="C102" s="40" t="s">
+        <v>273</v>
       </c>
       <c r="D102" s="5">
         <v>82810850</v>
@@ -4824,14 +4828,14 @@
         <v>82893600</v>
       </c>
       <c r="F102" s="29" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="G102" s="11"/>
       <c r="H102" s="11">
         <v>12</v>
       </c>
-      <c r="I102" s="46" t="s">
-        <v>286</v>
+      <c r="I102" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J102" s="2"/>
       <c r="K102" s="2"/>
@@ -4847,7 +4851,7 @@
       <c r="U102" s="2"/>
       <c r="V102" s="2"/>
     </row>
-    <row r="103" spans="1:22" ht="14.4">
+    <row r="103" spans="1:22" ht="15">
       <c r="A103" s="28" t="s">
         <v>110</v>
       </c>
@@ -4862,8 +4866,8 @@
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
-      <c r="I103" s="46" t="s">
-        <v>286</v>
+      <c r="I103" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
@@ -4879,15 +4883,15 @@
       <c r="U103" s="2"/>
       <c r="V103" s="2"/>
     </row>
-    <row r="104" spans="1:22" ht="16.8">
+    <row r="104" spans="1:22" ht="16.5">
       <c r="A104" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B104" s="50" t="s">
+      <c r="B104" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="C104" s="47" t="s">
-        <v>289</v>
+      <c r="C104" s="39" t="s">
+        <v>275</v>
       </c>
       <c r="D104" s="5">
         <v>82931563</v>
@@ -4896,14 +4900,14 @@
         <v>82985019</v>
       </c>
       <c r="F104" s="29" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="G104" s="11"/>
       <c r="H104" s="11">
         <v>0</v>
       </c>
-      <c r="I104" s="46" t="s">
-        <v>286</v>
+      <c r="I104" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J104" s="2"/>
       <c r="K104" s="2"/>
@@ -4919,15 +4923,15 @@
       <c r="U104" s="2"/>
       <c r="V104" s="2"/>
     </row>
-    <row r="105" spans="1:22" ht="14.4">
+    <row r="105" spans="1:22" ht="15">
       <c r="A105" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B105" s="47" t="s">
+      <c r="B105" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="C105" s="47" t="s">
-        <v>291</v>
+      <c r="C105" s="39" t="s">
+        <v>277</v>
       </c>
       <c r="D105" s="5">
         <v>82988294</v>
@@ -4936,14 +4940,14 @@
         <v>82995755</v>
       </c>
       <c r="F105" s="29" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="G105" s="11"/>
       <c r="H105" s="11">
         <v>3</v>
       </c>
-      <c r="I105" s="46" t="s">
-        <v>286</v>
+      <c r="I105" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
@@ -4959,15 +4963,15 @@
       <c r="U105" s="2"/>
       <c r="V105" s="2"/>
     </row>
-    <row r="106" spans="1:22" ht="14.4">
+    <row r="106" spans="1:22" ht="15">
       <c r="A106" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B106" s="47" t="s">
+      <c r="B106" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="C106" s="47" t="s">
-        <v>292</v>
+      <c r="C106" s="39" t="s">
+        <v>278</v>
       </c>
       <c r="D106" s="5">
         <v>82997831</v>
@@ -4976,14 +4980,14 @@
         <v>83104794</v>
       </c>
       <c r="F106" s="29" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="G106" s="11"/>
       <c r="H106" s="11">
         <v>3</v>
       </c>
-      <c r="I106" s="46" t="s">
-        <v>286</v>
+      <c r="I106" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
@@ -4999,7 +5003,7 @@
       <c r="U106" s="2"/>
       <c r="V106" s="2"/>
     </row>
-    <row r="107" spans="1:22" ht="14.4">
+    <row r="107" spans="1:22" ht="15">
       <c r="A107" s="28" t="s">
         <v>114</v>
       </c>
@@ -5014,8 +5018,8 @@
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
-      <c r="I107" s="46" t="s">
-        <v>286</v>
+      <c r="I107" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
@@ -5031,15 +5035,15 @@
       <c r="U107" s="2"/>
       <c r="V107" s="2"/>
     </row>
-    <row r="108" spans="1:22" ht="14.4">
+    <row r="108" spans="1:22" ht="15">
       <c r="A108" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="B108" s="47" t="s">
+      <c r="B108" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="C108" s="47" t="s">
-        <v>293</v>
+      <c r="C108" s="39" t="s">
+        <v>279</v>
       </c>
       <c r="D108" s="5">
         <v>83132206</v>
@@ -5048,14 +5052,14 @@
         <v>83168823</v>
       </c>
       <c r="F108" s="29" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="G108" s="11"/>
       <c r="H108" s="11">
         <v>3</v>
       </c>
-      <c r="I108" s="46" t="s">
-        <v>286</v>
+      <c r="I108" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
@@ -5071,7 +5075,7 @@
       <c r="U108" s="2"/>
       <c r="V108" s="2"/>
     </row>
-    <row r="109" spans="1:22" ht="14.4">
+    <row r="109" spans="1:22" ht="15">
       <c r="A109" s="28" t="s">
         <v>116</v>
       </c>
@@ -5086,8 +5090,8 @@
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
-      <c r="I109" s="46" t="s">
-        <v>286</v>
+      <c r="I109" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
@@ -5103,15 +5107,15 @@
       <c r="U109" s="2"/>
       <c r="V109" s="2"/>
     </row>
-    <row r="110" spans="1:22" ht="14.4">
+    <row r="110" spans="1:22" ht="15">
       <c r="A110" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B110" s="47" t="s">
+      <c r="B110" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="C110" s="47" t="s">
-        <v>297</v>
+      <c r="C110" s="39" t="s">
+        <v>283</v>
       </c>
       <c r="D110" s="5">
         <v>83232769</v>
@@ -5120,14 +5124,14 @@
         <v>83289469</v>
       </c>
       <c r="F110" s="29" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11">
         <v>0</v>
       </c>
-      <c r="I110" s="46" t="s">
-        <v>286</v>
+      <c r="I110" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
@@ -5143,7 +5147,7 @@
       <c r="U110" s="2"/>
       <c r="V110" s="2"/>
     </row>
-    <row r="111" spans="1:22" ht="14.4">
+    <row r="111" spans="1:22" ht="15">
       <c r="A111" s="28" t="s">
         <v>118</v>
       </c>
@@ -5158,8 +5162,8 @@
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="46" t="s">
-        <v>286</v>
+      <c r="I111" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
@@ -5175,15 +5179,15 @@
       <c r="U111" s="2"/>
       <c r="V111" s="2"/>
     </row>
-    <row r="112" spans="1:22" ht="14.4">
+    <row r="112" spans="1:22" ht="15">
       <c r="A112" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="B112" s="47" t="s">
+      <c r="B112" s="39" t="s">
         <v>222</v>
       </c>
-      <c r="C112" s="47" t="s">
-        <v>299</v>
+      <c r="C112" s="39" t="s">
+        <v>285</v>
       </c>
       <c r="D112" s="5">
         <v>83333199</v>
@@ -5192,12 +5196,12 @@
         <v>83613814</v>
       </c>
       <c r="F112" s="29" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="G112" s="11"/>
       <c r="H112" s="11"/>
-      <c r="I112" s="46" t="s">
-        <v>286</v>
+      <c r="I112" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
@@ -5213,7 +5217,7 @@
       <c r="U112" s="2"/>
       <c r="V112" s="2"/>
     </row>
-    <row r="113" spans="1:22" ht="14.4">
+    <row r="113" spans="1:22" ht="15">
       <c r="A113" s="28" t="s">
         <v>120</v>
       </c>
@@ -5228,8 +5232,8 @@
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="46" t="s">
-        <v>286</v>
+      <c r="I113" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
@@ -5245,7 +5249,7 @@
       <c r="U113" s="2"/>
       <c r="V113" s="2"/>
     </row>
-    <row r="114" spans="1:22" ht="14.4">
+    <row r="114" spans="1:22" ht="15">
       <c r="A114" s="28" t="s">
         <v>121</v>
       </c>
@@ -5260,8 +5264,8 @@
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
-      <c r="I114" s="46" t="s">
-        <v>286</v>
+      <c r="I114" s="38" t="s">
+        <v>272</v>
       </c>
       <c r="J114" s="2"/>
       <c r="K114" s="2"/>
@@ -5277,7 +5281,7 @@
       <c r="U114" s="2"/>
       <c r="V114" s="2"/>
     </row>
-    <row r="115" spans="1:22" ht="14.4">
+    <row r="115" spans="1:22" ht="15">
       <c r="A115" s="25" t="s">
         <v>122</v>
       </c>
@@ -5307,7 +5311,7 @@
       <c r="U115" s="2"/>
       <c r="V115" s="2"/>
     </row>
-    <row r="116" spans="1:22" ht="14.4">
+    <row r="116" spans="1:22" ht="15">
       <c r="A116" s="25" t="s">
         <v>123</v>
       </c>
@@ -5337,7 +5341,7 @@
       <c r="U116" s="2"/>
       <c r="V116" s="2"/>
     </row>
-    <row r="117" spans="1:22" ht="14.4">
+    <row r="117" spans="1:22" ht="15">
       <c r="A117" s="25" t="s">
         <v>124</v>
       </c>
@@ -5367,7 +5371,7 @@
       <c r="U117" s="2"/>
       <c r="V117" s="2"/>
     </row>
-    <row r="118" spans="1:22" ht="14.4">
+    <row r="118" spans="1:22" ht="15">
       <c r="A118" s="25" t="s">
         <v>125</v>
       </c>
@@ -5397,7 +5401,7 @@
       <c r="U118" s="2"/>
       <c r="V118" s="2"/>
     </row>
-    <row r="119" spans="1:22" ht="14.4">
+    <row r="119" spans="1:22" ht="15">
       <c r="A119" s="25" t="s">
         <v>126</v>
       </c>
@@ -5427,7 +5431,7 @@
       <c r="U119" s="2"/>
       <c r="V119" s="2"/>
     </row>
-    <row r="120" spans="1:22" ht="14.4">
+    <row r="120" spans="1:22" ht="15">
       <c r="A120" s="25" t="s">
         <v>127</v>
       </c>
@@ -5457,7 +5461,7 @@
       <c r="U120" s="2"/>
       <c r="V120" s="2"/>
     </row>
-    <row r="121" spans="1:22" ht="14.4">
+    <row r="121" spans="1:22" ht="15">
       <c r="A121" s="25" t="s">
         <v>10</v>
       </c>
@@ -5487,7 +5491,7 @@
       <c r="U121" s="2"/>
       <c r="V121" s="2"/>
     </row>
-    <row r="122" spans="1:22" ht="14.4">
+    <row r="122" spans="1:22" ht="15">
       <c r="A122" s="25" t="s">
         <v>128</v>
       </c>
@@ -5517,7 +5521,7 @@
       <c r="U122" s="2"/>
       <c r="V122" s="2"/>
     </row>
-    <row r="123" spans="1:22" ht="14.4">
+    <row r="123" spans="1:22" ht="15">
       <c r="A123" s="25" t="s">
         <v>129</v>
       </c>
@@ -5547,7 +5551,7 @@
       <c r="U123" s="2"/>
       <c r="V123" s="2"/>
     </row>
-    <row r="124" spans="1:22" ht="14.4">
+    <row r="124" spans="1:22" ht="15">
       <c r="A124" s="25" t="s">
         <v>130</v>
       </c>
@@ -5577,7 +5581,7 @@
       <c r="U124" s="2"/>
       <c r="V124" s="2"/>
     </row>
-    <row r="125" spans="1:22" ht="14.4">
+    <row r="125" spans="1:22" ht="15">
       <c r="A125" s="25" t="s">
         <v>131</v>
       </c>
@@ -5607,7 +5611,7 @@
       <c r="U125" s="2"/>
       <c r="V125" s="2"/>
     </row>
-    <row r="126" spans="1:22" ht="14.4">
+    <row r="126" spans="1:22" ht="15">
       <c r="A126" s="25" t="s">
         <v>132</v>
       </c>
@@ -5637,7 +5641,7 @@
       <c r="U126" s="2"/>
       <c r="V126" s="2"/>
     </row>
-    <row r="127" spans="1:22" ht="14.4">
+    <row r="127" spans="1:22" ht="15">
       <c r="A127" s="25" t="s">
         <v>133</v>
       </c>
@@ -5667,7 +5671,7 @@
       <c r="U127" s="2"/>
       <c r="V127" s="2"/>
     </row>
-    <row r="128" spans="1:22" ht="14.4">
+    <row r="128" spans="1:22" ht="15">
       <c r="A128" s="25" t="s">
         <v>134</v>
       </c>
@@ -5697,7 +5701,7 @@
       <c r="U128" s="2"/>
       <c r="V128" s="2"/>
     </row>
-    <row r="129" spans="1:22" ht="14.4">
+    <row r="129" spans="1:22" ht="15">
       <c r="A129" s="25" t="s">
         <v>135</v>
       </c>
@@ -5727,7 +5731,7 @@
       <c r="U129" s="2"/>
       <c r="V129" s="2"/>
     </row>
-    <row r="130" spans="1:22" ht="14.4">
+    <row r="130" spans="1:22" ht="15">
       <c r="A130" s="25" t="s">
         <v>136</v>
       </c>
@@ -5757,7 +5761,7 @@
       <c r="U130" s="2"/>
       <c r="V130" s="2"/>
     </row>
-    <row r="131" spans="1:22" ht="14.4">
+    <row r="131" spans="1:22" ht="15">
       <c r="A131" s="25" t="s">
         <v>137</v>
       </c>
@@ -5787,7 +5791,7 @@
       <c r="U131" s="2"/>
       <c r="V131" s="2"/>
     </row>
-    <row r="132" spans="1:22" ht="14.4">
+    <row r="132" spans="1:22" ht="15">
       <c r="A132" s="25" t="s">
         <v>138</v>
       </c>
@@ -5817,7 +5821,7 @@
       <c r="U132" s="2"/>
       <c r="V132" s="2"/>
     </row>
-    <row r="133" spans="1:22" ht="14.4">
+    <row r="133" spans="1:22" ht="15">
       <c r="A133" s="25" t="s">
         <v>139</v>
       </c>
@@ -5847,7 +5851,7 @@
       <c r="U133" s="2"/>
       <c r="V133" s="2"/>
     </row>
-    <row r="134" spans="1:22" ht="14.4">
+    <row r="134" spans="1:22" ht="15">
       <c r="A134" s="25" t="s">
         <v>140</v>
       </c>
@@ -5877,7 +5881,7 @@
       <c r="U134" s="2"/>
       <c r="V134" s="2"/>
     </row>
-    <row r="135" spans="1:22" ht="14.4">
+    <row r="135" spans="1:22" ht="15">
       <c r="A135" s="25" t="s">
         <v>141</v>
       </c>
@@ -5907,7 +5911,7 @@
       <c r="U135" s="2"/>
       <c r="V135" s="2"/>
     </row>
-    <row r="136" spans="1:22" ht="14.4">
+    <row r="136" spans="1:22" ht="15">
       <c r="A136" s="25" t="s">
         <v>142</v>
       </c>
@@ -5937,7 +5941,7 @@
       <c r="U136" s="2"/>
       <c r="V136" s="2"/>
     </row>
-    <row r="137" spans="1:22" ht="14.4">
+    <row r="137" spans="1:22" ht="15">
       <c r="A137" s="25" t="s">
         <v>143</v>
       </c>
@@ -5967,7 +5971,7 @@
       <c r="U137" s="2"/>
       <c r="V137" s="2"/>
     </row>
-    <row r="138" spans="1:22" ht="14.4">
+    <row r="138" spans="1:22" ht="15">
       <c r="A138" s="25" t="s">
         <v>144</v>
       </c>
@@ -5997,7 +6001,7 @@
       <c r="U138" s="2"/>
       <c r="V138" s="2"/>
     </row>
-    <row r="139" spans="1:22" ht="14.4">
+    <row r="139" spans="1:22" ht="15">
       <c r="A139" s="25" t="s">
         <v>145</v>
       </c>
@@ -6027,7 +6031,7 @@
       <c r="U139" s="2"/>
       <c r="V139" s="2"/>
     </row>
-    <row r="140" spans="1:22" ht="14.4">
+    <row r="140" spans="1:22" ht="15">
       <c r="A140" s="25" t="s">
         <v>146</v>
       </c>
@@ -6057,7 +6061,7 @@
       <c r="U140" s="2"/>
       <c r="V140" s="2"/>
     </row>
-    <row r="141" spans="1:22" ht="14.4">
+    <row r="141" spans="1:22" ht="15">
       <c r="A141" s="25" t="s">
         <v>147</v>
       </c>
@@ -6087,7 +6091,7 @@
       <c r="U141" s="2"/>
       <c r="V141" s="2"/>
     </row>
-    <row r="142" spans="1:22" ht="14.4">
+    <row r="142" spans="1:22" ht="15">
       <c r="A142" s="25" t="s">
         <v>148</v>
       </c>
@@ -6117,7 +6121,7 @@
       <c r="U142" s="2"/>
       <c r="V142" s="2"/>
     </row>
-    <row r="143" spans="1:22" ht="14.4">
+    <row r="143" spans="1:22" ht="15">
       <c r="A143" s="25" t="s">
         <v>149</v>
       </c>
@@ -6147,7 +6151,7 @@
       <c r="U143" s="2"/>
       <c r="V143" s="2"/>
     </row>
-    <row r="144" spans="1:22" ht="14.4">
+    <row r="144" spans="1:22" ht="15">
       <c r="A144" s="25" t="s">
         <v>150</v>
       </c>
@@ -6177,7 +6181,7 @@
       <c r="U144" s="2"/>
       <c r="V144" s="2"/>
     </row>
-    <row r="145" spans="1:22" ht="14.4">
+    <row r="145" spans="1:22" ht="15">
       <c r="A145" s="25" t="s">
         <v>151</v>
       </c>
@@ -6207,7 +6211,7 @@
       <c r="U145" s="2"/>
       <c r="V145" s="2"/>
     </row>
-    <row r="146" spans="1:22" ht="14.4">
+    <row r="146" spans="1:22" ht="15">
       <c r="A146" s="25" t="s">
         <v>152</v>
       </c>
@@ -6237,7 +6241,7 @@
       <c r="U146" s="2"/>
       <c r="V146" s="2"/>
     </row>
-    <row r="147" spans="1:22" ht="14.4">
+    <row r="147" spans="1:22" ht="15">
       <c r="A147" s="25" t="s">
         <v>153</v>
       </c>
@@ -6267,7 +6271,7 @@
       <c r="U147" s="2"/>
       <c r="V147" s="2"/>
     </row>
-    <row r="148" spans="1:22" ht="14.4">
+    <row r="148" spans="1:22" ht="15">
       <c r="A148" s="25" t="s">
         <v>154</v>
       </c>
@@ -6297,7 +6301,7 @@
       <c r="U148" s="2"/>
       <c r="V148" s="2"/>
     </row>
-    <row r="149" spans="1:22" ht="14.4">
+    <row r="149" spans="1:22" ht="15">
       <c r="A149" s="25" t="s">
         <v>155</v>
       </c>
@@ -6327,7 +6331,7 @@
       <c r="U149" s="2"/>
       <c r="V149" s="2"/>
     </row>
-    <row r="150" spans="1:22" ht="15" thickBot="1">
+    <row r="150" spans="1:22" thickBot="1">
       <c r="A150" s="25" t="s">
         <v>156</v>
       </c>
@@ -6395,7 +6399,7 @@
       <c r="U151" s="2"/>
       <c r="V151" s="2"/>
     </row>
-    <row r="152" spans="1:22" ht="14.4">
+    <row r="152" spans="1:22" ht="15">
       <c r="A152" s="25" t="s">
         <v>158</v>
       </c>
@@ -6425,7 +6429,7 @@
       <c r="U152" s="2"/>
       <c r="V152" s="2"/>
     </row>
-    <row r="153" spans="1:22" ht="14.4">
+    <row r="153" spans="1:22" ht="15">
       <c r="A153" s="25" t="s">
         <v>159</v>
       </c>
@@ -6455,7 +6459,7 @@
       <c r="U153" s="2"/>
       <c r="V153" s="2"/>
     </row>
-    <row r="154" spans="1:22" ht="14.4">
+    <row r="154" spans="1:22" ht="15">
       <c r="A154" s="25" t="s">
         <v>160</v>
       </c>
@@ -6485,7 +6489,7 @@
       <c r="U154" s="2"/>
       <c r="V154" s="2"/>
     </row>
-    <row r="155" spans="1:22" ht="14.4">
+    <row r="155" spans="1:22" ht="15">
       <c r="A155" s="25" t="s">
         <v>161</v>
       </c>
@@ -6515,7 +6519,7 @@
       <c r="U155" s="2"/>
       <c r="V155" s="2"/>
     </row>
-    <row r="156" spans="1:22" ht="14.4">
+    <row r="156" spans="1:22" ht="15">
       <c r="A156" s="25" t="s">
         <v>162</v>
       </c>
@@ -6545,7 +6549,7 @@
       <c r="U156" s="2"/>
       <c r="V156" s="2"/>
     </row>
-    <row r="157" spans="1:22" ht="14.4">
+    <row r="157" spans="1:22" ht="15">
       <c r="A157" s="25" t="s">
         <v>163</v>
       </c>
@@ -6575,7 +6579,7 @@
       <c r="U157" s="2"/>
       <c r="V157" s="2"/>
     </row>
-    <row r="158" spans="1:22" ht="14.4">
+    <row r="158" spans="1:22" ht="15">
       <c r="A158" s="25" t="s">
         <v>164</v>
       </c>
@@ -6605,7 +6609,7 @@
       <c r="U158" s="2"/>
       <c r="V158" s="2"/>
     </row>
-    <row r="159" spans="1:22" ht="14.4">
+    <row r="159" spans="1:22" ht="15">
       <c r="A159" s="25" t="s">
         <v>165</v>
       </c>
@@ -6635,7 +6639,7 @@
       <c r="U159" s="2"/>
       <c r="V159" s="2"/>
     </row>
-    <row r="160" spans="1:22" ht="14.4">
+    <row r="160" spans="1:22" ht="15">
       <c r="A160" s="25" t="s">
         <v>166</v>
       </c>
@@ -6665,7 +6669,7 @@
       <c r="U160" s="2"/>
       <c r="V160" s="2"/>
     </row>
-    <row r="161" spans="1:22" ht="14.4">
+    <row r="161" spans="1:22" ht="15">
       <c r="A161" s="25" t="s">
         <v>167</v>
       </c>
@@ -6695,7 +6699,7 @@
       <c r="U161" s="2"/>
       <c r="V161" s="2"/>
     </row>
-    <row r="162" spans="1:22" ht="14.4">
+    <row r="162" spans="1:22" ht="15">
       <c r="A162" s="25" t="s">
         <v>168</v>
       </c>
@@ -6725,7 +6729,7 @@
       <c r="U162" s="2"/>
       <c r="V162" s="2"/>
     </row>
-    <row r="163" spans="1:22" ht="14.4">
+    <row r="163" spans="1:22" ht="15">
       <c r="A163" s="25" t="s">
         <v>169</v>
       </c>
@@ -6755,7 +6759,7 @@
       <c r="U163" s="2"/>
       <c r="V163" s="2"/>
     </row>
-    <row r="164" spans="1:22" ht="14.4">
+    <row r="164" spans="1:22" ht="15">
       <c r="A164" s="25" t="s">
         <v>170</v>
       </c>
@@ -6785,7 +6789,7 @@
       <c r="U164" s="2"/>
       <c r="V164" s="2"/>
     </row>
-    <row r="165" spans="1:22" ht="14.4">
+    <row r="165" spans="1:22" ht="15">
       <c r="A165" s="25" t="s">
         <v>171</v>
       </c>
@@ -6815,7 +6819,7 @@
       <c r="U165" s="2"/>
       <c r="V165" s="2"/>
     </row>
-    <row r="166" spans="1:22" ht="14.4">
+    <row r="166" spans="1:22" ht="15">
       <c r="A166" s="25" t="s">
         <v>172</v>
       </c>
@@ -6845,7 +6849,7 @@
       <c r="U166" s="2"/>
       <c r="V166" s="2"/>
     </row>
-    <row r="167" spans="1:22" ht="14.4">
+    <row r="167" spans="1:22" ht="15">
       <c r="A167" s="25" t="s">
         <v>173</v>
       </c>
@@ -6875,7 +6879,7 @@
       <c r="U167" s="2"/>
       <c r="V167" s="2"/>
     </row>
-    <row r="168" spans="1:22" ht="14.4">
+    <row r="168" spans="1:22" ht="15">
       <c r="A168" s="25" t="s">
         <v>174</v>
       </c>
@@ -6905,7 +6909,7 @@
       <c r="U168" s="2"/>
       <c r="V168" s="2"/>
     </row>
-    <row r="169" spans="1:22" ht="14.4">
+    <row r="169" spans="1:22" ht="15">
       <c r="A169" s="25" t="s">
         <v>175</v>
       </c>
@@ -6935,7 +6939,7 @@
       <c r="U169" s="2"/>
       <c r="V169" s="2"/>
     </row>
-    <row r="170" spans="1:22" ht="14.4">
+    <row r="170" spans="1:22" ht="15">
       <c r="A170" s="25" t="s">
         <v>176</v>
       </c>
@@ -6965,7 +6969,7 @@
       <c r="U170" s="2"/>
       <c r="V170" s="2"/>
     </row>
-    <row r="171" spans="1:22" ht="14.4">
+    <row r="171" spans="1:22" ht="15">
       <c r="A171" s="25" t="s">
         <v>177</v>
       </c>
@@ -6995,7 +6999,7 @@
       <c r="U171" s="2"/>
       <c r="V171" s="2"/>
     </row>
-    <row r="172" spans="1:22" ht="14.4">
+    <row r="172" spans="1:22" ht="15">
       <c r="A172" s="25" t="s">
         <v>178</v>
       </c>
@@ -7025,7 +7029,7 @@
       <c r="U172" s="2"/>
       <c r="V172" s="2"/>
     </row>
-    <row r="173" spans="1:22" ht="14.4">
+    <row r="173" spans="1:22" ht="15">
       <c r="A173" s="25" t="s">
         <v>179</v>
       </c>
@@ -7055,7 +7059,7 @@
       <c r="U173" s="2"/>
       <c r="V173" s="2"/>
     </row>
-    <row r="174" spans="1:22" ht="14.4">
+    <row r="174" spans="1:22" ht="15">
       <c r="A174" s="25" t="s">
         <v>180</v>
       </c>
@@ -7085,7 +7089,7 @@
       <c r="U174" s="2"/>
       <c r="V174" s="2"/>
     </row>
-    <row r="175" spans="1:22" ht="14.4">
+    <row r="175" spans="1:22" ht="15">
       <c r="A175" s="25" t="s">
         <v>181</v>
       </c>
@@ -7115,7 +7119,7 @@
       <c r="U175" s="2"/>
       <c r="V175" s="2"/>
     </row>
-    <row r="176" spans="1:22" ht="14.4">
+    <row r="176" spans="1:22" ht="15">
       <c r="A176" s="25" t="s">
         <v>182</v>
       </c>
@@ -7145,7 +7149,7 @@
       <c r="U176" s="2"/>
       <c r="V176" s="2"/>
     </row>
-    <row r="177" spans="1:22" ht="14.4">
+    <row r="177" spans="1:22" ht="15">
       <c r="A177" s="25" t="s">
         <v>183</v>
       </c>
@@ -7175,7 +7179,7 @@
       <c r="U177" s="2"/>
       <c r="V177" s="2"/>
     </row>
-    <row r="178" spans="1:22" ht="14.4">
+    <row r="178" spans="1:22" ht="15">
       <c r="A178" s="25" t="s">
         <v>184</v>
       </c>
@@ -7205,7 +7209,7 @@
       <c r="U178" s="2"/>
       <c r="V178" s="2"/>
     </row>
-    <row r="179" spans="1:22" ht="14.4">
+    <row r="179" spans="1:22" ht="15">
       <c r="A179" s="25" t="s">
         <v>185</v>
       </c>
@@ -7235,7 +7239,7 @@
       <c r="U179" s="2"/>
       <c r="V179" s="2"/>
     </row>
-    <row r="180" spans="1:22" ht="14.4">
+    <row r="180" spans="1:22" ht="15">
       <c r="A180" s="25" t="s">
         <v>186</v>
       </c>
@@ -7265,7 +7269,7 @@
       <c r="U180" s="2"/>
       <c r="V180" s="2"/>
     </row>
-    <row r="181" spans="1:22" ht="14.4">
+    <row r="181" spans="1:22" ht="15">
       <c r="A181" s="25" t="s">
         <v>187</v>
       </c>
@@ -7295,7 +7299,7 @@
       <c r="U181" s="2"/>
       <c r="V181" s="2"/>
     </row>
-    <row r="182" spans="1:22" ht="14.4">
+    <row r="182" spans="1:22" ht="15">
       <c r="A182" s="25" t="s">
         <v>188</v>
       </c>
@@ -7325,7 +7329,7 @@
       <c r="U182" s="2"/>
       <c r="V182" s="2"/>
     </row>
-    <row r="183" spans="1:22" ht="14.4">
+    <row r="183" spans="1:22" ht="15">
       <c r="A183" s="25" t="s">
         <v>189</v>
       </c>
@@ -7355,7 +7359,7 @@
       <c r="U183" s="2"/>
       <c r="V183" s="2"/>
     </row>
-    <row r="184" spans="1:22" ht="15" thickBot="1">
+    <row r="184" spans="1:22" thickBot="1">
       <c r="A184" s="25" t="s">
         <v>190</v>
       </c>
@@ -7385,7 +7389,7 @@
       <c r="U184" s="2"/>
       <c r="V184" s="2"/>
     </row>
-    <row r="185" spans="1:22" ht="15.6" thickBot="1">
+    <row r="185" spans="1:22" thickBot="1">
       <c r="A185" s="28" t="s">
         <v>191</v>
       </c>
@@ -7421,7 +7425,7 @@
       <c r="U185" s="2"/>
       <c r="V185" s="2"/>
     </row>
-    <row r="186" spans="1:22" ht="15.6" thickBot="1">
+    <row r="186" spans="1:22" thickBot="1">
       <c r="A186" s="28" t="s">
         <v>192</v>
       </c>
@@ -7459,7 +7463,7 @@
       <c r="U186" s="2"/>
       <c r="V186" s="2"/>
     </row>
-    <row r="187" spans="1:22" ht="15.6" thickBot="1">
+    <row r="187" spans="1:22" thickBot="1">
       <c r="A187" s="28" t="s">
         <v>193</v>
       </c>
@@ -7497,7 +7501,7 @@
       <c r="U187" s="2"/>
       <c r="V187" s="2"/>
     </row>
-    <row r="188" spans="1:22" ht="15.6" thickBot="1">
+    <row r="188" spans="1:22" thickBot="1">
       <c r="A188" s="28" t="s">
         <v>194</v>
       </c>
@@ -7535,7 +7539,7 @@
       <c r="U188" s="2"/>
       <c r="V188" s="2"/>
     </row>
-    <row r="189" spans="1:22" ht="15.6" thickBot="1">
+    <row r="189" spans="1:22" thickBot="1">
       <c r="A189" s="28" t="s">
         <v>195</v>
       </c>
@@ -7611,7 +7615,7 @@
       <c r="U190" s="2"/>
       <c r="V190" s="2"/>
     </row>
-    <row r="191" spans="1:22" ht="14.4">
+    <row r="191" spans="1:22" ht="15">
       <c r="A191" s="28" t="s">
         <v>197</v>
       </c>
@@ -7641,7 +7645,7 @@
       <c r="U191" s="2"/>
       <c r="V191" s="2"/>
     </row>
-    <row r="192" spans="1:22" ht="14.4">
+    <row r="192" spans="1:22" ht="15">
       <c r="A192" s="28" t="s">
         <v>198</v>
       </c>
@@ -7679,7 +7683,7 @@
       <c r="U192" s="2"/>
       <c r="V192" s="2"/>
     </row>
-    <row r="193" spans="1:22" ht="14.4">
+    <row r="193" spans="1:22" ht="15">
       <c r="A193" s="28" t="s">
         <v>199</v>
       </c>
@@ -7717,7 +7721,7 @@
       <c r="U193" s="2"/>
       <c r="V193" s="2"/>
     </row>
-    <row r="194" spans="1:22" ht="14.4">
+    <row r="194" spans="1:22" ht="15">
       <c r="A194" s="28" t="s">
         <v>200</v>
       </c>
@@ -7753,7 +7757,7 @@
       <c r="U194" s="2"/>
       <c r="V194" s="2"/>
     </row>
-    <row r="195" spans="1:22" ht="14.4">
+    <row r="195" spans="1:22" ht="15">
       <c r="A195" s="28" t="s">
         <v>201</v>
       </c>
@@ -7791,7 +7795,7 @@
       <c r="U195" s="2"/>
       <c r="V195" s="2"/>
     </row>
-    <row r="196" spans="1:22" ht="14.4">
+    <row r="196" spans="1:22" ht="15">
       <c r="A196" s="28" t="s">
         <v>202</v>
       </c>
@@ -7829,7 +7833,7 @@
       <c r="U196" s="2"/>
       <c r="V196" s="2"/>
     </row>
-    <row r="197" spans="1:22" ht="14.4">
+    <row r="197" spans="1:22" ht="15">
       <c r="A197" s="28" t="s">
         <v>203</v>
       </c>
@@ -7867,7 +7871,7 @@
       <c r="U197" s="2"/>
       <c r="V197" s="2"/>
     </row>
-    <row r="198" spans="1:22" ht="14.4">
+    <row r="198" spans="1:22" ht="15">
       <c r="A198" s="25" t="s">
         <v>204</v>
       </c>
@@ -7905,7 +7909,7 @@
       <c r="U198" s="2"/>
       <c r="V198" s="2"/>
     </row>
-    <row r="199" spans="1:22" ht="14.4">
+    <row r="199" spans="1:22" ht="15">
       <c r="A199" s="28" t="s">
         <v>205</v>
       </c>
@@ -7981,7 +7985,7 @@
       <c r="U200" s="2"/>
       <c r="V200" s="2"/>
     </row>
-    <row r="201" spans="1:22" ht="14.4">
+    <row r="201" spans="1:22" ht="15">
       <c r="A201" s="28" t="s">
         <v>207</v>
       </c>
@@ -8011,7 +8015,7 @@
       <c r="U201" s="2"/>
       <c r="V201" s="2"/>
     </row>
-    <row r="202" spans="1:22" ht="14.4">
+    <row r="202" spans="1:22" ht="15">
       <c r="A202" s="28" t="s">
         <v>208</v>
       </c>
@@ -8041,7 +8045,7 @@
       <c r="U202" s="2"/>
       <c r="V202" s="2"/>
     </row>
-    <row r="203" spans="1:22" ht="14.4">
+    <row r="203" spans="1:22" ht="15">
       <c r="A203" s="28" t="s">
         <v>209</v>
       </c>
@@ -8079,7 +8083,7 @@
       <c r="U203" s="2"/>
       <c r="V203" s="2"/>
     </row>
-    <row r="204" spans="1:22" ht="14.4">
+    <row r="204" spans="1:22" ht="15">
       <c r="A204" s="28" t="s">
         <v>210</v>
       </c>
@@ -8117,7 +8121,7 @@
       <c r="U204" s="2"/>
       <c r="V204" s="2"/>
     </row>
-    <row r="205" spans="1:22" ht="15" thickBot="1">
+    <row r="205" spans="1:22" thickBot="1">
       <c r="A205" s="28" t="s">
         <v>211</v>
       </c>
@@ -8193,7 +8197,7 @@
       <c r="U206" s="2"/>
       <c r="V206" s="2"/>
     </row>
-    <row r="207" spans="1:22" ht="14.4">
+    <row r="207" spans="1:22" ht="15">
       <c r="A207" s="28" t="s">
         <v>213</v>
       </c>
@@ -8229,7 +8233,7 @@
       <c r="U207" s="2"/>
       <c r="V207" s="2"/>
     </row>
-    <row r="208" spans="1:22" ht="15" thickBot="1">
+    <row r="208" spans="1:22" thickBot="1">
       <c r="A208" s="28" t="s">
         <v>214</v>
       </c>
@@ -8259,7 +8263,7 @@
       <c r="U208" s="2"/>
       <c r="V208" s="2"/>
     </row>
-    <row r="209" spans="1:22" ht="15.6" thickBot="1">
+    <row r="209" spans="1:22" thickBot="1">
       <c r="A209" s="28" t="s">
         <v>215</v>
       </c>
@@ -8335,7 +8339,7 @@
       <c r="U210" s="2"/>
       <c r="V210" s="2"/>
     </row>
-    <row r="211" spans="1:22" ht="14.4">
+    <row r="211" spans="1:22" ht="15">
       <c r="A211" s="28" t="s">
         <v>217</v>
       </c>
@@ -8373,7 +8377,7 @@
       <c r="U211" s="2"/>
       <c r="V211" s="2"/>
     </row>
-    <row r="212" spans="1:22" ht="15" thickBot="1">
+    <row r="212" spans="1:22" thickBot="1">
       <c r="A212" s="28" t="s">
         <v>218</v>
       </c>
@@ -8441,7 +8445,7 @@
       <c r="U213" s="2"/>
       <c r="V213" s="2"/>
     </row>
-    <row r="214" spans="1:22" ht="14.4">
+    <row r="214" spans="1:22" ht="15">
       <c r="A214" s="28" t="s">
         <v>220</v>
       </c>

</xml_diff>

<commit_message>
Editando las primeras 73 filas del Excel
</commit_message>
<xml_diff>
--- a/CHGenesOrdenadosConVecinos.xlsx
+++ b/CHGenesOrdenadosConVecinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelly\Desktop\pc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0028E751-989D-46D8-9EA0-BABF82C74025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5AFBB5-3C77-4DA7-B84A-A53514D85BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="378">
   <si>
     <t>Localización</t>
   </si>
@@ -896,6 +896,264 @@
   </si>
   <si>
     <t>CGG Triplet Repeat Binding Protein 1</t>
+  </si>
+  <si>
+    <t>Zinc Finger Protein 654</t>
+  </si>
+  <si>
+    <t>Solute Carrier Family 12 Member 8</t>
+  </si>
+  <si>
+    <t>Zinc Finger Protein 148</t>
+  </si>
+  <si>
+    <t>Sorting Nexin 4</t>
+  </si>
+  <si>
+    <t>Oxysterol Binding Protein Like 11</t>
+  </si>
+  <si>
+    <t>Leishmanolysin Like Peptidase</t>
+  </si>
+  <si>
+    <t>Ribosomal Protein L35a</t>
+  </si>
+  <si>
+    <t>IQ Motif Containing G</t>
+  </si>
+  <si>
+    <t>Leucine Rich Repeats And Calponin Homology Domain Containing 3</t>
+  </si>
+  <si>
+    <t>Forty-Two-Three Domain Containing 1</t>
+  </si>
+  <si>
+    <t>Rubicon Autophagy Regulator</t>
+  </si>
+  <si>
+    <t>Mucin 20, Cell Surface Associated</t>
+  </si>
+  <si>
+    <t>Mucin 4, Cell Surface Associated</t>
+  </si>
+  <si>
+    <t>Tyrosine Kinase Non Receptor 2</t>
+  </si>
+  <si>
+    <t>Transferrin Receptor</t>
+  </si>
+  <si>
+    <t>Zinc Finger DHHC-Type Palmitoyltransferase 19</t>
+  </si>
+  <si>
+    <t>Solute Carrier Family 51 Subunit Alpha</t>
+  </si>
+  <si>
+    <t>Phosphate Cytidylyltransferase 1A, Choline</t>
+  </si>
+  <si>
+    <t>Transmembrane 4 L Six Family Member 19</t>
+  </si>
+  <si>
+    <t>UBX Domain Protein 7</t>
+  </si>
+  <si>
+    <t>Ring Finger Protein 168</t>
+  </si>
+  <si>
+    <t>Single-Pass Membrane Protein With Coiled-Coil Domains 1</t>
+  </si>
+  <si>
+    <t>WD Repeat Domain 53</t>
+  </si>
+  <si>
+    <t>F-Box Protein 45</t>
+  </si>
+  <si>
+    <t>Negative Regulator Of Reactive Oxygen Species</t>
+  </si>
+  <si>
+    <t>Centrosomal Protein 19</t>
+  </si>
+  <si>
+    <t>Phosphatidylinositol Glycan Anchor Biosynthesis Class X</t>
+  </si>
+  <si>
+    <t>P21 (RAC1) Activated Kinase 2</t>
+  </si>
+  <si>
+    <t>SUMO Specific Peptidase 5</t>
+  </si>
+  <si>
+    <t>Nuclear Cap Binding Protein Subunit 2</t>
+  </si>
+  <si>
+    <t>Phosphatidylinositol Glycan Anchor Biosynthesis Class Z</t>
+  </si>
+  <si>
+    <t>Melanotransferrin</t>
+  </si>
+  <si>
+    <t>Receptor Transporter Protein 2</t>
+  </si>
+  <si>
+    <t>Somatostatin</t>
+  </si>
+  <si>
+    <t>Receptor Transporter Protein 4</t>
+  </si>
+  <si>
+    <t>MBL Associated Serine Protease 1</t>
+  </si>
+  <si>
+    <t>Receptor Transporter Protein 1</t>
+  </si>
+  <si>
+    <t>ST6 Beta-Galactoside Alpha-2,6-Sialyltransferase 1</t>
+  </si>
+  <si>
+    <t>Adiponectin, C1Q And Collagen Domain Containing</t>
+  </si>
+  <si>
+    <t>Replication Factor C Subunit 4</t>
+  </si>
+  <si>
+    <t>Eukaryotic Translation Initiation Factor 4A2</t>
+  </si>
+  <si>
+    <t>RNA Gene</t>
+  </si>
+  <si>
+    <t>MicroRNA 1248</t>
+  </si>
+  <si>
+    <t>Kininogen 1</t>
+  </si>
+  <si>
+    <t>Histidine Rich Glycoprotein</t>
+  </si>
+  <si>
+    <t>Fetuin B</t>
+  </si>
+  <si>
+    <t>Alpha 2-HS Glycoprotein</t>
+  </si>
+  <si>
+    <t>DnaJ Heat Shock Protein Family (Hsp40) Member B11</t>
+  </si>
+  <si>
+    <t>25,44</t>
+  </si>
+  <si>
+    <t>42,44</t>
+  </si>
+  <si>
+    <t>6,3</t>
+  </si>
+  <si>
+    <t>43,49</t>
+  </si>
+  <si>
+    <t>23,20</t>
+  </si>
+  <si>
+    <t>10,11</t>
+  </si>
+  <si>
+    <t>22,26</t>
+  </si>
+  <si>
+    <t>35,38</t>
+  </si>
+  <si>
+    <t>22,27</t>
+  </si>
+  <si>
+    <t>16,11</t>
+  </si>
+  <si>
+    <t>15,29</t>
+  </si>
+  <si>
+    <t>39,55</t>
+  </si>
+  <si>
+    <t>9,14</t>
+  </si>
+  <si>
+    <t>10,2</t>
+  </si>
+  <si>
+    <t>44,27</t>
+  </si>
+  <si>
+    <t>32,44</t>
+  </si>
+  <si>
+    <t>5,1</t>
+  </si>
+  <si>
+    <t>23,50</t>
+  </si>
+  <si>
+    <t>7,28</t>
+  </si>
+  <si>
+    <t>24,27</t>
+  </si>
+  <si>
+    <t>26,30</t>
+  </si>
+  <si>
+    <t>20,28</t>
+  </si>
+  <si>
+    <t>15,20</t>
+  </si>
+  <si>
+    <t>10,10</t>
+  </si>
+  <si>
+    <t>20,32</t>
+  </si>
+  <si>
+    <t>41,43</t>
+  </si>
+  <si>
+    <t>26,26</t>
+  </si>
+  <si>
+    <t>44,58</t>
+  </si>
+  <si>
+    <t>22,24</t>
+  </si>
+  <si>
+    <t>16,15</t>
+  </si>
+  <si>
+    <t>9,18</t>
+  </si>
+  <si>
+    <t>1,0.84</t>
+  </si>
+  <si>
+    <t>31,32</t>
+  </si>
+  <si>
+    <t>21,27</t>
+  </si>
+  <si>
+    <t>1,0.69</t>
+  </si>
+  <si>
+    <t>1,0.18</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>2,4</t>
   </si>
 </sst>
 </file>
@@ -1205,6 +1463,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1213,14 +1479,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1236,315 +1494,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>310515</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>958215</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>108585</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Elipse 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1243965" y="2642235"/>
-          <a:ext cx="2886075" cy="2257425"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1249680</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Flecha curvada hacia arriba 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2183130" y="3251835"/>
-          <a:ext cx="1194435" cy="525780"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedUpArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1211580</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1653540</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Elipse 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2145030" y="2767965"/>
-          <a:ext cx="441960" cy="411480"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2146935</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>287655</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Elipse 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3080385" y="2779395"/>
-          <a:ext cx="379095" cy="411480"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1564949</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>28459</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2082899</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>144069</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Acorde 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="18150062">
-          <a:off x="2413819" y="3380114"/>
-          <a:ext cx="687110" cy="517950"/>
-        </a:xfrm>
-        <a:prstGeom prst="chord">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1750,8 +1699,8 @@
   </sheetPr>
   <dimension ref="A1:V216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1769,15 +1718,15 @@
       <c r="A1" s="24"/>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
@@ -1809,17 +1758,17 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="5">
         <v>32091689</v>
       </c>
       <c r="E3" s="5">
         <v>32091761</v>
       </c>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1839,17 +1788,17 @@
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="5">
         <v>32837131</v>
       </c>
       <c r="E4" s="5">
         <v>32838076</v>
       </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -1869,17 +1818,17 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="5">
         <v>33089112</v>
       </c>
       <c r="E5" s="5">
         <v>33090132</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1899,17 +1848,17 @@
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="5">
         <v>33764252</v>
       </c>
       <c r="E6" s="5">
         <v>33768221</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1929,17 +1878,17 @@
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="5">
         <v>33810174</v>
       </c>
       <c r="E7" s="5">
         <v>33811741</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1959,10 +1908,10 @@
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="46" t="s">
         <v>287</v>
       </c>
       <c r="D8" s="5">
@@ -1971,9 +1920,13 @@
       <c r="E8" s="5">
         <v>33934641</v>
       </c>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
+      <c r="F8" s="44" t="s">
+        <v>340</v>
+      </c>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44">
+        <v>0</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1993,10 +1946,10 @@
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="46" t="s">
         <v>288</v>
       </c>
       <c r="D9" s="5">
@@ -2005,9 +1958,13 @@
       <c r="E9" s="5">
         <v>34231630</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>341</v>
+      </c>
       <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11">
+        <v>21</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2039,9 +1996,13 @@
       <c r="E10" s="5">
         <v>34251973</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="11">
+        <v>2</v>
+      </c>
       <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="H10" s="11">
+        <v>3</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -2073,7 +2034,9 @@
       <c r="E11" s="5">
         <v>34812505</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="11" t="s">
+        <v>342</v>
+      </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="2"/>
@@ -2137,9 +2100,13 @@
       <c r="E13" s="5">
         <v>34864667</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="11" t="s">
+        <v>343</v>
+      </c>
       <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="11">
+        <v>18</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -2159,17 +2126,25 @@
       <c r="A14" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="13"/>
+      <c r="B14" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>292</v>
+      </c>
       <c r="D14" s="5">
         <v>34864860</v>
       </c>
       <c r="E14" s="5">
         <v>34953982</v>
       </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>344</v>
+      </c>
       <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -2249,15 +2224,21 @@
       <c r="A17" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>293</v>
+      </c>
       <c r="D17" s="5">
         <v>69289222</v>
       </c>
       <c r="E17" s="5">
         <v>69431839</v>
       </c>
-      <c r="F17" s="11"/>
+      <c r="F17" s="11" t="s">
+        <v>345</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="2"/>
@@ -2309,17 +2290,25 @@
       <c r="A19" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>294</v>
+      </c>
       <c r="D19" s="5">
         <v>69442967</v>
       </c>
       <c r="E19" s="5">
         <v>69586809</v>
       </c>
-      <c r="F19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>346</v>
+      </c>
       <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="H19" s="11">
+        <v>3</v>
+      </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2339,17 +2328,25 @@
       <c r="A20" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>295</v>
+      </c>
       <c r="D20" s="5">
         <v>69656519</v>
       </c>
       <c r="E20" s="5">
         <v>69708647</v>
       </c>
-      <c r="F20" s="11"/>
+      <c r="F20" s="11" t="s">
+        <v>347</v>
+      </c>
       <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
+      <c r="H20" s="11">
+        <v>6</v>
+      </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -2369,15 +2366,21 @@
       <c r="A21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>296</v>
+      </c>
       <c r="D21" s="5">
         <v>69727101</v>
       </c>
       <c r="E21" s="5">
         <v>69826032</v>
       </c>
-      <c r="F21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>348</v>
+      </c>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="2"/>
@@ -2399,17 +2402,25 @@
       <c r="A22" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>297</v>
+      </c>
       <c r="D22" s="5">
         <v>69881877</v>
       </c>
       <c r="E22" s="5">
         <v>69933388</v>
       </c>
-      <c r="F22" s="11"/>
+      <c r="F22" s="11" t="s">
+        <v>349</v>
+      </c>
       <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
+      <c r="H22" s="11">
+        <v>3</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -2429,15 +2440,21 @@
       <c r="A23" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>298</v>
+      </c>
       <c r="D23" s="5">
         <v>69937555</v>
       </c>
       <c r="E23" s="5">
         <v>69941662</v>
       </c>
-      <c r="F23" s="11"/>
+      <c r="F23" s="11">
+        <v>156260</v>
+      </c>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="2"/>
@@ -2459,17 +2476,25 @@
       <c r="A24" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>299</v>
+      </c>
       <c r="D24" s="5">
         <v>69941767</v>
       </c>
       <c r="E24" s="5">
         <v>69990604</v>
       </c>
-      <c r="F24" s="11"/>
+      <c r="F24" s="11" t="s">
+        <v>350</v>
+      </c>
       <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+      <c r="H24" s="11">
+        <v>0</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -2489,17 +2514,25 @@
       <c r="A25" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>300</v>
+      </c>
       <c r="D25" s="5">
         <v>69990461</v>
       </c>
       <c r="E25" s="5">
         <v>70101362</v>
       </c>
-      <c r="F25" s="11"/>
+      <c r="F25" s="11" t="s">
+        <v>230</v>
+      </c>
       <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="H25" s="11">
+        <v>7</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -2519,15 +2552,21 @@
       <c r="A26" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="15"/>
+      <c r="B26" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>301</v>
+      </c>
       <c r="D26" s="5">
         <v>70107479</v>
       </c>
       <c r="E26" s="5">
         <v>70139011</v>
       </c>
-      <c r="F26" s="11"/>
+      <c r="F26" s="11" t="s">
+        <v>351</v>
+      </c>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
       <c r="I26" s="2"/>
@@ -2549,8 +2588,12 @@
       <c r="A27" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>302</v>
+      </c>
       <c r="D27" s="5">
         <v>70150265</v>
       </c>
@@ -2579,17 +2622,25 @@
       <c r="A28" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>303</v>
+      </c>
       <c r="D28" s="5">
         <v>70225887</v>
       </c>
       <c r="E28" s="5">
         <v>70241268</v>
       </c>
-      <c r="F28" s="11"/>
+      <c r="F28" s="11" t="s">
+        <v>352</v>
+      </c>
       <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
+      <c r="H28" s="11">
+        <v>18</v>
+      </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -2609,15 +2660,21 @@
       <c r="A29" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="13"/>
+      <c r="B29" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>304</v>
+      </c>
       <c r="D29" s="5">
         <v>70248605</v>
       </c>
       <c r="E29" s="5">
         <v>70298576</v>
       </c>
-      <c r="F29" s="11"/>
+      <c r="F29" s="11" t="s">
+        <v>353</v>
+      </c>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="2"/>
@@ -2639,15 +2696,21 @@
       <c r="A30" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="D30" s="5">
         <v>70353419</v>
       </c>
       <c r="E30" s="5">
         <v>70394458</v>
       </c>
-      <c r="F30" s="11"/>
+      <c r="F30" s="11" t="s">
+        <v>354</v>
+      </c>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="2"/>
@@ -2669,17 +2732,25 @@
       <c r="A31" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>306</v>
+      </c>
       <c r="D31" s="5">
         <v>70405851</v>
       </c>
       <c r="E31" s="5">
         <v>70553035</v>
       </c>
-      <c r="F31" s="11"/>
+      <c r="F31" s="11" t="s">
+        <v>355</v>
+      </c>
       <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
+      <c r="H31" s="11">
+        <v>15</v>
+      </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -2699,17 +2770,25 @@
       <c r="A32" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>307</v>
+      </c>
       <c r="D32" s="5">
         <v>70543190</v>
       </c>
       <c r="E32" s="5">
         <v>70555784</v>
       </c>
-      <c r="F32" s="11"/>
+      <c r="F32" s="11" t="s">
+        <v>356</v>
+      </c>
       <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="H32" s="11">
+        <v>0</v>
+      </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
@@ -2729,15 +2808,21 @@
       <c r="A33" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>308</v>
+      </c>
       <c r="D33" s="5">
         <v>70563308</v>
       </c>
       <c r="E33" s="5">
         <v>70580733</v>
       </c>
-      <c r="F33" s="11"/>
+      <c r="F33" s="11">
+        <v>9</v>
+      </c>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="2"/>
@@ -2759,17 +2844,25 @@
       <c r="A34" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>309</v>
+      </c>
       <c r="D34" s="5">
         <v>70580065</v>
       </c>
       <c r="E34" s="5">
         <v>70627900</v>
       </c>
-      <c r="F34" s="11"/>
+      <c r="F34" s="11" t="s">
+        <v>357</v>
+      </c>
       <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
+      <c r="H34" s="11">
+        <v>0</v>
+      </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -2819,17 +2912,25 @@
       <c r="A36" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="15"/>
+      <c r="B36" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>310</v>
+      </c>
       <c r="D36" s="5">
         <v>70661439</v>
       </c>
       <c r="E36" s="5">
         <v>70665387</v>
       </c>
-      <c r="F36" s="11"/>
+      <c r="F36" s="11" t="s">
+        <v>358</v>
+      </c>
       <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
+      <c r="H36" s="11">
+        <v>0</v>
+      </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -2849,15 +2950,21 @@
       <c r="A37" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="15"/>
+      <c r="B37" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>311</v>
+      </c>
       <c r="D37" s="5">
         <v>70674326</v>
       </c>
       <c r="E37" s="5">
         <v>70732345</v>
       </c>
-      <c r="F37" s="11"/>
+      <c r="F37" s="11" t="s">
+        <v>359</v>
+      </c>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="2"/>
@@ -2939,17 +3046,25 @@
       <c r="A40" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="14"/>
+      <c r="B40" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>312</v>
+      </c>
       <c r="D40" s="5">
         <v>70765125</v>
       </c>
       <c r="E40" s="5">
         <v>70782692</v>
       </c>
-      <c r="F40" s="11"/>
+      <c r="F40" s="11" t="s">
+        <v>360</v>
+      </c>
       <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
+      <c r="H40" s="11">
+        <v>6</v>
+      </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -2969,17 +3084,25 @@
       <c r="A41" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="15"/>
+      <c r="B41" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>313</v>
+      </c>
       <c r="D41" s="5">
         <v>70784055</v>
       </c>
       <c r="E41" s="5">
         <v>70790921</v>
       </c>
-      <c r="F41" s="11"/>
+      <c r="F41" s="11">
+        <v>2</v>
+      </c>
       <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="H41" s="11">
+        <v>3</v>
+      </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
@@ -2999,17 +3122,25 @@
       <c r="A42" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="14"/>
+      <c r="B42" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>314</v>
+      </c>
       <c r="D42" s="5">
         <v>70820545</v>
       </c>
       <c r="E42" s="5">
         <v>70833184</v>
       </c>
-      <c r="F42" s="11"/>
+      <c r="F42" s="11" t="s">
+        <v>361</v>
+      </c>
       <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="H42" s="11">
+        <v>3</v>
+      </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
@@ -3029,17 +3160,25 @@
       <c r="A43" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>315</v>
+      </c>
       <c r="D43" s="5">
         <v>70833297</v>
       </c>
       <c r="E43" s="5">
         <v>70847080</v>
       </c>
-      <c r="F43" s="11"/>
+      <c r="F43" s="11" t="s">
+        <v>362</v>
+      </c>
       <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
+      <c r="H43" s="11">
+        <v>6</v>
+      </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -3089,17 +3228,25 @@
       <c r="A45" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="15"/>
+      <c r="B45" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>316</v>
+      </c>
       <c r="D45" s="5">
         <v>70890387</v>
       </c>
       <c r="E45" s="5">
         <v>70916589</v>
       </c>
-      <c r="F45" s="11"/>
+      <c r="F45" s="11">
+        <v>20</v>
+      </c>
       <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
+      <c r="H45" s="11">
+        <v>3</v>
+      </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
@@ -3119,17 +3266,25 @@
       <c r="A46" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="15"/>
+      <c r="B46" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>317</v>
+      </c>
       <c r="D46" s="5">
         <v>70953940</v>
       </c>
       <c r="E46" s="5">
         <v>70960688</v>
       </c>
-      <c r="F46" s="11"/>
+      <c r="F46" s="11" t="s">
+        <v>363</v>
+      </c>
       <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
+      <c r="H46" s="11">
+        <v>0</v>
+      </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
@@ -3149,15 +3304,21 @@
       <c r="A47" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="14"/>
+      <c r="B47" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>318</v>
+      </c>
       <c r="D47" s="5">
         <v>70957571</v>
       </c>
       <c r="E47" s="5">
         <v>70985213</v>
       </c>
-      <c r="F47" s="11"/>
+      <c r="F47" s="11" t="s">
+        <v>364</v>
+      </c>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="2"/>
@@ -3179,15 +3340,21 @@
       <c r="A48" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="15"/>
+      <c r="B48" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>319</v>
+      </c>
       <c r="D48" s="5">
         <v>70990569</v>
       </c>
       <c r="E48" s="5">
         <v>71073583</v>
       </c>
-      <c r="F48" s="11"/>
+      <c r="F48" s="11" t="s">
+        <v>365</v>
+      </c>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="2"/>
@@ -3239,17 +3406,25 @@
       <c r="A50" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="15"/>
+      <c r="B50" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>320</v>
+      </c>
       <c r="D50" s="5">
         <v>71085339</v>
       </c>
       <c r="E50" s="5">
         <v>71133963</v>
       </c>
-      <c r="F50" s="11"/>
+      <c r="F50" s="11" t="s">
+        <v>366</v>
+      </c>
       <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
+      <c r="H50" s="11">
+        <v>9</v>
+      </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -3269,17 +3444,25 @@
       <c r="A51" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="14"/>
+      <c r="B51" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>321</v>
+      </c>
       <c r="D51" s="5">
         <v>71133340</v>
       </c>
       <c r="E51" s="5">
         <v>71140105</v>
       </c>
-      <c r="F51" s="11"/>
+      <c r="F51" s="11" t="s">
+        <v>367</v>
+      </c>
       <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
+      <c r="H51" s="11">
+        <v>50</v>
+      </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
@@ -3299,17 +3482,25 @@
       <c r="A52" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="15"/>
+      <c r="B52" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>322</v>
+      </c>
       <c r="D52" s="5">
         <v>71144173</v>
       </c>
       <c r="E52" s="5">
         <v>71175164</v>
       </c>
-      <c r="F52" s="11"/>
+      <c r="F52" s="11" t="s">
+        <v>368</v>
+      </c>
       <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
+      <c r="H52" s="11">
+        <v>3</v>
+      </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -3359,8 +3550,12 @@
       <c r="A54" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="14"/>
+      <c r="B54" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>323</v>
+      </c>
       <c r="D54" s="5">
         <v>71209817</v>
       </c>
@@ -3389,15 +3584,21 @@
       <c r="A55" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="15"/>
+      <c r="B55" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>324</v>
+      </c>
       <c r="D55" s="5">
         <v>79336540</v>
       </c>
       <c r="E55" s="5">
         <v>79340104</v>
       </c>
-      <c r="F55" s="11"/>
+      <c r="F55" s="11">
+        <v>0.83</v>
+      </c>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
       <c r="I55" s="2"/>
@@ -3419,15 +3620,21 @@
       <c r="A56" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="14"/>
+      <c r="B56" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>325</v>
+      </c>
       <c r="D56" s="5">
         <v>79362883</v>
       </c>
       <c r="E56" s="5">
         <v>79364074</v>
       </c>
-      <c r="F56" s="11"/>
+      <c r="F56" s="11">
+        <v>7</v>
+      </c>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
       <c r="I56" s="2"/>
@@ -3449,17 +3656,25 @@
       <c r="A57" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="14"/>
+      <c r="B57" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>326</v>
+      </c>
       <c r="D57" s="5">
         <v>79616839</v>
       </c>
       <c r="E57" s="5">
         <v>79621245</v>
       </c>
-      <c r="F57" s="11"/>
+      <c r="F57" s="11" t="s">
+        <v>369</v>
+      </c>
       <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
+      <c r="H57" s="11">
+        <v>3</v>
+      </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
@@ -3509,17 +3724,25 @@
       <c r="A59" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="14"/>
+      <c r="B59" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>327</v>
+      </c>
       <c r="D59" s="5">
         <v>79705788</v>
       </c>
       <c r="E59" s="5">
         <v>79770724</v>
       </c>
-      <c r="F59" s="11"/>
+      <c r="F59" s="11" t="s">
+        <v>370</v>
+      </c>
       <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
+      <c r="H59" s="11">
+        <v>0</v>
+      </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -3539,17 +3762,25 @@
       <c r="A60" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="16"/>
-      <c r="C60" s="15"/>
+      <c r="B60" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>328</v>
+      </c>
       <c r="D60" s="5">
         <v>79780813</v>
       </c>
       <c r="E60" s="5">
         <v>79784271</v>
       </c>
-      <c r="F60" s="11"/>
+      <c r="F60" s="11" t="s">
+        <v>371</v>
+      </c>
       <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
+      <c r="H60" s="11">
+        <v>0</v>
+      </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -3599,17 +3830,25 @@
       <c r="A62" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B62" s="16"/>
-      <c r="C62" s="15"/>
+      <c r="B62" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>329</v>
+      </c>
       <c r="D62" s="5">
         <v>79880646</v>
       </c>
       <c r="E62" s="5">
         <v>80020253</v>
       </c>
-      <c r="F62" s="11"/>
+      <c r="F62" s="11" t="s">
+        <v>372</v>
+      </c>
       <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
+      <c r="H62" s="11">
+        <v>3</v>
+      </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -3659,17 +3898,25 @@
       <c r="A64" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="14"/>
+      <c r="B64" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>330</v>
+      </c>
       <c r="D64" s="5">
         <v>80092745</v>
       </c>
       <c r="E64" s="5">
         <v>80105787</v>
       </c>
-      <c r="F64" s="11"/>
+      <c r="F64" s="11">
+        <v>134227</v>
+      </c>
       <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
+      <c r="H64" s="11">
+        <v>3</v>
+      </c>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -3689,17 +3936,25 @@
       <c r="A65" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="14"/>
+      <c r="B65" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>331</v>
+      </c>
       <c r="D65" s="5">
         <v>80128438</v>
       </c>
       <c r="E65" s="5">
         <v>80141956</v>
       </c>
-      <c r="F65" s="11"/>
+      <c r="F65" s="11" t="s">
+        <v>373</v>
+      </c>
       <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
+      <c r="H65" s="11">
+        <v>6</v>
+      </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -3719,17 +3974,25 @@
       <c r="A66" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="14"/>
+      <c r="B66" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>332</v>
+      </c>
       <c r="D66" s="5">
         <v>80141693</v>
       </c>
       <c r="E66" s="5">
         <v>80148253</v>
       </c>
-      <c r="F66" s="11"/>
+      <c r="F66" s="11">
+        <v>114120</v>
+      </c>
       <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
+      <c r="H66" s="11">
+        <v>80</v>
+      </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -3749,8 +4012,12 @@
       <c r="A67" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="16"/>
-      <c r="C67" s="14"/>
+      <c r="B67" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>334</v>
+      </c>
       <c r="D67" s="5">
         <v>80144820</v>
       </c>
@@ -3779,15 +4046,21 @@
       <c r="A68" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="16"/>
-      <c r="C68" s="14"/>
+      <c r="B68" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>335</v>
+      </c>
       <c r="D68" s="5">
         <v>80175447</v>
       </c>
       <c r="E68" s="5">
         <v>80201003</v>
       </c>
-      <c r="F68" s="11"/>
+      <c r="F68" s="11" t="s">
+        <v>374</v>
+      </c>
       <c r="G68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="2"/>
@@ -3809,17 +4082,25 @@
       <c r="A69" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="16"/>
-      <c r="C69" s="14"/>
+      <c r="B69" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>336</v>
+      </c>
       <c r="D69" s="5">
         <v>80206861</v>
       </c>
       <c r="E69" s="5">
         <v>80214843</v>
       </c>
-      <c r="F69" s="11"/>
+      <c r="F69" s="11" t="s">
+        <v>375</v>
+      </c>
       <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
+      <c r="H69" s="11">
+        <v>0</v>
+      </c>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -3839,17 +4120,25 @@
       <c r="A70" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="16"/>
-      <c r="C70" s="14"/>
+      <c r="B70" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>337</v>
+      </c>
       <c r="D70" s="5">
         <v>80226559</v>
       </c>
       <c r="E70" s="5">
         <v>80241470</v>
       </c>
-      <c r="F70" s="11"/>
+      <c r="F70" s="11" t="s">
+        <v>376</v>
+      </c>
       <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
+      <c r="H70" s="11">
+        <v>0</v>
+      </c>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -3869,17 +4158,25 @@
       <c r="A71" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="16"/>
-      <c r="C71" s="14"/>
+      <c r="B71" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>338</v>
+      </c>
       <c r="D71" s="5">
         <v>80273479</v>
       </c>
       <c r="E71" s="5">
         <v>80280715</v>
       </c>
-      <c r="F71" s="11"/>
+      <c r="F71" s="11" t="s">
+        <v>377</v>
+      </c>
       <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
+      <c r="H71" s="11">
+        <v>0</v>
+      </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
@@ -3929,17 +4226,25 @@
       <c r="A73" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B73" s="16"/>
-      <c r="C73" s="13"/>
+      <c r="B73" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>339</v>
+      </c>
       <c r="D73" s="5">
         <v>80303639</v>
       </c>
       <c r="E73" s="5">
         <v>80323058</v>
       </c>
-      <c r="F73" s="11"/>
+      <c r="F73" s="11">
+        <v>47164</v>
+      </c>
       <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
+      <c r="H73" s="11">
+        <v>3</v>
+      </c>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
@@ -8498,6 +8803,5 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>